<commit_message>
Sprint 6 - corregido
</commit_message>
<xml_diff>
--- a/Documentos/ProductBacklogCorregido.xlsx
+++ b/Documentos/ProductBacklogCorregido.xlsx
@@ -5,18 +5,18 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://liveespochedu-my.sharepoint.com/personal/jonathan_aucancela_espoch_edu_ec/Documents/Documentos/Espoch/Octavo/Aplicaciones informáticas 2/SGT/Documentos/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\david\OneDrive - ESCUELA SUPERIOR POLITECNICA DE CHIMBORAZO\Documentos\Espoch\Octavo\Aplicaciones informáticas 2\SGT\Documentos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="602" documentId="8_{3B73CD9B-AD82-416D-96B8-D24AE7031C12}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7300378C-8671-4F01-9901-6A5CE36F860A}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47546FA3-5043-408C-8AD0-2913CCF288DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{7A8F741B-9112-4896-B995-875A9BDE94F9}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{7A8F741B-9112-4896-B995-875A9BDE94F9}"/>
   </bookViews>
   <sheets>
     <sheet name="Final" sheetId="1" r:id="rId1"/>
     <sheet name="Historias técnicas" sheetId="2" r:id="rId2"/>
     <sheet name="Historias de usuarios" sheetId="3" r:id="rId3"/>
-    <sheet name="proceso general" sheetId="4" r:id="rId4"/>
+    <sheet name="Sprints" sheetId="4" r:id="rId4"/>
     <sheet name="Metrica - seguridad" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="358" uniqueCount="277">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="364" uniqueCount="283">
   <si>
     <t>Product Backlog - SecuraBank</t>
   </si>
@@ -82,12 +82,6 @@
   </si>
   <si>
     <t>Diseñar notificaciones automáticas para administradores en caso de incidentes.</t>
-  </si>
-  <si>
-    <t>Integrar un registro de eventos de seguridad en el sistema.</t>
-  </si>
-  <si>
-    <t>Garantizar la compatibilidad del sistema con navegadores modernos.</t>
   </si>
   <si>
     <t>Realizar pruebas en dispositivos móviles y ajustar la interfaz.</t>
@@ -1013,6 +1007,30 @@
   </si>
   <si>
     <t>Realizar pruebas de seguridad para garantizar que las credenciales no sean vulnerables.</t>
+  </si>
+  <si>
+    <t>HT20</t>
+  </si>
+  <si>
+    <t>HT21</t>
+  </si>
+  <si>
+    <t>HT22</t>
+  </si>
+  <si>
+    <t>Implementar controles de seguridad en el ingreso (login)</t>
+  </si>
+  <si>
+    <t>Diseñar notificaciones automáticas para las transacciones bajo la lógica del nogicio.</t>
+  </si>
+  <si>
+    <t>Integrar un registro de eventos de seguridad en el sistema. Logs.</t>
+  </si>
+  <si>
+    <t>NGIX</t>
+  </si>
+  <si>
+    <t>HU5</t>
   </si>
 </sst>
 </file>
@@ -1332,6 +1350,12 @@
     <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1340,15 +1364,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1365,11 +1380,14 @@
     <xf numFmtId="0" fontId="0" fillId="12" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1391,10 +1409,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1716,8 +1730,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83A87B21-3BDC-40F9-B20F-2399C52423D9}">
   <dimension ref="A1:G41"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
@@ -1753,27 +1767,27 @@
         <v>10</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="F2" s="8" t="s">
         <v>6</v>
       </c>
       <c r="G2" s="3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="43.2" hidden="1" customHeight="1">
+      <c r="A3" s="27" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" ht="43.2" hidden="1" customHeight="1">
-      <c r="A3" s="25" t="s">
-        <v>41</v>
-      </c>
       <c r="B3" s="2" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="C3" s="10" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="E3" s="2">
         <v>4</v>
@@ -1782,19 +1796,19 @@
         <v>1</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="39" hidden="1" customHeight="1">
-      <c r="A4" s="26"/>
+      <c r="A4" s="28"/>
       <c r="B4" s="2" t="s">
         <v>4</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="E4" s="2">
         <v>4</v>
@@ -1803,19 +1817,19 @@
         <v>1</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="45.6" hidden="1" customHeight="1">
-      <c r="A5" s="26"/>
+      <c r="A5" s="28"/>
       <c r="B5" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="E5" s="2">
         <v>4</v>
@@ -1824,19 +1838,19 @@
         <v>1</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="36" hidden="1" customHeight="1">
-      <c r="A6" s="26"/>
+      <c r="A6" s="28"/>
       <c r="B6" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C6" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="C6" s="10" t="s">
-        <v>38</v>
-      </c>
       <c r="D6" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="E6" s="2">
         <v>4</v>
@@ -1845,19 +1859,19 @@
         <v>1</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="39" hidden="1" customHeight="1">
-      <c r="A7" s="27"/>
+      <c r="A7" s="29"/>
       <c r="B7" s="2" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="C7" s="10" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="E7" s="2">
         <v>4</v>
@@ -1866,21 +1880,21 @@
         <v>1</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="37.799999999999997" hidden="1" customHeight="1">
-      <c r="A8" s="25" t="s">
+      <c r="A8" s="27" t="s">
         <v>7</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E8" s="2">
         <v>4</v>
@@ -1889,16 +1903,16 @@
         <v>1</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="43.2" hidden="1" customHeight="1">
-      <c r="A9" s="26"/>
+      <c r="A9" s="28"/>
       <c r="B9" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C9" s="10" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>8</v>
@@ -1910,19 +1924,19 @@
         <v>2</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="39.6" hidden="1" customHeight="1">
-      <c r="A10" s="26"/>
+      <c r="A10" s="28"/>
       <c r="B10" s="2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C10" s="10" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="E10" s="2">
         <v>4</v>
@@ -1931,19 +1945,19 @@
         <v>1</v>
       </c>
       <c r="G10" s="2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="40.200000000000003" hidden="1" customHeight="1">
+      <c r="A11" s="28"/>
+      <c r="B11" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C11" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="D11" s="1" t="s">
         <v>59</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" ht="40.200000000000003" hidden="1" customHeight="1">
-      <c r="A11" s="26"/>
-      <c r="B11" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="C11" s="10" t="s">
-        <v>38</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>61</v>
       </c>
       <c r="E11" s="2">
         <v>4</v>
@@ -1952,19 +1966,19 @@
         <v>2</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="50.4" hidden="1" customHeight="1">
-      <c r="A12" s="27"/>
+      <c r="A12" s="29"/>
       <c r="B12" s="2" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C12" s="10" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E12" s="2">
         <v>4</v>
@@ -1973,21 +1987,21 @@
         <v>2</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="48.6" hidden="1" customHeight="1">
-      <c r="A13" s="25" t="s">
+      <c r="A13" s="27" t="s">
         <v>9</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="C13" s="10" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="E13" s="2">
         <v>4</v>
@@ -1996,19 +2010,19 @@
         <v>1</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="54.6" hidden="1" customHeight="1">
-      <c r="A14" s="26"/>
+      <c r="A14" s="28"/>
       <c r="B14" s="2" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="C14" s="10" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="E14" s="2">
         <v>4</v>
@@ -2017,19 +2031,19 @@
         <v>2</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="45.6" hidden="1" customHeight="1">
-      <c r="A15" s="27"/>
+      <c r="A15" s="29"/>
       <c r="B15" s="2" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="C15" s="10" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="E15" s="2">
         <v>4</v>
@@ -2038,21 +2052,21 @@
         <v>1</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="51.6" hidden="1" customHeight="1">
-      <c r="A16" s="25" t="s">
-        <v>174</v>
+      <c r="A16" s="27" t="s">
+        <v>172</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="C16" s="10" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="E16" s="2">
         <v>4</v>
@@ -2061,19 +2075,19 @@
         <v>1</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="58.8" hidden="1" customHeight="1">
-      <c r="A17" s="26"/>
+      <c r="A17" s="28"/>
       <c r="B17" s="2" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="C17" s="10" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="E17" s="2">
         <v>4</v>
@@ -2082,19 +2096,19 @@
         <v>1</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
     </row>
     <row r="18" spans="1:7" ht="53.4" hidden="1" customHeight="1">
-      <c r="A18" s="27"/>
+      <c r="A18" s="29"/>
       <c r="B18" s="2" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="C18" s="10" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="E18" s="2">
         <v>4</v>
@@ -2103,21 +2117,21 @@
         <v>1</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="19" spans="1:7" ht="43.2" customHeight="1">
-      <c r="A19" s="31" t="s">
-        <v>224</v>
+      <c r="A19" s="30" t="s">
+        <v>222</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="C19" s="10" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="E19" s="2">
         <v>2</v>
@@ -2126,19 +2140,19 @@
         <v>2</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="43.2">
-      <c r="A20" s="31"/>
+      <c r="A20" s="30"/>
       <c r="B20" s="2" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="C20" s="10" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="E20" s="2">
         <v>4</v>
@@ -2147,19 +2161,19 @@
         <v>2</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="31.2" customHeight="1">
-      <c r="A21" s="31"/>
+      <c r="A21" s="30"/>
       <c r="B21" s="2" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="C21" s="10" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="E21" s="2">
         <v>4</v>
@@ -2168,19 +2182,19 @@
         <v>2</v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
     </row>
     <row r="22" spans="1:7" ht="34.200000000000003" customHeight="1">
-      <c r="A22" s="31"/>
+      <c r="A22" s="30"/>
       <c r="B22" s="2" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="C22" s="10" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="E22" s="2">
         <v>1</v>
@@ -2189,18 +2203,18 @@
         <v>1</v>
       </c>
       <c r="G22" s="2" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
     </row>
     <row r="23" spans="1:7" ht="43.2">
-      <c r="A23" s="25" t="s">
-        <v>28</v>
+      <c r="A23" s="27" t="s">
+        <v>26</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C23" s="10" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D23" s="1" t="s">
         <v>11</v>
@@ -2212,16 +2226,16 @@
         <v>2</v>
       </c>
       <c r="G23" s="2" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
     </row>
     <row r="24" spans="1:7" ht="28.8">
-      <c r="A24" s="26"/>
+      <c r="A24" s="28"/>
       <c r="B24" s="2" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="C24" s="10" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D24" s="1" t="s">
         <v>12</v>
@@ -2233,16 +2247,16 @@
         <v>1</v>
       </c>
       <c r="G24" s="2" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
     </row>
     <row r="25" spans="1:7" ht="43.2">
-      <c r="A25" s="27"/>
+      <c r="A25" s="29"/>
       <c r="B25" s="2" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="C25" s="10" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D25" s="1" t="s">
         <v>13</v>
@@ -2254,17 +2268,21 @@
         <v>1</v>
       </c>
       <c r="G25" s="2" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
     </row>
     <row r="26" spans="1:7" ht="28.8" customHeight="1">
-      <c r="A26" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="B26" s="2"/>
-      <c r="C26" s="11"/>
+      <c r="A26" s="27" t="s">
+        <v>27</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>275</v>
+      </c>
+      <c r="C26" s="11" t="s">
+        <v>5</v>
+      </c>
       <c r="D26" s="1" t="s">
-        <v>12</v>
+        <v>278</v>
       </c>
       <c r="E26" s="2">
         <v>4</v>
@@ -2275,11 +2293,15 @@
       <c r="G26" s="2"/>
     </row>
     <row r="27" spans="1:7" ht="43.2">
-      <c r="A27" s="9"/>
-      <c r="B27" s="2"/>
-      <c r="C27" s="11"/>
+      <c r="A27" s="28"/>
+      <c r="B27" s="2" t="s">
+        <v>276</v>
+      </c>
+      <c r="C27" s="11" t="s">
+        <v>5</v>
+      </c>
       <c r="D27" s="1" t="s">
-        <v>13</v>
+        <v>279</v>
       </c>
       <c r="E27" s="2">
         <v>4</v>
@@ -2290,13 +2312,15 @@
       <c r="G27" s="2"/>
     </row>
     <row r="28" spans="1:7" ht="28.8">
-      <c r="A28" s="9"/>
-      <c r="B28" s="2"/>
+      <c r="A28" s="29"/>
+      <c r="B28" s="2" t="s">
+        <v>277</v>
+      </c>
       <c r="C28" s="11" t="s">
         <v>5</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>14</v>
+        <v>280</v>
       </c>
       <c r="E28" s="2">
         <v>4</v>
@@ -2308,14 +2332,16 @@
     </row>
     <row r="29" spans="1:7" ht="43.2">
       <c r="A29" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="B29" s="2"/>
+        <v>28</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>282</v>
+      </c>
       <c r="C29" s="11" t="s">
         <v>5</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>15</v>
+        <v>281</v>
       </c>
       <c r="E29" s="2">
         <v>4</v>
@@ -2332,7 +2358,7 @@
         <v>5</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E30" s="2">
         <v>4</v>
@@ -2344,14 +2370,14 @@
     </row>
     <row r="31" spans="1:7" ht="28.8">
       <c r="A31" s="9" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B31" s="2"/>
       <c r="C31" s="11" t="s">
         <v>5</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="E31" s="2">
         <v>4</v>
@@ -2368,7 +2394,7 @@
         <v>5</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E32" s="2">
         <v>4</v>
@@ -2385,7 +2411,7 @@
         <v>5</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="E33" s="2">
         <v>4</v>
@@ -2397,14 +2423,14 @@
     </row>
     <row r="34" spans="1:7" ht="57.6">
       <c r="A34" s="9" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B34" s="2"/>
       <c r="C34" s="11" t="s">
         <v>5</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E34" s="2">
         <v>4</v>
@@ -2421,7 +2447,7 @@
         <v>5</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E35" s="2">
         <v>4</v>
@@ -2433,14 +2459,14 @@
     </row>
     <row r="36" spans="1:7" ht="43.2">
       <c r="A36" s="9" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B36" s="2"/>
       <c r="C36" s="11" t="s">
         <v>5</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E36" s="2">
         <v>4</v>
@@ -2457,7 +2483,7 @@
         <v>5</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="E37" s="2">
         <v>4</v>
@@ -2474,7 +2500,7 @@
         <v>5</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="E38" s="2">
         <v>4</v>
@@ -2486,14 +2512,14 @@
     </row>
     <row r="39" spans="1:7" ht="43.2">
       <c r="A39" s="9" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B39" s="2"/>
       <c r="C39" s="11" t="s">
         <v>5</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="E39" s="2">
         <v>4</v>
@@ -2510,7 +2536,7 @@
         <v>5</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="E40" s="2">
         <v>4</v>
@@ -2527,7 +2553,7 @@
         <v>5</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="E41" s="2">
         <v>4</v>
@@ -2538,7 +2564,8 @@
       <c r="G41" s="2"/>
     </row>
   </sheetData>
-  <mergeCells count="6">
+  <mergeCells count="7">
+    <mergeCell ref="A26:A28"/>
     <mergeCell ref="A23:A25"/>
     <mergeCell ref="A16:A18"/>
     <mergeCell ref="A3:A7"/>
@@ -2572,13 +2599,13 @@
         <v>1</v>
       </c>
       <c r="B1" s="20" t="s">
+        <v>66</v>
+      </c>
+      <c r="C1" s="20" t="s">
+        <v>67</v>
+      </c>
+      <c r="D1" s="20" t="s">
         <v>68</v>
-      </c>
-      <c r="C1" s="20" t="s">
-        <v>69</v>
-      </c>
-      <c r="D1" s="20" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="72" hidden="1">
@@ -2586,351 +2613,351 @@
         <v>4</v>
       </c>
       <c r="B2" s="23" t="s">
-        <v>49</v>
-      </c>
-      <c r="C2" s="37" t="s">
-        <v>183</v>
-      </c>
-      <c r="D2" s="37" t="s">
-        <v>184</v>
+        <v>47</v>
+      </c>
+      <c r="C2" s="26" t="s">
+        <v>181</v>
+      </c>
+      <c r="D2" s="26" t="s">
+        <v>182</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="43.2" hidden="1">
       <c r="A3" s="21" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B3" s="23" t="s">
+        <v>183</v>
+      </c>
+      <c r="C3" s="26" t="s">
+        <v>184</v>
+      </c>
+      <c r="D3" s="26" t="s">
         <v>185</v>
-      </c>
-      <c r="C3" s="37" t="s">
-        <v>186</v>
-      </c>
-      <c r="D3" s="37" t="s">
-        <v>187</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="57.6" hidden="1">
       <c r="A4" s="21" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B4" s="23" t="s">
-        <v>53</v>
-      </c>
-      <c r="C4" s="37" t="s">
-        <v>188</v>
-      </c>
-      <c r="D4" s="37" t="s">
-        <v>189</v>
+        <v>51</v>
+      </c>
+      <c r="C4" s="26" t="s">
+        <v>186</v>
+      </c>
+      <c r="D4" s="26" t="s">
+        <v>187</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="57.6" hidden="1">
       <c r="A5" s="21" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B5" s="23" t="s">
+        <v>188</v>
+      </c>
+      <c r="C5" s="26" t="s">
+        <v>189</v>
+      </c>
+      <c r="D5" s="26" t="s">
         <v>190</v>
-      </c>
-      <c r="C5" s="37" t="s">
-        <v>191</v>
-      </c>
-      <c r="D5" s="37" t="s">
-        <v>192</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="57.6" hidden="1">
       <c r="A6" s="21" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B6" s="23" t="s">
+        <v>191</v>
+      </c>
+      <c r="C6" s="26" t="s">
+        <v>192</v>
+      </c>
+      <c r="D6" s="26" t="s">
         <v>193</v>
-      </c>
-      <c r="C6" s="37" t="s">
-        <v>194</v>
-      </c>
-      <c r="D6" s="37" t="s">
-        <v>195</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="43.2" hidden="1">
       <c r="A7" s="21" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B7" s="23" t="s">
+        <v>194</v>
+      </c>
+      <c r="C7" s="26" t="s">
+        <v>195</v>
+      </c>
+      <c r="D7" s="26" t="s">
         <v>196</v>
-      </c>
-      <c r="C7" s="37" t="s">
-        <v>197</v>
-      </c>
-      <c r="D7" s="37" t="s">
-        <v>198</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="43.2" hidden="1">
       <c r="A8" s="21" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B8" s="23" t="s">
+        <v>197</v>
+      </c>
+      <c r="C8" s="26" t="s">
+        <v>198</v>
+      </c>
+      <c r="D8" s="26" t="s">
         <v>199</v>
-      </c>
-      <c r="C8" s="37" t="s">
-        <v>200</v>
-      </c>
-      <c r="D8" s="37" t="s">
-        <v>201</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="43.2" hidden="1">
       <c r="A9" s="21" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="B9" s="23" t="s">
+        <v>200</v>
+      </c>
+      <c r="C9" s="26" t="s">
+        <v>201</v>
+      </c>
+      <c r="D9" s="26" t="s">
         <v>202</v>
-      </c>
-      <c r="C9" s="37" t="s">
-        <v>203</v>
-      </c>
-      <c r="D9" s="37" t="s">
-        <v>204</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="57.6" hidden="1">
       <c r="A10" s="21" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B10" s="23" t="s">
+        <v>203</v>
+      </c>
+      <c r="C10" s="26" t="s">
+        <v>204</v>
+      </c>
+      <c r="D10" s="26" t="s">
         <v>205</v>
-      </c>
-      <c r="C10" s="37" t="s">
-        <v>206</v>
-      </c>
-      <c r="D10" s="37" t="s">
-        <v>207</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="57.6" hidden="1">
       <c r="A11" s="21" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="B11" s="23" t="s">
-        <v>156</v>
-      </c>
-      <c r="C11" s="37" t="s">
-        <v>208</v>
-      </c>
-      <c r="D11" s="37" t="s">
-        <v>209</v>
+        <v>154</v>
+      </c>
+      <c r="C11" s="26" t="s">
+        <v>206</v>
+      </c>
+      <c r="D11" s="26" t="s">
+        <v>207</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="57.6" hidden="1">
       <c r="A12" s="21" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B12" s="23" t="s">
+        <v>208</v>
+      </c>
+      <c r="C12" s="26" t="s">
+        <v>209</v>
+      </c>
+      <c r="D12" s="26" t="s">
         <v>210</v>
-      </c>
-      <c r="C12" s="37" t="s">
-        <v>211</v>
-      </c>
-      <c r="D12" s="37" t="s">
-        <v>212</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="43.2" hidden="1">
       <c r="A13" s="21" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="B13" s="23" t="s">
-        <v>162</v>
-      </c>
-      <c r="C13" s="37" t="s">
-        <v>213</v>
-      </c>
-      <c r="D13" s="37" t="s">
-        <v>214</v>
+        <v>160</v>
+      </c>
+      <c r="C13" s="26" t="s">
+        <v>211</v>
+      </c>
+      <c r="D13" s="26" t="s">
+        <v>212</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="43.2">
       <c r="A14" s="21" t="s">
+        <v>216</v>
+      </c>
+      <c r="B14" s="23" t="s">
+        <v>213</v>
+      </c>
+      <c r="C14" s="26" t="s">
+        <v>214</v>
+      </c>
+      <c r="D14" s="26" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="28.8">
+      <c r="A15" s="31" t="s">
+        <v>217</v>
+      </c>
+      <c r="B15" s="32" t="s">
+        <v>233</v>
+      </c>
+      <c r="C15" s="26" t="s">
+        <v>234</v>
+      </c>
+      <c r="D15" s="26" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="28.8">
+      <c r="A16" s="31"/>
+      <c r="B16" s="33"/>
+      <c r="C16" s="26" t="s">
+        <v>235</v>
+      </c>
+      <c r="D16" s="26" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="28.8">
+      <c r="A17" s="31"/>
+      <c r="B17" s="34"/>
+      <c r="C17" s="26" t="s">
+        <v>236</v>
+      </c>
+      <c r="D17" s="26" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="43.2">
+      <c r="A18" s="31" t="s">
         <v>218</v>
       </c>
-      <c r="B14" s="23" t="s">
-        <v>215</v>
-      </c>
-      <c r="C14" s="37" t="s">
-        <v>216</v>
-      </c>
-      <c r="D14" s="37" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" ht="28.8">
-      <c r="A15" s="32" t="s">
-        <v>219</v>
-      </c>
-      <c r="B15" s="33" t="s">
-        <v>235</v>
-      </c>
-      <c r="C15" s="37" t="s">
-        <v>236</v>
-      </c>
-      <c r="D15" s="37" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" ht="28.8">
-      <c r="A16" s="32"/>
-      <c r="B16" s="34"/>
-      <c r="C16" s="37" t="s">
-        <v>237</v>
-      </c>
-      <c r="D16" s="37" t="s">
+      <c r="B18" s="32" t="s">
         <v>240</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" ht="28.8">
-      <c r="A17" s="32"/>
-      <c r="B17" s="35"/>
-      <c r="C17" s="37" t="s">
-        <v>238</v>
-      </c>
-      <c r="D17" s="37" t="s">
+      <c r="C18" s="26" t="s">
         <v>241</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" ht="43.2">
-      <c r="A18" s="32" t="s">
-        <v>220</v>
-      </c>
-      <c r="B18" s="33" t="s">
+      <c r="D18" s="26" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="28.8">
+      <c r="A19" s="31"/>
+      <c r="B19" s="33"/>
+      <c r="C19" s="26" t="s">
         <v>242</v>
       </c>
-      <c r="C18" s="37" t="s">
+      <c r="D19" s="26" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="28.8">
+      <c r="A20" s="31"/>
+      <c r="B20" s="34"/>
+      <c r="C20" s="26" t="s">
         <v>243</v>
       </c>
-      <c r="D18" s="37" t="s">
+      <c r="D20" s="26" t="s">
         <v>246</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="28.8">
-      <c r="A19" s="32"/>
-      <c r="B19" s="34"/>
-      <c r="C19" s="37" t="s">
-        <v>244</v>
-      </c>
-      <c r="D19" s="37" t="s">
+    <row r="21" spans="1:4" ht="28.8">
+      <c r="A21" s="31" t="s">
+        <v>223</v>
+      </c>
+      <c r="B21" s="32" t="s">
+        <v>253</v>
+      </c>
+      <c r="C21" s="22" t="s">
         <v>247</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" ht="28.8">
-      <c r="A20" s="32"/>
-      <c r="B20" s="35"/>
-      <c r="C20" s="37" t="s">
-        <v>245</v>
-      </c>
-      <c r="D20" s="37" t="s">
+      <c r="D21" s="22" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="28.8">
+      <c r="A22" s="31"/>
+      <c r="B22" s="33"/>
+      <c r="C22" s="22" t="s">
         <v>248</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" ht="28.8">
-      <c r="A21" s="32" t="s">
+      <c r="D22" s="22" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="28.8">
+      <c r="A23" s="31"/>
+      <c r="B23" s="34"/>
+      <c r="C23" s="22" t="s">
+        <v>249</v>
+      </c>
+      <c r="D23" s="22" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="28.8">
+      <c r="A24" s="31" t="s">
         <v>225</v>
       </c>
-      <c r="B21" s="33" t="s">
+      <c r="B24" s="32" t="s">
+        <v>254</v>
+      </c>
+      <c r="C24" s="25" t="s">
         <v>255</v>
       </c>
-      <c r="C21" s="22" t="s">
-        <v>249</v>
-      </c>
-      <c r="D21" s="22" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" ht="28.8">
-      <c r="A22" s="32"/>
-      <c r="B22" s="34"/>
-      <c r="C22" s="22" t="s">
-        <v>250</v>
-      </c>
-      <c r="D22" s="22" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" ht="28.8">
-      <c r="A23" s="32"/>
-      <c r="B23" s="35"/>
-      <c r="C23" s="22" t="s">
-        <v>251</v>
-      </c>
-      <c r="D23" s="22" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" ht="28.8">
-      <c r="A24" s="32" t="s">
-        <v>227</v>
-      </c>
-      <c r="B24" s="33" t="s">
+      <c r="D24" s="25" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="28.8">
+      <c r="A25" s="31"/>
+      <c r="B25" s="33"/>
+      <c r="C25" s="25" t="s">
         <v>256</v>
       </c>
-      <c r="C24" s="36" t="s">
+      <c r="D25" s="25" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="28.8">
+      <c r="A26" s="31"/>
+      <c r="B26" s="34"/>
+      <c r="C26" s="25" t="s">
         <v>257</v>
       </c>
-      <c r="D24" s="36" t="s">
+      <c r="D26" s="25" t="s">
         <v>260</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="28.8">
-      <c r="A25" s="32"/>
-      <c r="B25" s="34"/>
-      <c r="C25" s="36" t="s">
-        <v>258</v>
-      </c>
-      <c r="D25" s="36" t="s">
+    <row r="27" spans="1:4" ht="28.8">
+      <c r="A27" s="31" t="s">
+        <v>226</v>
+      </c>
+      <c r="B27" s="32" t="s">
         <v>261</v>
       </c>
-    </row>
-    <row r="26" spans="1:4" ht="28.8">
-      <c r="A26" s="32"/>
-      <c r="B26" s="35"/>
-      <c r="C26" s="36" t="s">
-        <v>259</v>
-      </c>
-      <c r="D26" s="36" t="s">
+      <c r="C27" s="25" t="s">
         <v>262</v>
       </c>
-    </row>
-    <row r="27" spans="1:4" ht="28.8">
-      <c r="A27" s="32" t="s">
-        <v>228</v>
-      </c>
-      <c r="B27" s="33" t="s">
+      <c r="D27" s="25" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" ht="28.8">
+      <c r="A28" s="31"/>
+      <c r="B28" s="33"/>
+      <c r="C28" s="25" t="s">
         <v>263</v>
       </c>
-      <c r="C27" s="36" t="s">
+      <c r="D28" s="25" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" ht="28.8">
+      <c r="A29" s="31"/>
+      <c r="B29" s="34"/>
+      <c r="C29" s="25" t="s">
         <v>264</v>
       </c>
-      <c r="D27" s="36" t="s">
+      <c r="D29" s="25" t="s">
         <v>267</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" ht="28.8">
-      <c r="A28" s="32"/>
-      <c r="B28" s="34"/>
-      <c r="C28" s="36" t="s">
-        <v>265</v>
-      </c>
-      <c r="D28" s="36" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" ht="28.8">
-      <c r="A29" s="32"/>
-      <c r="B29" s="35"/>
-      <c r="C29" s="36" t="s">
-        <v>266</v>
-      </c>
-      <c r="D29" s="36" t="s">
-        <v>269</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="28.8" customHeight="1"/>
@@ -2972,89 +2999,89 @@
         <v>1</v>
       </c>
       <c r="B1" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="C1" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="D1" s="12" t="s">
         <v>68</v>
-      </c>
-      <c r="C1" s="12" t="s">
-        <v>69</v>
-      </c>
-      <c r="D1" s="12" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="57.6">
       <c r="A2" s="13" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B2" s="24" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C2" s="22" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="D2" s="22" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="86.4">
       <c r="A3" s="13" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B3" s="23" t="s">
+        <v>175</v>
+      </c>
+      <c r="C3" s="22" t="s">
+        <v>176</v>
+      </c>
+      <c r="D3" s="22" t="s">
         <v>177</v>
-      </c>
-      <c r="C3" s="22" t="s">
-        <v>178</v>
-      </c>
-      <c r="D3" s="22" t="s">
-        <v>179</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="72">
       <c r="A4" s="13" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B4" s="23" t="s">
+        <v>178</v>
+      </c>
+      <c r="C4" s="22" t="s">
         <v>180</v>
       </c>
-      <c r="C4" s="22" t="s">
-        <v>182</v>
-      </c>
       <c r="D4" s="22" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="28.8">
-      <c r="A5" s="32" t="s">
-        <v>64</v>
-      </c>
-      <c r="B5" s="33" t="s">
+      <c r="A5" s="31" t="s">
+        <v>62</v>
+      </c>
+      <c r="B5" s="32" t="s">
+        <v>268</v>
+      </c>
+      <c r="C5" s="25" t="s">
+        <v>269</v>
+      </c>
+      <c r="D5" s="25" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="28.8">
+      <c r="A6" s="31"/>
+      <c r="B6" s="33"/>
+      <c r="C6" s="25" t="s">
         <v>270</v>
       </c>
-      <c r="C5" s="36" t="s">
+      <c r="D6" s="25" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="43.2">
+      <c r="A7" s="31"/>
+      <c r="B7" s="34"/>
+      <c r="C7" s="25" t="s">
         <v>271</v>
       </c>
-      <c r="D5" s="36" t="s">
+      <c r="D7" s="25" t="s">
         <v>274</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="28.8">
-      <c r="A6" s="32"/>
-      <c r="B6" s="34"/>
-      <c r="C6" s="36" t="s">
-        <v>272</v>
-      </c>
-      <c r="D6" s="36" t="s">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="43.2">
-      <c r="A7" s="32"/>
-      <c r="B7" s="35"/>
-      <c r="C7" s="36" t="s">
-        <v>273</v>
-      </c>
-      <c r="D7" s="36" t="s">
-        <v>276</v>
       </c>
     </row>
   </sheetData>
@@ -3070,7 +3097,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4078C501-E131-475B-B5C2-02382EA68E52}">
   <dimension ref="B2:B151"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
@@ -3078,12 +3105,12 @@
   <sheetData>
     <row r="2" spans="2:2">
       <c r="B2" s="14" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="4" spans="2:2" ht="18">
       <c r="B4" s="15" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="5" spans="2:2">
@@ -3091,27 +3118,27 @@
     </row>
     <row r="6" spans="2:2">
       <c r="B6" s="16" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="7" spans="2:2">
       <c r="B7" s="16" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="8" spans="2:2">
       <c r="B8" s="16" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="9" spans="2:2">
       <c r="B9" s="16" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="11" spans="2:2">
       <c r="B11" s="14" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="12" spans="2:2">
@@ -3119,17 +3146,17 @@
     </row>
     <row r="13" spans="2:2">
       <c r="B13" s="16" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="14" spans="2:2">
       <c r="B14" s="16" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="18" spans="2:2" ht="18">
       <c r="B18" s="15" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="19" spans="2:2">
@@ -3137,22 +3164,22 @@
     </row>
     <row r="20" spans="2:2">
       <c r="B20" s="16" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="21" spans="2:2">
       <c r="B21" s="16" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="22" spans="2:2">
       <c r="B22" s="16" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="24" spans="2:2">
       <c r="B24" s="14" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="25" spans="2:2">
@@ -3160,17 +3187,17 @@
     </row>
     <row r="26" spans="2:2">
       <c r="B26" s="16" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="27" spans="2:2">
       <c r="B27" s="16" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="31" spans="2:2" ht="18">
       <c r="B31" s="15" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="32" spans="2:2">
@@ -3178,22 +3205,22 @@
     </row>
     <row r="33" spans="2:2">
       <c r="B33" s="16" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="34" spans="2:2">
       <c r="B34" s="16" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="35" spans="2:2">
       <c r="B35" s="16" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="37" spans="2:2">
       <c r="B37" s="14" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="38" spans="2:2">
@@ -3201,17 +3228,17 @@
     </row>
     <row r="39" spans="2:2">
       <c r="B39" s="16" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="40" spans="2:2">
       <c r="B40" s="16" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="44" spans="2:2" ht="18">
       <c r="B44" s="15" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="45" spans="2:2">
@@ -3219,22 +3246,22 @@
     </row>
     <row r="46" spans="2:2">
       <c r="B46" s="16" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="47" spans="2:2">
       <c r="B47" s="16" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="48" spans="2:2">
       <c r="B48" s="16" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="50" spans="2:2">
       <c r="B50" s="14" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="51" spans="2:2">
@@ -3242,17 +3269,17 @@
     </row>
     <row r="52" spans="2:2">
       <c r="B52" s="16" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="53" spans="2:2">
       <c r="B53" s="16" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="57" spans="2:2" ht="18">
       <c r="B57" s="15" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="58" spans="2:2">
@@ -3260,22 +3287,22 @@
     </row>
     <row r="59" spans="2:2">
       <c r="B59" s="16" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="60" spans="2:2">
       <c r="B60" s="16" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="61" spans="2:2">
       <c r="B61" s="16" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="63" spans="2:2">
       <c r="B63" s="14" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="64" spans="2:2">
@@ -3283,17 +3310,17 @@
     </row>
     <row r="65" spans="2:2">
       <c r="B65" s="16" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="66" spans="2:2">
       <c r="B66" s="16" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="70" spans="2:2" ht="18">
       <c r="B70" s="15" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="71" spans="2:2">
@@ -3301,22 +3328,22 @@
     </row>
     <row r="72" spans="2:2">
       <c r="B72" s="16" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="73" spans="2:2">
       <c r="B73" s="16" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="74" spans="2:2">
       <c r="B74" s="16" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="76" spans="2:2">
       <c r="B76" s="14" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="77" spans="2:2">
@@ -3324,17 +3351,17 @@
     </row>
     <row r="78" spans="2:2">
       <c r="B78" s="16" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="79" spans="2:2">
       <c r="B79" s="16" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="83" spans="2:2" ht="18">
       <c r="B83" s="15" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="84" spans="2:2">
@@ -3342,17 +3369,17 @@
     </row>
     <row r="85" spans="2:2">
       <c r="B85" s="16" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="86" spans="2:2">
       <c r="B86" s="16" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="88" spans="2:2">
       <c r="B88" s="14" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="89" spans="2:2">
@@ -3360,17 +3387,17 @@
     </row>
     <row r="90" spans="2:2">
       <c r="B90" s="16" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="91" spans="2:2">
       <c r="B91" s="16" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="95" spans="2:2" ht="18">
       <c r="B95" s="15" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="96" spans="2:2">
@@ -3378,17 +3405,17 @@
     </row>
     <row r="97" spans="2:2">
       <c r="B97" s="16" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="98" spans="2:2">
       <c r="B98" s="16" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="100" spans="2:2">
       <c r="B100" s="14" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="101" spans="2:2">
@@ -3396,17 +3423,17 @@
     </row>
     <row r="102" spans="2:2">
       <c r="B102" s="16" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="103" spans="2:2">
       <c r="B103" s="16" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="107" spans="2:2" ht="18">
       <c r="B107" s="15" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="108" spans="2:2">
@@ -3414,17 +3441,17 @@
     </row>
     <row r="109" spans="2:2">
       <c r="B109" s="16" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="110" spans="2:2">
       <c r="B110" s="16" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="112" spans="2:2">
       <c r="B112" s="14" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="113" spans="2:2">
@@ -3432,17 +3459,17 @@
     </row>
     <row r="114" spans="2:2">
       <c r="B114" s="16" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="115" spans="2:2">
       <c r="B115" s="16" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="119" spans="2:2" ht="18">
       <c r="B119" s="15" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
     </row>
     <row r="120" spans="2:2">
@@ -3450,17 +3477,17 @@
     </row>
     <row r="121" spans="2:2">
       <c r="B121" s="16" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="122" spans="2:2">
       <c r="B122" s="16" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
     </row>
     <row r="124" spans="2:2">
       <c r="B124" s="14" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="125" spans="2:2">
@@ -3468,17 +3495,17 @@
     </row>
     <row r="126" spans="2:2">
       <c r="B126" s="16" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="127" spans="2:2">
       <c r="B127" s="16" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="131" spans="2:2" ht="18">
       <c r="B131" s="15" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
     </row>
     <row r="132" spans="2:2">
@@ -3486,17 +3513,17 @@
     </row>
     <row r="133" spans="2:2">
       <c r="B133" s="16" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
     <row r="134" spans="2:2">
       <c r="B134" s="16" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
     </row>
     <row r="136" spans="2:2">
       <c r="B136" s="14" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="137" spans="2:2">
@@ -3504,17 +3531,17 @@
     </row>
     <row r="138" spans="2:2">
       <c r="B138" s="16" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
     </row>
     <row r="139" spans="2:2">
       <c r="B139" s="16" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="143" spans="2:2" ht="18">
       <c r="B143" s="15" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
     </row>
     <row r="144" spans="2:2">
@@ -3522,17 +3549,17 @@
     </row>
     <row r="145" spans="2:2">
       <c r="B145" s="16" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="146" spans="2:2">
       <c r="B146" s="16" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="148" spans="2:2">
       <c r="B148" s="14" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="149" spans="2:2">
@@ -3540,12 +3567,12 @@
     </row>
     <row r="150" spans="2:2">
       <c r="B150" s="16" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
     </row>
     <row r="151" spans="2:2">
       <c r="B151" s="16" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
   </sheetData>
@@ -3569,18 +3596,18 @@
   <sheetData>
     <row r="2" spans="2:3" ht="39" customHeight="1">
       <c r="B2" s="17" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="C2" s="17" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
     </row>
     <row r="3" spans="2:3">
       <c r="B3" s="18" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="C3" s="19" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="4" spans="2:3">
@@ -3588,51 +3615,51 @@
         <v>1</v>
       </c>
       <c r="C4" s="19" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="5" spans="2:3">
       <c r="B5" s="18" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C5" s="19" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="6" spans="2:3">
       <c r="B6" s="18" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C6" s="19" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
     <row r="7" spans="2:3">
       <c r="B7" s="18" t="s">
+        <v>146</v>
+      </c>
+      <c r="C7" s="19" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="8" spans="2:3">
+      <c r="B8" s="35" t="s">
+        <v>152</v>
+      </c>
+      <c r="C8" s="19" t="s">
         <v>148</v>
       </c>
-      <c r="C7" s="19" t="s">
+    </row>
+    <row r="9" spans="2:3">
+      <c r="B9" s="36"/>
+      <c r="C9" s="19" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="8" spans="2:3">
-      <c r="B8" s="28" t="s">
-        <v>154</v>
-      </c>
-      <c r="C8" s="19" t="s">
+    <row r="10" spans="2:3">
+      <c r="B10" s="37"/>
+      <c r="C10" s="19" t="s">
         <v>150</v>
-      </c>
-    </row>
-    <row r="9" spans="2:3">
-      <c r="B9" s="29"/>
-      <c r="C9" s="19" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="10" spans="2:3">
-      <c r="B10" s="30"/>
-      <c r="C10" s="19" t="s">
-        <v>152</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Sprint 8 - correciones
</commit_message>
<xml_diff>
--- a/Documentos/ProductBacklogCorregido.xlsx
+++ b/Documentos/ProductBacklogCorregido.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://liveespochedu-my.sharepoint.com/personal/jonathan_aucancela_espoch_edu_ec/Documents/Documentos/Espoch/Octavo/Aplicaciones informáticas 2/SGT/Documentos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="91" documentId="13_ncr:1_{B9B78D3F-7366-4A45-83C5-702E4F60A49B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B2658C80-DFC5-4EC3-96DA-F042EE1875BD}"/>
+  <xr:revisionPtr revIDLastSave="179" documentId="13_ncr:1_{B9B78D3F-7366-4A45-83C5-702E4F60A49B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{749C93F4-35E8-4E3E-B252-85F60E522C8F}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{7A8F741B-9112-4896-B995-875A9BDE94F9}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{7A8F741B-9112-4896-B995-875A9BDE94F9}"/>
   </bookViews>
   <sheets>
     <sheet name="Final" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="430" uniqueCount="340">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="436" uniqueCount="345">
   <si>
     <t>Product Backlog - SecuraBank</t>
   </si>
@@ -1003,9 +1003,6 @@
     <t>Realizar los diagramas de actividades de los modulos de transacciones, cuentas, login, MFA, y seguridad</t>
   </si>
   <si>
-    <t>Restablecer la contraseña por correo implmentado normas de control</t>
-  </si>
-  <si>
     <t>Diseñar la conexión mediante las reglas del negocio para transacciones y cuentas</t>
   </si>
   <si>
@@ -1027,9 +1024,6 @@
     <t>Configurar apartado de blocklist para token caducados y bloqueados</t>
   </si>
   <si>
-    <t xml:space="preserve">Configurar interfaces claras </t>
-  </si>
-  <si>
     <t>Implementación y controle de seguridad para transacciones</t>
   </si>
   <si>
@@ -1114,51 +1108,6 @@
     <t>Validar entradas y realizar pruebas de seguridad."</t>
   </si>
   <si>
-    <t>Configurar interfaces claras</t>
-  </si>
-  <si>
-    <t>"Diseño intuitivo validado por usuarios.</t>
-  </si>
-  <si>
-    <t>Cumplir con estándares de accesibilidad (WCAG).</t>
-  </si>
-  <si>
-    <t>Navegación fluida sin errores de carga."</t>
-  </si>
-  <si>
-    <t>"Diseñar interfaces en Figma o similar.</t>
-  </si>
-  <si>
-    <t>Implementar prototipos y validar con pruebas de usuarios.</t>
-  </si>
-  <si>
-    <t>Ajustar diseño tras retroalimentación."</t>
-  </si>
-  <si>
-    <t>HU01</t>
-  </si>
-  <si>
-    <t>"Diseño intuitivo aprobado por usuarios finales.</t>
-  </si>
-  <si>
-    <t>Cumplimiento de estándares de accesibilidad (WCAG).</t>
-  </si>
-  <si>
-    <t>Sin errores de navegación o carga."</t>
-  </si>
-  <si>
-    <t>"Diseñar interfaces iniciales en Figma o herramienta similar.</t>
-  </si>
-  <si>
-    <t>Validar diseño con pruebas de usuarios.</t>
-  </si>
-  <si>
-    <t>Implementar ajustes basados en retroalimentación."</t>
-  </si>
-  <si>
-    <t>HU02</t>
-  </si>
-  <si>
     <t>Restablecer la contraseña por correo implementando normas de control</t>
   </si>
   <si>
@@ -1180,9 +1129,6 @@
     <t>Probar el flujo con casos reales."</t>
   </si>
   <si>
-    <t>HU03</t>
-  </si>
-  <si>
     <t>Realizar los diagramas de actividades de los módulos de transacciones, cuentas, login, MFA y seguridad</t>
   </si>
   <si>
@@ -1202,6 +1148,75 @@
   </si>
   <si>
     <t>Validar los diagramas con el equipo."</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Establecer la contraseña por correo aplicando las reglas de regocio </t>
+  </si>
+  <si>
+    <t>Implementar mecanismos de seguridad al modulo de restablecer contraseña</t>
+  </si>
+  <si>
+    <t>HT24</t>
+  </si>
+  <si>
+    <t>Verificación del correo del usuario.</t>
+  </si>
+  <si>
+    <t>Configurar validaciones en el backend.</t>
+  </si>
+  <si>
+    <t>La contraseña debe cumplir con los requisitos de complejidad establecidos (longitud mínima, caracteres especiales, etc.).</t>
+  </si>
+  <si>
+    <t>Mensajes de validación claros en caso de error</t>
+  </si>
+  <si>
+    <t>Definir reglas de negocio para contraseñas.</t>
+  </si>
+  <si>
+    <t>Probar el flujo con diferentes casos de prueba</t>
+  </si>
+  <si>
+    <t>Validación de identidad del usuario (MFA o preguntas de seguridad).</t>
+  </si>
+  <si>
+    <t>Enlaces de restablecimiento deben caducar tras un tiempo definido.</t>
+  </si>
+  <si>
+    <t>Proceso debe estar protegido contra ataques de fuerza bruta o phishing.</t>
+  </si>
+  <si>
+    <t>"Integrar mecanismos de validación de identidad.</t>
+  </si>
+  <si>
+    <t>Configurar tiempo de expiración para enlaces de restablecimiento.</t>
+  </si>
+  <si>
+    <t>Probar flujo con escenarios simulados."</t>
+  </si>
+  <si>
+    <t>HT25</t>
+  </si>
+  <si>
+    <t>HT26</t>
+  </si>
+  <si>
+    <t>HT27</t>
+  </si>
+  <si>
+    <t>HT28</t>
+  </si>
+  <si>
+    <t>HT29</t>
+  </si>
+  <si>
+    <t>HT30</t>
+  </si>
+  <si>
+    <t>HU6</t>
+  </si>
+  <si>
+    <t>HU7</t>
   </si>
 </sst>
 </file>
@@ -1449,7 +1464,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1527,6 +1542,12 @@
     <xf numFmtId="0" fontId="7" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1560,11 +1581,12 @@
     <xf numFmtId="0" fontId="0" fillId="10" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1586,6 +1608,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1907,8 +1933,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83A87B21-3BDC-40F9-B20F-2399C52423D9}">
   <dimension ref="A1:G42"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D29" activeCellId="1" sqref="D31 D29"/>
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D29" sqref="D29:D31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
@@ -1954,7 +1980,7 @@
       </c>
     </row>
     <row r="3" spans="1:7" ht="43.2" hidden="1" customHeight="1">
-      <c r="A3" s="27" t="s">
+      <c r="A3" s="29" t="s">
         <v>27</v>
       </c>
       <c r="B3" s="2" t="s">
@@ -1977,7 +2003,7 @@
       </c>
     </row>
     <row r="4" spans="1:7" ht="39" hidden="1" customHeight="1">
-      <c r="A4" s="28"/>
+      <c r="A4" s="30"/>
       <c r="B4" s="2" t="s">
         <v>4</v>
       </c>
@@ -1998,7 +2024,7 @@
       </c>
     </row>
     <row r="5" spans="1:7" ht="45.6" hidden="1" customHeight="1">
-      <c r="A5" s="28"/>
+      <c r="A5" s="30"/>
       <c r="B5" s="2" t="s">
         <v>21</v>
       </c>
@@ -2019,7 +2045,7 @@
       </c>
     </row>
     <row r="6" spans="1:7" ht="36" hidden="1" customHeight="1">
-      <c r="A6" s="28"/>
+      <c r="A6" s="30"/>
       <c r="B6" s="2" t="s">
         <v>22</v>
       </c>
@@ -2040,7 +2066,7 @@
       </c>
     </row>
     <row r="7" spans="1:7" ht="39" hidden="1" customHeight="1">
-      <c r="A7" s="29"/>
+      <c r="A7" s="31"/>
       <c r="B7" s="2" t="s">
         <v>153</v>
       </c>
@@ -2061,7 +2087,7 @@
       </c>
     </row>
     <row r="8" spans="1:7" ht="37.799999999999997" hidden="1" customHeight="1">
-      <c r="A8" s="27" t="s">
+      <c r="A8" s="29" t="s">
         <v>7</v>
       </c>
       <c r="B8" s="2" t="s">
@@ -2084,7 +2110,7 @@
       </c>
     </row>
     <row r="9" spans="1:7" ht="43.2" hidden="1" customHeight="1">
-      <c r="A9" s="28"/>
+      <c r="A9" s="30"/>
       <c r="B9" s="2" t="s">
         <v>30</v>
       </c>
@@ -2105,7 +2131,7 @@
       </c>
     </row>
     <row r="10" spans="1:7" ht="39.6" hidden="1" customHeight="1">
-      <c r="A10" s="28"/>
+      <c r="A10" s="30"/>
       <c r="B10" s="2" t="s">
         <v>32</v>
       </c>
@@ -2126,7 +2152,7 @@
       </c>
     </row>
     <row r="11" spans="1:7" ht="40.200000000000003" hidden="1" customHeight="1">
-      <c r="A11" s="28"/>
+      <c r="A11" s="30"/>
       <c r="B11" s="2" t="s">
         <v>34</v>
       </c>
@@ -2147,7 +2173,7 @@
       </c>
     </row>
     <row r="12" spans="1:7" ht="50.4" hidden="1" customHeight="1">
-      <c r="A12" s="29"/>
+      <c r="A12" s="31"/>
       <c r="B12" s="2" t="s">
         <v>52</v>
       </c>
@@ -2168,7 +2194,7 @@
       </c>
     </row>
     <row r="13" spans="1:7" ht="48.6" hidden="1" customHeight="1">
-      <c r="A13" s="27" t="s">
+      <c r="A13" s="29" t="s">
         <v>9</v>
       </c>
       <c r="B13" s="2" t="s">
@@ -2191,7 +2217,7 @@
       </c>
     </row>
     <row r="14" spans="1:7" ht="54.6" hidden="1" customHeight="1">
-      <c r="A14" s="28"/>
+      <c r="A14" s="30"/>
       <c r="B14" s="2" t="s">
         <v>155</v>
       </c>
@@ -2212,7 +2238,7 @@
       </c>
     </row>
     <row r="15" spans="1:7" ht="45.6" hidden="1" customHeight="1">
-      <c r="A15" s="29"/>
+      <c r="A15" s="31"/>
       <c r="B15" s="2" t="s">
         <v>156</v>
       </c>
@@ -2233,7 +2259,7 @@
       </c>
     </row>
     <row r="16" spans="1:7" ht="51.6" hidden="1" customHeight="1">
-      <c r="A16" s="27" t="s">
+      <c r="A16" s="29" t="s">
         <v>160</v>
       </c>
       <c r="B16" s="2" t="s">
@@ -2256,7 +2282,7 @@
       </c>
     </row>
     <row r="17" spans="1:7" ht="58.8" hidden="1" customHeight="1">
-      <c r="A17" s="28"/>
+      <c r="A17" s="30"/>
       <c r="B17" s="2" t="s">
         <v>159</v>
       </c>
@@ -2277,7 +2303,7 @@
       </c>
     </row>
     <row r="18" spans="1:7" ht="53.4" hidden="1" customHeight="1">
-      <c r="A18" s="29"/>
+      <c r="A18" s="31"/>
       <c r="B18" s="2" t="s">
         <v>157</v>
       </c>
@@ -2298,7 +2324,7 @@
       </c>
     </row>
     <row r="19" spans="1:7" ht="43.2" hidden="1" customHeight="1">
-      <c r="A19" s="30" t="s">
+      <c r="A19" s="32" t="s">
         <v>210</v>
       </c>
       <c r="B19" s="2" t="s">
@@ -2321,7 +2347,7 @@
       </c>
     </row>
     <row r="20" spans="1:7" ht="43.2" hidden="1">
-      <c r="A20" s="30"/>
+      <c r="A20" s="32"/>
       <c r="B20" s="2" t="s">
         <v>205</v>
       </c>
@@ -2342,7 +2368,7 @@
       </c>
     </row>
     <row r="21" spans="1:7" ht="31.2" hidden="1" customHeight="1">
-      <c r="A21" s="30"/>
+      <c r="A21" s="32"/>
       <c r="B21" s="2" t="s">
         <v>206</v>
       </c>
@@ -2363,7 +2389,7 @@
       </c>
     </row>
     <row r="22" spans="1:7" ht="34.200000000000003" hidden="1" customHeight="1">
-      <c r="A22" s="30"/>
+      <c r="A22" s="32"/>
       <c r="B22" s="2" t="s">
         <v>211</v>
       </c>
@@ -2383,8 +2409,8 @@
         <v>217</v>
       </c>
     </row>
-    <row r="23" spans="1:7" ht="43.2" hidden="1">
-      <c r="A23" s="27" t="s">
+    <row r="23" spans="1:7" ht="43.2">
+      <c r="A23" s="29" t="s">
         <v>20</v>
       </c>
       <c r="B23" s="2" t="s">
@@ -2406,8 +2432,8 @@
         <v>216</v>
       </c>
     </row>
-    <row r="24" spans="1:7" ht="28.8" hidden="1">
-      <c r="A24" s="28"/>
+    <row r="24" spans="1:7" ht="28.8">
+      <c r="A24" s="30"/>
       <c r="B24" s="2" t="s">
         <v>213</v>
       </c>
@@ -2427,8 +2453,8 @@
         <v>215</v>
       </c>
     </row>
-    <row r="25" spans="1:7" ht="43.2" hidden="1">
-      <c r="A25" s="29"/>
+    <row r="25" spans="1:7" ht="43.2">
+      <c r="A25" s="31"/>
       <c r="B25" s="2" t="s">
         <v>214</v>
       </c>
@@ -2445,11 +2471,11 @@
         <v>1</v>
       </c>
       <c r="G25" s="2" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="26" spans="1:7" ht="45" customHeight="1">
-      <c r="A26" s="27" t="s">
+      <c r="A26" s="29" t="s">
         <v>269</v>
       </c>
       <c r="B26" s="2" t="s">
@@ -2465,14 +2491,14 @@
         <v>4</v>
       </c>
       <c r="F26" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G26" s="2" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
     </row>
     <row r="27" spans="1:7" ht="41.4" customHeight="1">
-      <c r="A27" s="28"/>
+      <c r="A27" s="30"/>
       <c r="B27" s="2" t="s">
         <v>263</v>
       </c>
@@ -2480,20 +2506,20 @@
         <v>24</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="E27" s="2">
         <v>4</v>
       </c>
       <c r="F27" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G27" s="2" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
     </row>
     <row r="28" spans="1:7" ht="38.4" customHeight="1">
-      <c r="A28" s="29"/>
+      <c r="A28" s="31"/>
       <c r="B28" s="2" t="s">
         <v>264</v>
       </c>
@@ -2501,7 +2527,7 @@
         <v>24</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="E28" s="2">
         <v>4</v>
@@ -2510,21 +2536,21 @@
         <v>1</v>
       </c>
       <c r="G28" s="2" t="s">
-        <v>286</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" ht="28.8" customHeight="1">
-      <c r="A29" s="27" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" ht="44.4" customHeight="1">
+      <c r="A29" s="29" t="s">
         <v>270</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="C29" s="10" t="s">
         <v>24</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>281</v>
+        <v>322</v>
       </c>
       <c r="E29" s="2">
         <v>4</v>
@@ -2533,19 +2559,19 @@
         <v>1</v>
       </c>
       <c r="G29" s="2" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" ht="43.2">
-      <c r="A30" s="28"/>
+        <v>283</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" ht="58.2" customHeight="1">
+      <c r="A30" s="30"/>
       <c r="B30" s="2" t="s">
-        <v>268</v>
+        <v>324</v>
       </c>
       <c r="C30" s="10" t="s">
         <v>24</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>273</v>
+        <v>323</v>
       </c>
       <c r="E30" s="2">
         <v>4</v>
@@ -2554,11 +2580,11 @@
         <v>1</v>
       </c>
       <c r="G30" s="2" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
     </row>
     <row r="31" spans="1:7" ht="57.6">
-      <c r="A31" s="29"/>
+      <c r="A31" s="31"/>
       <c r="B31" s="2" t="s">
         <v>267</v>
       </c>
@@ -2572,14 +2598,14 @@
         <v>4</v>
       </c>
       <c r="F31" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G31" s="2" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
     </row>
     <row r="32" spans="1:7" ht="28.8">
-      <c r="A32" s="27" t="s">
+      <c r="A32" s="29" t="s">
         <v>271</v>
       </c>
       <c r="B32" s="2"/>
@@ -2598,13 +2624,13 @@
       <c r="G32" s="2"/>
     </row>
     <row r="33" spans="1:7" ht="43.2">
-      <c r="A33" s="28"/>
+      <c r="A33" s="30"/>
       <c r="B33" s="2"/>
       <c r="C33" s="11" t="s">
         <v>5</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="E33" s="2">
         <v>4</v>
@@ -2615,13 +2641,13 @@
       <c r="G33" s="2"/>
     </row>
     <row r="34" spans="1:7" ht="28.8">
-      <c r="A34" s="29"/>
+      <c r="A34" s="31"/>
       <c r="B34" s="2"/>
       <c r="C34" s="11" t="s">
         <v>5</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="E34" s="2">
         <v>4</v>
@@ -2632,8 +2658,8 @@
       <c r="G34" s="2"/>
     </row>
     <row r="35" spans="1:7">
-      <c r="A35" s="27" t="s">
-        <v>276</v>
+      <c r="A35" s="29" t="s">
+        <v>275</v>
       </c>
       <c r="B35" s="2"/>
       <c r="C35" s="11" t="s">
@@ -2651,13 +2677,13 @@
       <c r="G35" s="2"/>
     </row>
     <row r="36" spans="1:7">
-      <c r="A36" s="29"/>
+      <c r="A36" s="31"/>
       <c r="B36" s="2"/>
       <c r="C36" s="11" t="s">
         <v>5</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="E36" s="2">
         <v>4</v>
@@ -2668,8 +2694,8 @@
       <c r="G36" s="2"/>
     </row>
     <row r="37" spans="1:7" ht="43.2">
-      <c r="A37" s="39" t="s">
-        <v>277</v>
+      <c r="A37" s="28" t="s">
+        <v>276</v>
       </c>
       <c r="B37" s="2"/>
       <c r="C37" s="11" t="s">
@@ -2687,7 +2713,7 @@
       <c r="G37" s="2"/>
     </row>
     <row r="38" spans="1:7" ht="43.2">
-      <c r="A38" s="38"/>
+      <c r="A38" s="27"/>
       <c r="B38" s="2"/>
       <c r="C38" s="11" t="s">
         <v>5</v>
@@ -2704,7 +2730,7 @@
       <c r="G38" s="2"/>
     </row>
     <row r="39" spans="1:7" ht="28.8">
-      <c r="A39" s="38"/>
+      <c r="A39" s="27"/>
       <c r="B39" s="2"/>
       <c r="C39" s="11" t="s">
         <v>5</v>
@@ -2722,7 +2748,7 @@
     </row>
     <row r="40" spans="1:7" ht="28.8">
       <c r="A40" s="9" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B40" s="2"/>
       <c r="C40" s="11" t="s">
@@ -2775,16 +2801,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="A16:A18"/>
+    <mergeCell ref="A3:A7"/>
+    <mergeCell ref="A8:A12"/>
+    <mergeCell ref="A13:A15"/>
+    <mergeCell ref="A19:A22"/>
     <mergeCell ref="A29:A31"/>
     <mergeCell ref="A32:A34"/>
     <mergeCell ref="A35:A36"/>
     <mergeCell ref="A26:A28"/>
     <mergeCell ref="A23:A25"/>
-    <mergeCell ref="A16:A18"/>
-    <mergeCell ref="A3:A7"/>
-    <mergeCell ref="A8:A12"/>
-    <mergeCell ref="A13:A15"/>
-    <mergeCell ref="A19:A22"/>
   </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2793,10 +2819,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68EE2C79-A7B0-4BE1-9026-6C6F59ABCFC9}">
-  <dimension ref="A1:D41"/>
+  <dimension ref="A1:D62"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E27" sqref="E27"/>
+    <sheetView topLeftCell="A35" workbookViewId="0">
+      <selection activeCell="C56" sqref="C56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
@@ -3004,10 +3030,10 @@
       </c>
     </row>
     <row r="15" spans="1:4" ht="28.8" hidden="1">
-      <c r="A15" s="31" t="s">
+      <c r="A15" s="33" t="s">
         <v>205</v>
       </c>
-      <c r="B15" s="32" t="s">
+      <c r="B15" s="34" t="s">
         <v>220</v>
       </c>
       <c r="C15" s="26" t="s">
@@ -3018,8 +3044,8 @@
       </c>
     </row>
     <row r="16" spans="1:4" ht="28.8" hidden="1">
-      <c r="A16" s="31"/>
-      <c r="B16" s="33"/>
+      <c r="A16" s="33"/>
+      <c r="B16" s="35"/>
       <c r="C16" s="26" t="s">
         <v>222</v>
       </c>
@@ -3028,8 +3054,8 @@
       </c>
     </row>
     <row r="17" spans="1:4" ht="28.8" hidden="1">
-      <c r="A17" s="31"/>
-      <c r="B17" s="34"/>
+      <c r="A17" s="33"/>
+      <c r="B17" s="36"/>
       <c r="C17" s="26" t="s">
         <v>223</v>
       </c>
@@ -3038,10 +3064,10 @@
       </c>
     </row>
     <row r="18" spans="1:4" ht="43.2" hidden="1">
-      <c r="A18" s="31" t="s">
+      <c r="A18" s="33" t="s">
         <v>206</v>
       </c>
-      <c r="B18" s="32" t="s">
+      <c r="B18" s="34" t="s">
         <v>227</v>
       </c>
       <c r="C18" s="26" t="s">
@@ -3052,8 +3078,8 @@
       </c>
     </row>
     <row r="19" spans="1:4" ht="28.8" hidden="1">
-      <c r="A19" s="31"/>
-      <c r="B19" s="33"/>
+      <c r="A19" s="33"/>
+      <c r="B19" s="35"/>
       <c r="C19" s="26" t="s">
         <v>229</v>
       </c>
@@ -3062,8 +3088,8 @@
       </c>
     </row>
     <row r="20" spans="1:4" ht="28.8" hidden="1">
-      <c r="A20" s="31"/>
-      <c r="B20" s="34"/>
+      <c r="A20" s="33"/>
+      <c r="B20" s="36"/>
       <c r="C20" s="26" t="s">
         <v>230</v>
       </c>
@@ -3072,10 +3098,10 @@
       </c>
     </row>
     <row r="21" spans="1:4" ht="28.8" hidden="1">
-      <c r="A21" s="31" t="s">
+      <c r="A21" s="33" t="s">
         <v>211</v>
       </c>
-      <c r="B21" s="32" t="s">
+      <c r="B21" s="34" t="s">
         <v>240</v>
       </c>
       <c r="C21" s="22" t="s">
@@ -3086,8 +3112,8 @@
       </c>
     </row>
     <row r="22" spans="1:4" ht="28.8" hidden="1">
-      <c r="A22" s="31"/>
-      <c r="B22" s="33"/>
+      <c r="A22" s="33"/>
+      <c r="B22" s="35"/>
       <c r="C22" s="22" t="s">
         <v>235</v>
       </c>
@@ -3096,8 +3122,8 @@
       </c>
     </row>
     <row r="23" spans="1:4" ht="28.8" hidden="1">
-      <c r="A23" s="31"/>
-      <c r="B23" s="34"/>
+      <c r="A23" s="33"/>
+      <c r="B23" s="36"/>
       <c r="C23" s="22" t="s">
         <v>236</v>
       </c>
@@ -3106,10 +3132,10 @@
       </c>
     </row>
     <row r="24" spans="1:4" ht="28.8">
-      <c r="A24" s="31" t="s">
+      <c r="A24" s="33" t="s">
         <v>213</v>
       </c>
-      <c r="B24" s="32" t="s">
+      <c r="B24" s="34" t="s">
         <v>241</v>
       </c>
       <c r="C24" s="25" t="s">
@@ -3120,8 +3146,8 @@
       </c>
     </row>
     <row r="25" spans="1:4" ht="28.8">
-      <c r="A25" s="31"/>
-      <c r="B25" s="33"/>
+      <c r="A25" s="33"/>
+      <c r="B25" s="35"/>
       <c r="C25" s="25" t="s">
         <v>243</v>
       </c>
@@ -3130,8 +3156,8 @@
       </c>
     </row>
     <row r="26" spans="1:4" ht="28.8">
-      <c r="A26" s="31"/>
-      <c r="B26" s="34"/>
+      <c r="A26" s="33"/>
+      <c r="B26" s="36"/>
       <c r="C26" s="25" t="s">
         <v>244</v>
       </c>
@@ -3140,10 +3166,10 @@
       </c>
     </row>
     <row r="27" spans="1:4" ht="28.8">
-      <c r="A27" s="31" t="s">
+      <c r="A27" s="33" t="s">
         <v>214</v>
       </c>
-      <c r="B27" s="32" t="s">
+      <c r="B27" s="34" t="s">
         <v>248</v>
       </c>
       <c r="C27" s="25" t="s">
@@ -3154,8 +3180,8 @@
       </c>
     </row>
     <row r="28" spans="1:4" ht="28.8">
-      <c r="A28" s="31"/>
-      <c r="B28" s="33"/>
+      <c r="A28" s="33"/>
+      <c r="B28" s="35"/>
       <c r="C28" s="25" t="s">
         <v>250</v>
       </c>
@@ -3164,8 +3190,8 @@
       </c>
     </row>
     <row r="29" spans="1:4" ht="28.8">
-      <c r="A29" s="31"/>
-      <c r="B29" s="34"/>
+      <c r="A29" s="33"/>
+      <c r="B29" s="36"/>
       <c r="C29" s="25" t="s">
         <v>251</v>
       </c>
@@ -3174,143 +3200,319 @@
       </c>
     </row>
     <row r="30" spans="1:4" ht="14.4" customHeight="1">
-      <c r="A30" s="31" t="s">
-        <v>205</v>
-      </c>
-      <c r="B30" s="32" t="s">
+      <c r="A30" s="33" t="s">
+        <v>262</v>
+      </c>
+      <c r="B30" s="34" t="s">
         <v>265</v>
       </c>
       <c r="C30" s="25" t="s">
+        <v>288</v>
+      </c>
+      <c r="D30" s="25" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" ht="33" customHeight="1">
+      <c r="A31" s="33"/>
+      <c r="B31" s="35"/>
+      <c r="C31" s="25" t="s">
+        <v>289</v>
+      </c>
+      <c r="D31" s="25" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" ht="24" customHeight="1">
+      <c r="A32" s="33"/>
+      <c r="B32" s="36"/>
+      <c r="C32" s="25" t="s">
         <v>290</v>
       </c>
-      <c r="D30" s="25" t="s">
+      <c r="D32" s="25" t="s">
         <v>293</v>
       </c>
     </row>
-    <row r="31" spans="1:4" ht="33" customHeight="1">
-      <c r="A31" s="31"/>
-      <c r="B31" s="33"/>
-      <c r="C31" s="25" t="s">
-        <v>291</v>
-      </c>
-      <c r="D31" s="25" t="s">
+    <row r="33" spans="1:4" ht="36.6" customHeight="1">
+      <c r="A33" s="33" t="s">
+        <v>263</v>
+      </c>
+      <c r="B33" s="34" t="s">
         <v>294</v>
       </c>
-    </row>
-    <row r="32" spans="1:4" ht="24" customHeight="1">
-      <c r="A32" s="31"/>
-      <c r="B32" s="34"/>
-      <c r="C32" s="25" t="s">
-        <v>292</v>
-      </c>
-      <c r="D32" s="25" t="s">
+      <c r="C33" s="25" t="s">
         <v>295</v>
       </c>
-    </row>
-    <row r="33" spans="1:4" ht="36.6" customHeight="1">
-      <c r="A33" s="31" t="s">
-        <v>206</v>
-      </c>
-      <c r="B33" s="32" t="s">
+      <c r="D33" s="25" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" ht="26.4" customHeight="1">
+      <c r="A34" s="33"/>
+      <c r="B34" s="35"/>
+      <c r="C34" s="25" t="s">
         <v>296</v>
       </c>
-      <c r="C33" s="25" t="s">
+      <c r="D34" s="25" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" ht="24" customHeight="1">
+      <c r="A35" s="33"/>
+      <c r="B35" s="36"/>
+      <c r="C35" s="25" t="s">
         <v>297</v>
       </c>
-      <c r="D33" s="25" t="s">
+      <c r="D35" s="25" t="s">
         <v>300</v>
       </c>
     </row>
-    <row r="34" spans="1:4" ht="26.4" customHeight="1">
-      <c r="A34" s="31"/>
-      <c r="B34" s="33"/>
-      <c r="C34" s="25" t="s">
-        <v>298</v>
-      </c>
-      <c r="D34" s="25" t="s">
+    <row r="36" spans="1:4" ht="36.6" customHeight="1">
+      <c r="A36" s="33" t="s">
+        <v>264</v>
+      </c>
+      <c r="B36" s="34" t="s">
         <v>301</v>
       </c>
-    </row>
-    <row r="35" spans="1:4" ht="24" customHeight="1">
-      <c r="A35" s="31"/>
-      <c r="B35" s="34"/>
-      <c r="C35" s="25" t="s">
-        <v>299</v>
-      </c>
-      <c r="D35" s="25" t="s">
+      <c r="C36" s="22" t="s">
         <v>302</v>
       </c>
-    </row>
-    <row r="36" spans="1:4" ht="21.6" customHeight="1">
-      <c r="A36" s="31" t="s">
-        <v>211</v>
-      </c>
-      <c r="B36" s="32" t="s">
+      <c r="D36" s="22" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" ht="34.200000000000003" customHeight="1">
+      <c r="A37" s="33"/>
+      <c r="B37" s="35"/>
+      <c r="C37" s="22" t="s">
         <v>303</v>
       </c>
-      <c r="C36" s="25" t="s">
+      <c r="D37" s="22" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" ht="30" customHeight="1">
+      <c r="A38" s="33"/>
+      <c r="B38" s="36"/>
+      <c r="C38" s="22" t="s">
         <v>304</v>
       </c>
-      <c r="D36" s="25" t="s">
+      <c r="D38" s="22" t="s">
         <v>307</v>
       </c>
     </row>
-    <row r="37" spans="1:4" ht="24" customHeight="1">
-      <c r="A37" s="31"/>
-      <c r="B37" s="33"/>
-      <c r="C37" s="25" t="s">
-        <v>305</v>
-      </c>
-      <c r="D37" s="25" t="s">
-        <v>308</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4">
-      <c r="A38" s="31"/>
-      <c r="B38" s="34"/>
-      <c r="C38" s="25" t="s">
-        <v>306</v>
-      </c>
-      <c r="D38" s="25" t="s">
-        <v>309</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" ht="23.4" customHeight="1">
-      <c r="A39" s="31" t="s">
-        <v>213</v>
-      </c>
-      <c r="B39" s="32" t="s">
-        <v>310</v>
-      </c>
-      <c r="C39" s="25" t="s">
-        <v>311</v>
-      </c>
-      <c r="D39" s="25" t="s">
-        <v>314</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4">
-      <c r="A40" s="31"/>
-      <c r="B40" s="33"/>
-      <c r="C40" s="25" t="s">
-        <v>312</v>
-      </c>
-      <c r="D40" s="25" t="s">
-        <v>315</v>
+    <row r="39" spans="1:4" ht="61.2" customHeight="1">
+      <c r="A39" s="33" t="s">
+        <v>268</v>
+      </c>
+      <c r="B39" s="40" t="s">
+        <v>322</v>
+      </c>
+      <c r="C39" s="22" t="s">
+        <v>327</v>
+      </c>
+      <c r="D39" s="42" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" ht="23.4" customHeight="1">
+      <c r="A40" s="33"/>
+      <c r="B40" s="40"/>
+      <c r="C40" s="42" t="s">
+        <v>325</v>
+      </c>
+      <c r="D40" s="42" t="s">
+        <v>326</v>
       </c>
     </row>
     <row r="41" spans="1:4" ht="25.2" customHeight="1">
-      <c r="A41" s="31"/>
-      <c r="B41" s="34"/>
-      <c r="C41" s="25" t="s">
-        <v>313</v>
-      </c>
-      <c r="D41" s="25" t="s">
-        <v>316</v>
-      </c>
+      <c r="A41" s="33"/>
+      <c r="B41" s="40"/>
+      <c r="C41" s="42" t="s">
+        <v>328</v>
+      </c>
+      <c r="D41" s="42" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" ht="43.2" customHeight="1">
+      <c r="A42" s="33" t="s">
+        <v>324</v>
+      </c>
+      <c r="B42" s="40" t="s">
+        <v>323</v>
+      </c>
+      <c r="C42" s="22" t="s">
+        <v>331</v>
+      </c>
+      <c r="D42" s="22" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" ht="28.8">
+      <c r="A43" s="33"/>
+      <c r="B43" s="40"/>
+      <c r="C43" s="22" t="s">
+        <v>332</v>
+      </c>
+      <c r="D43" s="22" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" ht="28.8">
+      <c r="A44" s="33"/>
+      <c r="B44" s="40"/>
+      <c r="C44" s="22" t="s">
+        <v>333</v>
+      </c>
+      <c r="D44" s="22" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4">
+      <c r="A45" s="33" t="s">
+        <v>337</v>
+      </c>
+      <c r="B45" s="40"/>
+      <c r="C45" s="41"/>
+      <c r="D45" s="41"/>
+    </row>
+    <row r="46" spans="1:4">
+      <c r="A46" s="33"/>
+      <c r="B46" s="40"/>
+      <c r="C46" s="41"/>
+      <c r="D46" s="41"/>
+    </row>
+    <row r="47" spans="1:4">
+      <c r="A47" s="33"/>
+      <c r="B47" s="40"/>
+      <c r="C47" s="41"/>
+      <c r="D47" s="41"/>
+    </row>
+    <row r="48" spans="1:4">
+      <c r="A48" s="33" t="s">
+        <v>338</v>
+      </c>
+      <c r="B48" s="40"/>
+      <c r="C48" s="41"/>
+      <c r="D48" s="41"/>
+    </row>
+    <row r="49" spans="1:4">
+      <c r="A49" s="33"/>
+      <c r="B49" s="40"/>
+      <c r="C49" s="41"/>
+      <c r="D49" s="41"/>
+    </row>
+    <row r="50" spans="1:4">
+      <c r="A50" s="33"/>
+      <c r="B50" s="40"/>
+      <c r="C50" s="41"/>
+      <c r="D50" s="41"/>
+    </row>
+    <row r="51" spans="1:4">
+      <c r="A51" s="33" t="s">
+        <v>339</v>
+      </c>
+      <c r="B51" s="40"/>
+      <c r="C51" s="41"/>
+      <c r="D51" s="41"/>
+    </row>
+    <row r="52" spans="1:4">
+      <c r="A52" s="33"/>
+      <c r="B52" s="40"/>
+      <c r="C52" s="41"/>
+      <c r="D52" s="41"/>
+    </row>
+    <row r="53" spans="1:4">
+      <c r="A53" s="33"/>
+      <c r="B53" s="40"/>
+      <c r="C53" s="41"/>
+      <c r="D53" s="41"/>
+    </row>
+    <row r="54" spans="1:4">
+      <c r="A54" s="33" t="s">
+        <v>340</v>
+      </c>
+      <c r="B54" s="40"/>
+      <c r="C54" s="41"/>
+      <c r="D54" s="41"/>
+    </row>
+    <row r="55" spans="1:4">
+      <c r="A55" s="33"/>
+      <c r="B55" s="40"/>
+      <c r="C55" s="41"/>
+      <c r="D55" s="41"/>
+    </row>
+    <row r="56" spans="1:4">
+      <c r="A56" s="33"/>
+      <c r="B56" s="40"/>
+      <c r="C56" s="41"/>
+      <c r="D56" s="41"/>
+    </row>
+    <row r="57" spans="1:4">
+      <c r="A57" s="33" t="s">
+        <v>341</v>
+      </c>
+      <c r="B57" s="40"/>
+      <c r="C57" s="41"/>
+      <c r="D57" s="41"/>
+    </row>
+    <row r="58" spans="1:4">
+      <c r="A58" s="33"/>
+      <c r="B58" s="40"/>
+      <c r="C58" s="41"/>
+      <c r="D58" s="41"/>
+    </row>
+    <row r="59" spans="1:4">
+      <c r="A59" s="33"/>
+      <c r="B59" s="40"/>
+      <c r="C59" s="41"/>
+      <c r="D59" s="41"/>
+    </row>
+    <row r="60" spans="1:4">
+      <c r="A60" s="33" t="s">
+        <v>342</v>
+      </c>
+      <c r="B60" s="40"/>
+      <c r="C60" s="41"/>
+      <c r="D60" s="41"/>
+    </row>
+    <row r="61" spans="1:4">
+      <c r="A61" s="33"/>
+      <c r="B61" s="40"/>
+      <c r="C61" s="41"/>
+      <c r="D61" s="41"/>
+    </row>
+    <row r="62" spans="1:4">
+      <c r="A62" s="33"/>
+      <c r="B62" s="40"/>
+      <c r="C62" s="41"/>
+      <c r="D62" s="41"/>
     </row>
   </sheetData>
-  <mergeCells count="18">
+  <mergeCells count="32">
+    <mergeCell ref="A60:A62"/>
+    <mergeCell ref="B45:B47"/>
+    <mergeCell ref="B48:B50"/>
+    <mergeCell ref="B51:B53"/>
+    <mergeCell ref="B54:B56"/>
+    <mergeCell ref="B57:B59"/>
+    <mergeCell ref="B60:B62"/>
+    <mergeCell ref="A45:A47"/>
+    <mergeCell ref="A48:A50"/>
+    <mergeCell ref="A51:A53"/>
+    <mergeCell ref="A54:A56"/>
+    <mergeCell ref="A57:A59"/>
+    <mergeCell ref="B42:B44"/>
+    <mergeCell ref="A42:A44"/>
+    <mergeCell ref="A39:A41"/>
+    <mergeCell ref="B39:B41"/>
+    <mergeCell ref="A30:A32"/>
+    <mergeCell ref="B30:B32"/>
+    <mergeCell ref="A33:A35"/>
+    <mergeCell ref="B33:B35"/>
+    <mergeCell ref="A36:A38"/>
+    <mergeCell ref="B36:B38"/>
     <mergeCell ref="A27:A29"/>
     <mergeCell ref="B21:B23"/>
     <mergeCell ref="B24:B26"/>
@@ -3321,14 +3523,6 @@
     <mergeCell ref="A18:A20"/>
     <mergeCell ref="A21:A23"/>
     <mergeCell ref="A24:A26"/>
-    <mergeCell ref="A39:A41"/>
-    <mergeCell ref="B39:B41"/>
-    <mergeCell ref="A30:A32"/>
-    <mergeCell ref="B30:B32"/>
-    <mergeCell ref="A33:A35"/>
-    <mergeCell ref="B33:B35"/>
-    <mergeCell ref="A36:A38"/>
-    <mergeCell ref="B36:B38"/>
   </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3337,10 +3531,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{113AD7C8-E432-4900-8C71-627982E552B0}">
-  <dimension ref="A1:D16"/>
+  <dimension ref="A1:D13"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11:B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
@@ -3407,10 +3601,10 @@
       </c>
     </row>
     <row r="5" spans="1:4" ht="28.8">
-      <c r="A5" s="31" t="s">
+      <c r="A5" s="33" t="s">
         <v>50</v>
       </c>
-      <c r="B5" s="32" t="s">
+      <c r="B5" s="34" t="s">
         <v>255</v>
       </c>
       <c r="C5" s="25" t="s">
@@ -3421,8 +3615,8 @@
       </c>
     </row>
     <row r="6" spans="1:4" ht="28.8">
-      <c r="A6" s="31"/>
-      <c r="B6" s="33"/>
+      <c r="A6" s="33"/>
+      <c r="B6" s="35"/>
       <c r="C6" s="25" t="s">
         <v>257</v>
       </c>
@@ -3431,8 +3625,8 @@
       </c>
     </row>
     <row r="7" spans="1:4" ht="43.2">
-      <c r="A7" s="31"/>
-      <c r="B7" s="34"/>
+      <c r="A7" s="33"/>
+      <c r="B7" s="36"/>
       <c r="C7" s="25" t="s">
         <v>258</v>
       </c>
@@ -3440,119 +3634,84 @@
         <v>261</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="28.8">
-      <c r="A8" s="31" t="s">
+    <row r="8" spans="1:4" ht="28.8" customHeight="1">
+      <c r="A8" s="33" t="s">
+        <v>343</v>
+      </c>
+      <c r="B8" s="34" t="s">
+        <v>308</v>
+      </c>
+      <c r="C8" s="25" t="s">
+        <v>309</v>
+      </c>
+      <c r="D8" s="25" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="28.8">
+      <c r="A9" s="33"/>
+      <c r="B9" s="35"/>
+      <c r="C9" s="25" t="s">
+        <v>310</v>
+      </c>
+      <c r="D9" s="25" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="28.8">
+      <c r="A10" s="33"/>
+      <c r="B10" s="36"/>
+      <c r="C10" s="25" t="s">
+        <v>311</v>
+      </c>
+      <c r="D10" s="25" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="14.4" customHeight="1">
+      <c r="A11" s="33" t="s">
+        <v>344</v>
+      </c>
+      <c r="B11" s="34" t="s">
+        <v>315</v>
+      </c>
+      <c r="C11" s="25" t="s">
+        <v>316</v>
+      </c>
+      <c r="D11" s="25" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="28.8">
+      <c r="A12" s="33"/>
+      <c r="B12" s="35"/>
+      <c r="C12" s="25" t="s">
         <v>317</v>
       </c>
-      <c r="B8" s="32" t="s">
-        <v>310</v>
-      </c>
-      <c r="C8" s="25" t="s">
+      <c r="D12" s="25" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13" s="33"/>
+      <c r="B13" s="36"/>
+      <c r="C13" s="25" t="s">
         <v>318</v>
       </c>
-      <c r="D8" s="25" t="s">
+      <c r="D13" s="25" t="s">
         <v>321</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="28.8">
-      <c r="A9" s="31"/>
-      <c r="B9" s="33"/>
-      <c r="C9" s="25" t="s">
-        <v>319</v>
-      </c>
-      <c r="D9" s="25" t="s">
-        <v>322</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" ht="28.8">
-      <c r="A10" s="31"/>
-      <c r="B10" s="34"/>
-      <c r="C10" s="25" t="s">
-        <v>320</v>
-      </c>
-      <c r="D10" s="25" t="s">
-        <v>323</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" ht="28.8" customHeight="1">
-      <c r="A11" s="31" t="s">
-        <v>324</v>
-      </c>
-      <c r="B11" s="32" t="s">
-        <v>325</v>
-      </c>
-      <c r="C11" s="25" t="s">
-        <v>326</v>
-      </c>
-      <c r="D11" s="25" t="s">
-        <v>329</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" ht="28.8">
-      <c r="A12" s="31"/>
-      <c r="B12" s="33"/>
-      <c r="C12" s="25" t="s">
-        <v>327</v>
-      </c>
-      <c r="D12" s="25" t="s">
-        <v>330</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" ht="28.8">
-      <c r="A13" s="31"/>
-      <c r="B13" s="34"/>
-      <c r="C13" s="25" t="s">
-        <v>328</v>
-      </c>
-      <c r="D13" s="25" t="s">
-        <v>331</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" ht="14.4" customHeight="1">
-      <c r="A14" s="31" t="s">
-        <v>332</v>
-      </c>
-      <c r="B14" s="32" t="s">
-        <v>333</v>
-      </c>
-      <c r="C14" s="25" t="s">
-        <v>334</v>
-      </c>
-      <c r="D14" s="25" t="s">
-        <v>337</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" ht="28.8">
-      <c r="A15" s="31"/>
-      <c r="B15" s="33"/>
-      <c r="C15" s="25" t="s">
-        <v>335</v>
-      </c>
-      <c r="D15" s="25" t="s">
-        <v>338</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4">
-      <c r="A16" s="31"/>
-      <c r="B16" s="34"/>
-      <c r="C16" s="25" t="s">
-        <v>336</v>
-      </c>
-      <c r="D16" s="25" t="s">
-        <v>339</v>
-      </c>
-    </row>
   </sheetData>
-  <mergeCells count="8">
-    <mergeCell ref="A14:A16"/>
-    <mergeCell ref="B14:B16"/>
+  <mergeCells count="6">
+    <mergeCell ref="A11:A13"/>
+    <mergeCell ref="B11:B13"/>
     <mergeCell ref="A5:A7"/>
     <mergeCell ref="B5:B7"/>
     <mergeCell ref="A8:A10"/>
     <mergeCell ref="B8:B10"/>
-    <mergeCell ref="A11:A13"/>
-    <mergeCell ref="B11:B13"/>
   </mergeCells>
+  <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -4107,7 +4266,7 @@
       </c>
     </row>
     <row r="8" spans="2:3">
-      <c r="B8" s="35" t="s">
+      <c r="B8" s="37" t="s">
         <v>140</v>
       </c>
       <c r="C8" s="19" t="s">
@@ -4115,13 +4274,13 @@
       </c>
     </row>
     <row r="9" spans="2:3">
-      <c r="B9" s="36"/>
+      <c r="B9" s="38"/>
       <c r="C9" s="19" t="s">
         <v>137</v>
       </c>
     </row>
     <row r="10" spans="2:3">
-      <c r="B10" s="37"/>
+      <c r="B10" s="39"/>
       <c r="C10" s="19" t="s">
         <v>138</v>
       </c>

</xml_diff>

<commit_message>
Sprint 9 - completo
</commit_message>
<xml_diff>
--- a/Documentos/ProductBacklogCorregido.xlsx
+++ b/Documentos/ProductBacklogCorregido.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://liveespochedu-my.sharepoint.com/personal/jonathan_aucancela_espoch_edu_ec/Documents/Documentos/Espoch/Octavo/Aplicaciones informáticas 2/SGT/Documentos/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\david\OneDrive - ESCUELA SUPERIOR POLITECNICA DE CHIMBORAZO\Documentos\Espoch\Octavo\Aplicaciones informáticas 2\SGT\Documentos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="179" documentId="13_ncr:1_{B9B78D3F-7366-4A45-83C5-702E4F60A49B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{749C93F4-35E8-4E3E-B252-85F60E522C8F}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{569A54D0-C256-42F5-A166-327ADD140FB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{7A8F741B-9112-4896-B995-875A9BDE94F9}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{7A8F741B-9112-4896-B995-875A9BDE94F9}"/>
   </bookViews>
   <sheets>
     <sheet name="Final" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="436" uniqueCount="345">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="481" uniqueCount="375">
   <si>
     <t>Product Backlog - SecuraBank</t>
   </si>
@@ -982,12 +982,6 @@
     <t>Implementar controles de seguridad en el ingreso (login)</t>
   </si>
   <si>
-    <t>NGIX</t>
-  </si>
-  <si>
-    <t>HU5</t>
-  </si>
-  <si>
     <t>HT23</t>
   </si>
   <si>
@@ -1006,18 +1000,9 @@
     <t>Diseñar la conexión mediante las reglas del negocio para transacciones y cuentas</t>
   </si>
   <si>
-    <t>Conexión de la base de datos para formulario de transacciones</t>
-  </si>
-  <si>
     <t>10  Pruebas</t>
   </si>
   <si>
-    <t>11 Analisis de resultado</t>
-  </si>
-  <si>
-    <t>12 Entrega final</t>
-  </si>
-  <si>
     <t>01 de enero de 2024</t>
   </si>
   <si>
@@ -1045,9 +1030,6 @@
     <t>04 de enero de 2025</t>
   </si>
   <si>
-    <t>Pruebas generales</t>
-  </si>
-  <si>
     <t>"Verificar autenticación correcta con credenciales válidas.</t>
   </si>
   <si>
@@ -1217,6 +1199,114 @@
   </si>
   <si>
     <t>HU7</t>
+  </si>
+  <si>
+    <t>15 de enero de 2025</t>
+  </si>
+  <si>
+    <t>17 de enero de 2025</t>
+  </si>
+  <si>
+    <t>18 de enero de 2025</t>
+  </si>
+  <si>
+    <t>Creación del modulo de configuración para los apartados de seguridad</t>
+  </si>
+  <si>
+    <t>Pruebas unitarias para validar la lógica de cada módulo</t>
+  </si>
+  <si>
+    <t>Pruebas de integración para asegurarse de que el front-end se comunique correctamente con la API.</t>
+  </si>
+  <si>
+    <t>NGIX para despligue de correos</t>
+  </si>
+  <si>
+    <t>11 Correciones y mejoras</t>
+  </si>
+  <si>
+    <t xml:space="preserve">12 Entrega </t>
+  </si>
+  <si>
+    <t>HU8</t>
+  </si>
+  <si>
+    <t>19 de enero de 2025</t>
+  </si>
+  <si>
+    <t>HT31</t>
+  </si>
+  <si>
+    <t>HT32</t>
+  </si>
+  <si>
+    <t>HT33</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Creación de una barra de navegación Layout para los distintos componentes </t>
+  </si>
+  <si>
+    <t>Control del modulo de cuentas mediante superusuario</t>
+  </si>
+  <si>
+    <t>Desarrollar e implementar un módulo que gestione la conexión y las interacciones entre transacciones y cuentas, siguiendo las reglas de negocio establecidas.</t>
+  </si>
+  <si>
+    <t>Este módulo deberá asegurar la integridad y seguridad de los datos</t>
+  </si>
+  <si>
+    <t>Validar que todas las operaciones respeten las reglas definidas</t>
+  </si>
+  <si>
+    <t>Confirmar que solo usuarios autorizados puedan realizar o modificar transacciones.</t>
+  </si>
+  <si>
+    <t>Asegurar la encriptación de datos sensibles durante la transmisión y almacenamiento.</t>
+  </si>
+  <si>
+    <t>Desarrollar un módulo de configuración dedicado a gestionar todos los aspectos de seguridad del sistema.</t>
+  </si>
+  <si>
+    <t>Este módulo permitirá la configuración de políticas de acceso, gestión de roles, autenticación, autorización y otros parámetros de seguridad necesarios para proteger el sistema.</t>
+  </si>
+  <si>
+    <t>Verificar que los administradores puedan modificar las políticas de seguridad sin necesidad de cambios en el código.</t>
+  </si>
+  <si>
+    <t>Asegurar que los roles se puedan crear, modificar y asignar correctamente.</t>
+  </si>
+  <si>
+    <t>Implementar las funcionalidades de configuración de seguridad, incluyendo gestión de roles, políticas de acceso y mecanismos de autenticación.</t>
+  </si>
+  <si>
+    <t>Implementar funcionalidades que permitan a un superusuario tener control total sobre el módulo de cuentas.</t>
+  </si>
+  <si>
+    <t>Asegurar que el superusuario pueda realizar todas las operaciones CRUD (Crear, Leer, Actualizar, Eliminar) sobre las cuentas.</t>
+  </si>
+  <si>
+    <t>Verificar que las credenciales y sesiones del superusuario estén protegidas contra accesos no autorizados.</t>
+  </si>
+  <si>
+    <t>Implementar las funcionalidades de gestión completa de cuentas, asegurando que se respeten las restricciones de seguridad.</t>
+  </si>
+  <si>
+    <t>Revisar y validar el diseño con los stakeholders para asegurar que cumple con las expectativas y requerimientos.</t>
+  </si>
+  <si>
+    <t>Identificar las funcionalidades y elementos que debe incluir la barra de navegación (por ejemplo, enlaces, menús desplegables, iconos).</t>
+  </si>
+  <si>
+    <t>Elegir las tecnologías y frameworks adecuados Django y React</t>
+  </si>
+  <si>
+    <t>Aplicar estilos CSS para el diseño visual y asegurar la responsividad en diferentes dispositivos.</t>
+  </si>
+  <si>
+    <t>Verificar que todos los enlaces y menús funcionen correctamente.</t>
+  </si>
+  <si>
+    <t>Monitorear su rendimiento y realizar ajustes según sea necesario para mantener la eficiencia y funcionalidad.</t>
   </si>
 </sst>
 </file>
@@ -1464,7 +1554,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1489,9 +1579,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1542,11 +1629,9 @@
     <xf numFmtId="0" fontId="7" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1561,6 +1646,9 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1581,12 +1669,17 @@
     <xf numFmtId="0" fontId="0" fillId="10" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1608,10 +1701,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1931,10 +2020,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83A87B21-3BDC-40F9-B20F-2399C52423D9}">
-  <dimension ref="A1:G42"/>
+  <dimension ref="A1:G44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D29" sqref="D29:D31"/>
+    <sheetView topLeftCell="A31" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D32" sqref="D32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
@@ -1980,13 +2069,13 @@
       </c>
     </row>
     <row r="3" spans="1:7" ht="43.2" hidden="1" customHeight="1">
-      <c r="A3" s="29" t="s">
+      <c r="A3" s="28" t="s">
         <v>27</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>152</v>
       </c>
-      <c r="C3" s="10" t="s">
+      <c r="C3" s="9" t="s">
         <v>24</v>
       </c>
       <c r="D3" s="1" t="s">
@@ -2003,11 +2092,11 @@
       </c>
     </row>
     <row r="4" spans="1:7" ht="39" hidden="1" customHeight="1">
-      <c r="A4" s="30"/>
+      <c r="A4" s="29"/>
       <c r="B4" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="10" t="s">
+      <c r="C4" s="9" t="s">
         <v>24</v>
       </c>
       <c r="D4" s="1" t="s">
@@ -2024,11 +2113,11 @@
       </c>
     </row>
     <row r="5" spans="1:7" ht="45.6" hidden="1" customHeight="1">
-      <c r="A5" s="30"/>
+      <c r="A5" s="29"/>
       <c r="B5" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C5" s="10" t="s">
+      <c r="C5" s="9" t="s">
         <v>24</v>
       </c>
       <c r="D5" s="1" t="s">
@@ -2045,11 +2134,11 @@
       </c>
     </row>
     <row r="6" spans="1:7" ht="36" hidden="1" customHeight="1">
-      <c r="A6" s="30"/>
+      <c r="A6" s="29"/>
       <c r="B6" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="C6" s="10" t="s">
+      <c r="C6" s="9" t="s">
         <v>24</v>
       </c>
       <c r="D6" s="1" t="s">
@@ -2066,11 +2155,11 @@
       </c>
     </row>
     <row r="7" spans="1:7" ht="39" hidden="1" customHeight="1">
-      <c r="A7" s="31"/>
+      <c r="A7" s="30"/>
       <c r="B7" s="2" t="s">
         <v>153</v>
       </c>
-      <c r="C7" s="10" t="s">
+      <c r="C7" s="9" t="s">
         <v>24</v>
       </c>
       <c r="D7" s="1" t="s">
@@ -2087,13 +2176,13 @@
       </c>
     </row>
     <row r="8" spans="1:7" ht="37.799999999999997" hidden="1" customHeight="1">
-      <c r="A8" s="29" t="s">
+      <c r="A8" s="28" t="s">
         <v>7</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="C8" s="10" t="s">
+      <c r="C8" s="9" t="s">
         <v>24</v>
       </c>
       <c r="D8" s="1" t="s">
@@ -2110,11 +2199,11 @@
       </c>
     </row>
     <row r="9" spans="1:7" ht="43.2" hidden="1" customHeight="1">
-      <c r="A9" s="30"/>
+      <c r="A9" s="29"/>
       <c r="B9" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="C9" s="10" t="s">
+      <c r="C9" s="9" t="s">
         <v>24</v>
       </c>
       <c r="D9" s="1" t="s">
@@ -2131,11 +2220,11 @@
       </c>
     </row>
     <row r="10" spans="1:7" ht="39.6" hidden="1" customHeight="1">
-      <c r="A10" s="30"/>
+      <c r="A10" s="29"/>
       <c r="B10" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="C10" s="10" t="s">
+      <c r="C10" s="9" t="s">
         <v>24</v>
       </c>
       <c r="D10" s="1" t="s">
@@ -2152,11 +2241,11 @@
       </c>
     </row>
     <row r="11" spans="1:7" ht="40.200000000000003" hidden="1" customHeight="1">
-      <c r="A11" s="30"/>
+      <c r="A11" s="29"/>
       <c r="B11" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="C11" s="10" t="s">
+      <c r="C11" s="9" t="s">
         <v>24</v>
       </c>
       <c r="D11" s="1" t="s">
@@ -2173,11 +2262,11 @@
       </c>
     </row>
     <row r="12" spans="1:7" ht="50.4" hidden="1" customHeight="1">
-      <c r="A12" s="31"/>
+      <c r="A12" s="30"/>
       <c r="B12" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="C12" s="10" t="s">
+      <c r="C12" s="9" t="s">
         <v>24</v>
       </c>
       <c r="D12" s="1" t="s">
@@ -2194,13 +2283,13 @@
       </c>
     </row>
     <row r="13" spans="1:7" ht="48.6" hidden="1" customHeight="1">
-      <c r="A13" s="29" t="s">
+      <c r="A13" s="28" t="s">
         <v>9</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>154</v>
       </c>
-      <c r="C13" s="10" t="s">
+      <c r="C13" s="9" t="s">
         <v>24</v>
       </c>
       <c r="D13" s="1" t="s">
@@ -2217,11 +2306,11 @@
       </c>
     </row>
     <row r="14" spans="1:7" ht="54.6" hidden="1" customHeight="1">
-      <c r="A14" s="30"/>
+      <c r="A14" s="29"/>
       <c r="B14" s="2" t="s">
         <v>155</v>
       </c>
-      <c r="C14" s="10" t="s">
+      <c r="C14" s="9" t="s">
         <v>24</v>
       </c>
       <c r="D14" s="1" t="s">
@@ -2238,11 +2327,11 @@
       </c>
     </row>
     <row r="15" spans="1:7" ht="45.6" hidden="1" customHeight="1">
-      <c r="A15" s="31"/>
+      <c r="A15" s="30"/>
       <c r="B15" s="2" t="s">
         <v>156</v>
       </c>
-      <c r="C15" s="10" t="s">
+      <c r="C15" s="9" t="s">
         <v>24</v>
       </c>
       <c r="D15" s="1" t="s">
@@ -2259,13 +2348,13 @@
       </c>
     </row>
     <row r="16" spans="1:7" ht="51.6" hidden="1" customHeight="1">
-      <c r="A16" s="29" t="s">
+      <c r="A16" s="28" t="s">
         <v>160</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>158</v>
       </c>
-      <c r="C16" s="10" t="s">
+      <c r="C16" s="9" t="s">
         <v>24</v>
       </c>
       <c r="D16" s="1" t="s">
@@ -2282,11 +2371,11 @@
       </c>
     </row>
     <row r="17" spans="1:7" ht="58.8" hidden="1" customHeight="1">
-      <c r="A17" s="30"/>
+      <c r="A17" s="29"/>
       <c r="B17" s="2" t="s">
         <v>159</v>
       </c>
-      <c r="C17" s="10" t="s">
+      <c r="C17" s="9" t="s">
         <v>24</v>
       </c>
       <c r="D17" s="1" t="s">
@@ -2303,11 +2392,11 @@
       </c>
     </row>
     <row r="18" spans="1:7" ht="53.4" hidden="1" customHeight="1">
-      <c r="A18" s="31"/>
+      <c r="A18" s="30"/>
       <c r="B18" s="2" t="s">
         <v>157</v>
       </c>
-      <c r="C18" s="10" t="s">
+      <c r="C18" s="9" t="s">
         <v>24</v>
       </c>
       <c r="D18" s="1" t="s">
@@ -2324,13 +2413,13 @@
       </c>
     </row>
     <row r="19" spans="1:7" ht="43.2" hidden="1" customHeight="1">
-      <c r="A19" s="32" t="s">
+      <c r="A19" s="31" t="s">
         <v>210</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>204</v>
       </c>
-      <c r="C19" s="10" t="s">
+      <c r="C19" s="9" t="s">
         <v>24</v>
       </c>
       <c r="D19" s="1" t="s">
@@ -2347,11 +2436,11 @@
       </c>
     </row>
     <row r="20" spans="1:7" ht="43.2" hidden="1">
-      <c r="A20" s="32"/>
+      <c r="A20" s="31"/>
       <c r="B20" s="2" t="s">
         <v>205</v>
       </c>
-      <c r="C20" s="10" t="s">
+      <c r="C20" s="9" t="s">
         <v>24</v>
       </c>
       <c r="D20" s="1" t="s">
@@ -2368,11 +2457,11 @@
       </c>
     </row>
     <row r="21" spans="1:7" ht="31.2" hidden="1" customHeight="1">
-      <c r="A21" s="32"/>
+      <c r="A21" s="31"/>
       <c r="B21" s="2" t="s">
         <v>206</v>
       </c>
-      <c r="C21" s="10" t="s">
+      <c r="C21" s="9" t="s">
         <v>24</v>
       </c>
       <c r="D21" s="1" t="s">
@@ -2389,11 +2478,11 @@
       </c>
     </row>
     <row r="22" spans="1:7" ht="34.200000000000003" hidden="1" customHeight="1">
-      <c r="A22" s="32"/>
+      <c r="A22" s="31"/>
       <c r="B22" s="2" t="s">
         <v>211</v>
       </c>
-      <c r="C22" s="10" t="s">
+      <c r="C22" s="9" t="s">
         <v>24</v>
       </c>
       <c r="D22" s="1" t="s">
@@ -2409,14 +2498,14 @@
         <v>217</v>
       </c>
     </row>
-    <row r="23" spans="1:7" ht="43.2">
-      <c r="A23" s="29" t="s">
+    <row r="23" spans="1:7" ht="43.2" hidden="1">
+      <c r="A23" s="28" t="s">
         <v>20</v>
       </c>
       <c r="B23" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="C23" s="10" t="s">
+      <c r="C23" s="9" t="s">
         <v>24</v>
       </c>
       <c r="D23" s="1" t="s">
@@ -2432,12 +2521,12 @@
         <v>216</v>
       </c>
     </row>
-    <row r="24" spans="1:7" ht="28.8">
-      <c r="A24" s="30"/>
+    <row r="24" spans="1:7" ht="28.8" hidden="1">
+      <c r="A24" s="29"/>
       <c r="B24" s="2" t="s">
         <v>213</v>
       </c>
-      <c r="C24" s="10" t="s">
+      <c r="C24" s="9" t="s">
         <v>24</v>
       </c>
       <c r="D24" s="1" t="s">
@@ -2453,12 +2542,12 @@
         <v>215</v>
       </c>
     </row>
-    <row r="25" spans="1:7" ht="43.2">
-      <c r="A25" s="31"/>
+    <row r="25" spans="1:7" ht="43.2" hidden="1">
+      <c r="A25" s="30"/>
       <c r="B25" s="2" t="s">
         <v>214</v>
       </c>
-      <c r="C25" s="10" t="s">
+      <c r="C25" s="9" t="s">
         <v>24</v>
       </c>
       <c r="D25" s="1" t="s">
@@ -2471,17 +2560,17 @@
         <v>1</v>
       </c>
       <c r="G25" s="2" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" ht="45" customHeight="1">
-      <c r="A26" s="29" t="s">
-        <v>269</v>
+        <v>273</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" ht="45" hidden="1" customHeight="1">
+      <c r="A26" s="28" t="s">
+        <v>267</v>
       </c>
       <c r="B26" s="2" t="s">
         <v>262</v>
       </c>
-      <c r="C26" s="10" t="s">
+      <c r="C26" s="9" t="s">
         <v>24</v>
       </c>
       <c r="D26" s="1" t="s">
@@ -2494,19 +2583,19 @@
         <v>2</v>
       </c>
       <c r="G26" s="2" t="s">
-        <v>286</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" ht="41.4" customHeight="1">
-      <c r="A27" s="30"/>
+        <v>281</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" ht="41.4" hidden="1" customHeight="1">
+      <c r="A27" s="29"/>
       <c r="B27" s="2" t="s">
         <v>263</v>
       </c>
-      <c r="C27" s="10" t="s">
+      <c r="C27" s="9" t="s">
         <v>24</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>279</v>
+        <v>274</v>
       </c>
       <c r="E27" s="2">
         <v>4</v>
@@ -2515,19 +2604,19 @@
         <v>2</v>
       </c>
       <c r="G27" s="2" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" ht="38.4" customHeight="1">
-      <c r="A28" s="31"/>
+        <v>280</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" ht="38.4" hidden="1" customHeight="1">
+      <c r="A28" s="30"/>
       <c r="B28" s="2" t="s">
         <v>264</v>
       </c>
-      <c r="C28" s="10" t="s">
+      <c r="C28" s="9" t="s">
         <v>24</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>280</v>
+        <v>275</v>
       </c>
       <c r="E28" s="2">
         <v>4</v>
@@ -2536,21 +2625,21 @@
         <v>1</v>
       </c>
       <c r="G28" s="2" t="s">
-        <v>284</v>
+        <v>279</v>
       </c>
     </row>
     <row r="29" spans="1:7" ht="44.4" customHeight="1">
-      <c r="A29" s="29" t="s">
-        <v>270</v>
+      <c r="A29" s="28" t="s">
+        <v>268</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>268</v>
-      </c>
-      <c r="C29" s="10" t="s">
+        <v>266</v>
+      </c>
+      <c r="C29" s="9" t="s">
         <v>24</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>322</v>
+        <v>316</v>
       </c>
       <c r="E29" s="2">
         <v>4</v>
@@ -2559,19 +2648,19 @@
         <v>1</v>
       </c>
       <c r="G29" s="2" t="s">
-        <v>283</v>
+        <v>278</v>
       </c>
     </row>
     <row r="30" spans="1:7" ht="58.2" customHeight="1">
-      <c r="A30" s="30"/>
+      <c r="A30" s="29"/>
       <c r="B30" s="2" t="s">
-        <v>324</v>
-      </c>
-      <c r="C30" s="10" t="s">
+        <v>318</v>
+      </c>
+      <c r="C30" s="9" t="s">
         <v>24</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>323</v>
+        <v>317</v>
       </c>
       <c r="E30" s="2">
         <v>4</v>
@@ -2580,19 +2669,19 @@
         <v>1</v>
       </c>
       <c r="G30" s="2" t="s">
-        <v>282</v>
+        <v>277</v>
       </c>
     </row>
     <row r="31" spans="1:7" ht="57.6">
-      <c r="A31" s="31"/>
+      <c r="A31" s="30"/>
       <c r="B31" s="2" t="s">
-        <v>267</v>
-      </c>
-      <c r="C31" s="10" t="s">
+        <v>338</v>
+      </c>
+      <c r="C31" s="9" t="s">
         <v>24</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="E31" s="2">
         <v>4</v>
@@ -2601,19 +2690,21 @@
         <v>2</v>
       </c>
       <c r="G31" s="2" t="s">
-        <v>281</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" ht="28.8">
-      <c r="A32" s="29" t="s">
-        <v>271</v>
-      </c>
-      <c r="B32" s="2"/>
-      <c r="C32" s="11" t="s">
-        <v>5</v>
+        <v>276</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" ht="43.2">
+      <c r="A32" s="28" t="s">
+        <v>269</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>348</v>
+      </c>
+      <c r="C32" s="9" t="s">
+        <v>24</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>35</v>
+        <v>353</v>
       </c>
       <c r="E32" s="2">
         <v>4</v>
@@ -2621,16 +2712,20 @@
       <c r="F32" s="2">
         <v>2</v>
       </c>
-      <c r="G32" s="2"/>
-    </row>
-    <row r="33" spans="1:7" ht="43.2">
-      <c r="A33" s="30"/>
-      <c r="B33" s="2"/>
-      <c r="C33" s="11" t="s">
-        <v>5</v>
+      <c r="G32" s="2" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" ht="48" customHeight="1">
+      <c r="A33" s="29"/>
+      <c r="B33" s="2" t="s">
+        <v>331</v>
+      </c>
+      <c r="C33" s="9" t="s">
+        <v>24</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="E33" s="2">
         <v>4</v>
@@ -2638,16 +2733,20 @@
       <c r="F33" s="2">
         <v>1</v>
       </c>
-      <c r="G33" s="2"/>
-    </row>
-    <row r="34" spans="1:7" ht="28.8">
-      <c r="A34" s="31"/>
-      <c r="B34" s="2"/>
-      <c r="C34" s="11" t="s">
-        <v>5</v>
+      <c r="G33" s="2" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" ht="45" customHeight="1">
+      <c r="A34" s="29"/>
+      <c r="B34" s="2" t="s">
+        <v>332</v>
+      </c>
+      <c r="C34" s="9" t="s">
+        <v>24</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>274</v>
+        <v>342</v>
       </c>
       <c r="E34" s="2">
         <v>4</v>
@@ -2655,71 +2754,77 @@
       <c r="F34" s="2">
         <v>2</v>
       </c>
-      <c r="G34" s="2"/>
-    </row>
-    <row r="35" spans="1:7">
-      <c r="A35" s="29" t="s">
-        <v>275</v>
-      </c>
-      <c r="B35" s="2"/>
-      <c r="C35" s="11" t="s">
-        <v>5</v>
+      <c r="G34" s="2" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" ht="45" customHeight="1">
+      <c r="A35" s="30"/>
+      <c r="B35" s="2" t="s">
+        <v>333</v>
+      </c>
+      <c r="C35" s="9" t="s">
+        <v>24</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>266</v>
+        <v>354</v>
       </c>
       <c r="E35" s="2">
         <v>4</v>
       </c>
       <c r="F35" s="2">
-        <v>2</v>
-      </c>
-      <c r="G35" s="2"/>
-    </row>
-    <row r="36" spans="1:7">
-      <c r="A36" s="31"/>
-      <c r="B36" s="2"/>
-      <c r="C36" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="G35" s="2" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" ht="36.6" customHeight="1">
+      <c r="A36" s="28" t="s">
+        <v>272</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>334</v>
+      </c>
+      <c r="C36" s="10" t="s">
         <v>5</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>287</v>
+        <v>345</v>
       </c>
       <c r="E36" s="2">
         <v>4</v>
       </c>
       <c r="F36" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G36" s="2"/>
     </row>
-    <row r="37" spans="1:7" ht="43.2">
-      <c r="A37" s="28" t="s">
-        <v>276</v>
-      </c>
-      <c r="B37" s="2"/>
-      <c r="C37" s="11" t="s">
+    <row r="37" spans="1:7" ht="42" customHeight="1">
+      <c r="A37" s="29"/>
+      <c r="B37" s="2" t="s">
+        <v>335</v>
+      </c>
+      <c r="C37" s="10" t="s">
         <v>5</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E37" s="2">
-        <v>4</v>
-      </c>
-      <c r="F37" s="2">
-        <v>2</v>
-      </c>
+        <v>343</v>
+      </c>
+      <c r="E37" s="2"/>
+      <c r="F37" s="2"/>
       <c r="G37" s="2"/>
     </row>
-    <row r="38" spans="1:7" ht="43.2">
-      <c r="A38" s="27"/>
-      <c r="B38" s="2"/>
-      <c r="C38" s="11" t="s">
+    <row r="38" spans="1:7" ht="57.6">
+      <c r="A38" s="30"/>
+      <c r="B38" s="2" t="s">
+        <v>336</v>
+      </c>
+      <c r="C38" s="10" t="s">
         <v>5</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>15</v>
+        <v>344</v>
       </c>
       <c r="E38" s="2">
         <v>4</v>
@@ -2729,14 +2834,18 @@
       </c>
       <c r="G38" s="2"/>
     </row>
-    <row r="39" spans="1:7" ht="28.8">
-      <c r="A39" s="27"/>
-      <c r="B39" s="2"/>
-      <c r="C39" s="11" t="s">
+    <row r="39" spans="1:7" ht="43.2">
+      <c r="A39" s="28" t="s">
+        <v>346</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>350</v>
+      </c>
+      <c r="C39" s="10" t="s">
         <v>5</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E39" s="2">
         <v>4</v>
@@ -2746,16 +2855,16 @@
       </c>
       <c r="G39" s="2"/>
     </row>
-    <row r="40" spans="1:7" ht="28.8">
-      <c r="A40" s="9" t="s">
-        <v>277</v>
-      </c>
-      <c r="B40" s="2"/>
-      <c r="C40" s="11" t="s">
+    <row r="40" spans="1:7" ht="43.2">
+      <c r="A40" s="29"/>
+      <c r="B40" s="2" t="s">
+        <v>351</v>
+      </c>
+      <c r="C40" s="10" t="s">
         <v>5</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="E40" s="2">
         <v>4</v>
@@ -2765,31 +2874,35 @@
       </c>
       <c r="G40" s="2"/>
     </row>
-    <row r="41" spans="1:7" ht="43.2">
-      <c r="A41" s="9"/>
-      <c r="B41" s="2"/>
-      <c r="C41" s="11" t="s">
+    <row r="41" spans="1:7" ht="28.8">
+      <c r="A41" s="30"/>
+      <c r="B41" s="2" t="s">
+        <v>352</v>
+      </c>
+      <c r="C41" s="10" t="s">
         <v>5</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E41" s="2">
         <v>4</v>
       </c>
       <c r="F41" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G41" s="2"/>
     </row>
     <row r="42" spans="1:7" ht="28.8">
-      <c r="A42" s="9"/>
+      <c r="A42" s="28" t="s">
+        <v>347</v>
+      </c>
       <c r="B42" s="2"/>
-      <c r="C42" s="11" t="s">
+      <c r="C42" s="10" t="s">
         <v>5</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="E42" s="2">
         <v>4</v>
@@ -2799,18 +2912,54 @@
       </c>
       <c r="G42" s="2"/>
     </row>
+    <row r="43" spans="1:7" ht="43.2">
+      <c r="A43" s="29"/>
+      <c r="B43" s="2"/>
+      <c r="C43" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="D43" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E43" s="2">
+        <v>4</v>
+      </c>
+      <c r="F43" s="2">
+        <v>1</v>
+      </c>
+      <c r="G43" s="2"/>
+    </row>
+    <row r="44" spans="1:7" ht="28.8">
+      <c r="A44" s="30"/>
+      <c r="B44" s="2"/>
+      <c r="C44" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="D44" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E44" s="2">
+        <v>4</v>
+      </c>
+      <c r="F44" s="2">
+        <v>1</v>
+      </c>
+      <c r="G44" s="2"/>
+    </row>
   </sheetData>
-  <mergeCells count="10">
+  <mergeCells count="12">
+    <mergeCell ref="A39:A41"/>
+    <mergeCell ref="A42:A44"/>
+    <mergeCell ref="A32:A35"/>
+    <mergeCell ref="A29:A31"/>
+    <mergeCell ref="A36:A38"/>
+    <mergeCell ref="A26:A28"/>
+    <mergeCell ref="A23:A25"/>
     <mergeCell ref="A16:A18"/>
     <mergeCell ref="A3:A7"/>
     <mergeCell ref="A8:A12"/>
     <mergeCell ref="A13:A15"/>
     <mergeCell ref="A19:A22"/>
-    <mergeCell ref="A29:A31"/>
-    <mergeCell ref="A32:A34"/>
-    <mergeCell ref="A35:A36"/>
-    <mergeCell ref="A26:A28"/>
-    <mergeCell ref="A23:A25"/>
   </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2821,8 +2970,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68EE2C79-A7B0-4BE1-9026-6C6F59ABCFC9}">
   <dimension ref="A1:D62"/>
   <sheetViews>
-    <sheetView topLeftCell="A35" workbookViewId="0">
-      <selection activeCell="C56" sqref="C56"/>
+    <sheetView topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="B60" sqref="B60:B62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
@@ -2834,663 +2983,724 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="30.6" customHeight="1">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="20" t="s">
+      <c r="B1" s="19" t="s">
         <v>54</v>
       </c>
-      <c r="C1" s="20" t="s">
+      <c r="C1" s="19" t="s">
         <v>55</v>
       </c>
-      <c r="D1" s="20" t="s">
+      <c r="D1" s="19" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="72" hidden="1">
-      <c r="A2" s="21" t="s">
+      <c r="A2" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="23" t="s">
+      <c r="B2" s="22" t="s">
         <v>35</v>
       </c>
-      <c r="C2" s="26" t="s">
+      <c r="C2" s="25" t="s">
         <v>169</v>
       </c>
-      <c r="D2" s="26" t="s">
+      <c r="D2" s="25" t="s">
         <v>170</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="43.2" hidden="1">
-      <c r="A3" s="21" t="s">
+      <c r="A3" s="20" t="s">
         <v>21</v>
       </c>
-      <c r="B3" s="23" t="s">
+      <c r="B3" s="22" t="s">
         <v>171</v>
       </c>
-      <c r="C3" s="26" t="s">
+      <c r="C3" s="25" t="s">
         <v>172</v>
       </c>
-      <c r="D3" s="26" t="s">
+      <c r="D3" s="25" t="s">
         <v>173</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="57.6" hidden="1">
-      <c r="A4" s="21" t="s">
+      <c r="A4" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="B4" s="23" t="s">
+      <c r="B4" s="22" t="s">
         <v>39</v>
       </c>
-      <c r="C4" s="26" t="s">
+      <c r="C4" s="25" t="s">
         <v>174</v>
       </c>
-      <c r="D4" s="26" t="s">
+      <c r="D4" s="25" t="s">
         <v>175</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="57.6" hidden="1">
-      <c r="A5" s="21" t="s">
+      <c r="A5" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="B5" s="23" t="s">
+      <c r="B5" s="22" t="s">
         <v>176</v>
       </c>
-      <c r="C5" s="26" t="s">
+      <c r="C5" s="25" t="s">
         <v>177</v>
       </c>
-      <c r="D5" s="26" t="s">
+      <c r="D5" s="25" t="s">
         <v>178</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="57.6" hidden="1">
-      <c r="A6" s="21" t="s">
+      <c r="A6" s="20" t="s">
         <v>30</v>
       </c>
-      <c r="B6" s="23" t="s">
+      <c r="B6" s="22" t="s">
         <v>179</v>
       </c>
-      <c r="C6" s="26" t="s">
+      <c r="C6" s="25" t="s">
         <v>180</v>
       </c>
-      <c r="D6" s="26" t="s">
+      <c r="D6" s="25" t="s">
         <v>181</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="43.2" hidden="1">
-      <c r="A7" s="21" t="s">
+      <c r="A7" s="20" t="s">
         <v>32</v>
       </c>
-      <c r="B7" s="23" t="s">
+      <c r="B7" s="22" t="s">
         <v>182</v>
       </c>
-      <c r="C7" s="26" t="s">
+      <c r="C7" s="25" t="s">
         <v>183</v>
       </c>
-      <c r="D7" s="26" t="s">
+      <c r="D7" s="25" t="s">
         <v>184</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="43.2" hidden="1">
-      <c r="A8" s="21" t="s">
+      <c r="A8" s="20" t="s">
         <v>34</v>
       </c>
-      <c r="B8" s="23" t="s">
+      <c r="B8" s="22" t="s">
         <v>185</v>
       </c>
-      <c r="C8" s="26" t="s">
+      <c r="C8" s="25" t="s">
         <v>186</v>
       </c>
-      <c r="D8" s="26" t="s">
+      <c r="D8" s="25" t="s">
         <v>187</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="43.2" hidden="1">
-      <c r="A9" s="21" t="s">
+      <c r="A9" s="20" t="s">
         <v>154</v>
       </c>
-      <c r="B9" s="23" t="s">
+      <c r="B9" s="22" t="s">
         <v>188</v>
       </c>
-      <c r="C9" s="26" t="s">
+      <c r="C9" s="25" t="s">
         <v>189</v>
       </c>
-      <c r="D9" s="26" t="s">
+      <c r="D9" s="25" t="s">
         <v>190</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="57.6" hidden="1">
-      <c r="A10" s="21" t="s">
+      <c r="A10" s="20" t="s">
         <v>155</v>
       </c>
-      <c r="B10" s="23" t="s">
+      <c r="B10" s="22" t="s">
         <v>191</v>
       </c>
-      <c r="C10" s="26" t="s">
+      <c r="C10" s="25" t="s">
         <v>192</v>
       </c>
-      <c r="D10" s="26" t="s">
+      <c r="D10" s="25" t="s">
         <v>193</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="57.6" hidden="1">
-      <c r="A11" s="21" t="s">
+      <c r="A11" s="20" t="s">
         <v>156</v>
       </c>
-      <c r="B11" s="23" t="s">
+      <c r="B11" s="22" t="s">
         <v>142</v>
       </c>
-      <c r="C11" s="26" t="s">
+      <c r="C11" s="25" t="s">
         <v>194</v>
       </c>
-      <c r="D11" s="26" t="s">
+      <c r="D11" s="25" t="s">
         <v>195</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="57.6" hidden="1">
-      <c r="A12" s="21" t="s">
+      <c r="A12" s="20" t="s">
         <v>158</v>
       </c>
-      <c r="B12" s="23" t="s">
+      <c r="B12" s="22" t="s">
         <v>196</v>
       </c>
-      <c r="C12" s="26" t="s">
+      <c r="C12" s="25" t="s">
         <v>197</v>
       </c>
-      <c r="D12" s="26" t="s">
+      <c r="D12" s="25" t="s">
         <v>198</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="43.2" hidden="1">
-      <c r="A13" s="21" t="s">
+      <c r="A13" s="20" t="s">
         <v>159</v>
       </c>
-      <c r="B13" s="23" t="s">
+      <c r="B13" s="22" t="s">
         <v>148</v>
       </c>
-      <c r="C13" s="26" t="s">
+      <c r="C13" s="25" t="s">
         <v>199</v>
       </c>
-      <c r="D13" s="26" t="s">
+      <c r="D13" s="25" t="s">
         <v>200</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="43.2" hidden="1">
-      <c r="A14" s="21" t="s">
+      <c r="A14" s="20" t="s">
         <v>204</v>
       </c>
-      <c r="B14" s="23" t="s">
+      <c r="B14" s="22" t="s">
         <v>201</v>
       </c>
-      <c r="C14" s="26" t="s">
+      <c r="C14" s="25" t="s">
         <v>202</v>
       </c>
-      <c r="D14" s="26" t="s">
+      <c r="D14" s="25" t="s">
         <v>203</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="28.8" hidden="1">
-      <c r="A15" s="33" t="s">
+      <c r="A15" s="32" t="s">
         <v>205</v>
       </c>
       <c r="B15" s="34" t="s">
         <v>220</v>
       </c>
-      <c r="C15" s="26" t="s">
+      <c r="C15" s="25" t="s">
         <v>221</v>
       </c>
-      <c r="D15" s="26" t="s">
+      <c r="D15" s="25" t="s">
         <v>224</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="28.8" hidden="1">
-      <c r="A16" s="33"/>
+      <c r="A16" s="32"/>
       <c r="B16" s="35"/>
-      <c r="C16" s="26" t="s">
+      <c r="C16" s="25" t="s">
         <v>222</v>
       </c>
-      <c r="D16" s="26" t="s">
+      <c r="D16" s="25" t="s">
         <v>225</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="28.8" hidden="1">
-      <c r="A17" s="33"/>
+      <c r="A17" s="32"/>
       <c r="B17" s="36"/>
-      <c r="C17" s="26" t="s">
+      <c r="C17" s="25" t="s">
         <v>223</v>
       </c>
-      <c r="D17" s="26" t="s">
+      <c r="D17" s="25" t="s">
         <v>226</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="43.2" hidden="1">
-      <c r="A18" s="33" t="s">
+      <c r="A18" s="32" t="s">
         <v>206</v>
       </c>
       <c r="B18" s="34" t="s">
         <v>227</v>
       </c>
-      <c r="C18" s="26" t="s">
+      <c r="C18" s="25" t="s">
         <v>228</v>
       </c>
-      <c r="D18" s="26" t="s">
+      <c r="D18" s="25" t="s">
         <v>231</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="28.8" hidden="1">
-      <c r="A19" s="33"/>
+      <c r="A19" s="32"/>
       <c r="B19" s="35"/>
-      <c r="C19" s="26" t="s">
+      <c r="C19" s="25" t="s">
         <v>229</v>
       </c>
-      <c r="D19" s="26" t="s">
+      <c r="D19" s="25" t="s">
         <v>232</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="28.8" hidden="1">
-      <c r="A20" s="33"/>
+      <c r="A20" s="32"/>
       <c r="B20" s="36"/>
-      <c r="C20" s="26" t="s">
+      <c r="C20" s="25" t="s">
         <v>230</v>
       </c>
-      <c r="D20" s="26" t="s">
+      <c r="D20" s="25" t="s">
         <v>233</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="28.8" hidden="1">
-      <c r="A21" s="33" t="s">
+      <c r="A21" s="32" t="s">
         <v>211</v>
       </c>
       <c r="B21" s="34" t="s">
         <v>240</v>
       </c>
-      <c r="C21" s="22" t="s">
+      <c r="C21" s="21" t="s">
         <v>234</v>
       </c>
-      <c r="D21" s="22" t="s">
+      <c r="D21" s="21" t="s">
         <v>237</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="28.8" hidden="1">
-      <c r="A22" s="33"/>
+      <c r="A22" s="32"/>
       <c r="B22" s="35"/>
-      <c r="C22" s="22" t="s">
+      <c r="C22" s="21" t="s">
         <v>235</v>
       </c>
-      <c r="D22" s="22" t="s">
+      <c r="D22" s="21" t="s">
         <v>238</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="28.8" hidden="1">
-      <c r="A23" s="33"/>
+      <c r="A23" s="32"/>
       <c r="B23" s="36"/>
-      <c r="C23" s="22" t="s">
+      <c r="C23" s="21" t="s">
         <v>236</v>
       </c>
-      <c r="D23" s="22" t="s">
+      <c r="D23" s="21" t="s">
         <v>239</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="28.8">
-      <c r="A24" s="33" t="s">
+      <c r="A24" s="32" t="s">
         <v>213</v>
       </c>
       <c r="B24" s="34" t="s">
         <v>241</v>
       </c>
-      <c r="C24" s="25" t="s">
+      <c r="C24" s="24" t="s">
         <v>242</v>
       </c>
-      <c r="D24" s="25" t="s">
+      <c r="D24" s="24" t="s">
         <v>245</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="28.8">
-      <c r="A25" s="33"/>
+      <c r="A25" s="32"/>
       <c r="B25" s="35"/>
-      <c r="C25" s="25" t="s">
+      <c r="C25" s="24" t="s">
         <v>243</v>
       </c>
-      <c r="D25" s="25" t="s">
+      <c r="D25" s="24" t="s">
         <v>246</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="28.8">
-      <c r="A26" s="33"/>
+      <c r="A26" s="32"/>
       <c r="B26" s="36"/>
-      <c r="C26" s="25" t="s">
+      <c r="C26" s="24" t="s">
         <v>244</v>
       </c>
-      <c r="D26" s="25" t="s">
+      <c r="D26" s="24" t="s">
         <v>247</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="28.8">
-      <c r="A27" s="33" t="s">
+      <c r="A27" s="32" t="s">
         <v>214</v>
       </c>
       <c r="B27" s="34" t="s">
         <v>248</v>
       </c>
-      <c r="C27" s="25" t="s">
+      <c r="C27" s="24" t="s">
         <v>249</v>
       </c>
-      <c r="D27" s="25" t="s">
+      <c r="D27" s="24" t="s">
         <v>252</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="28.8">
-      <c r="A28" s="33"/>
+      <c r="A28" s="32"/>
       <c r="B28" s="35"/>
-      <c r="C28" s="25" t="s">
+      <c r="C28" s="24" t="s">
         <v>250</v>
       </c>
-      <c r="D28" s="25" t="s">
+      <c r="D28" s="24" t="s">
         <v>253</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="28.8">
-      <c r="A29" s="33"/>
+      <c r="A29" s="32"/>
       <c r="B29" s="36"/>
-      <c r="C29" s="25" t="s">
+      <c r="C29" s="24" t="s">
         <v>251</v>
       </c>
-      <c r="D29" s="25" t="s">
+      <c r="D29" s="24" t="s">
         <v>254</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="14.4" customHeight="1">
-      <c r="A30" s="33" t="s">
+      <c r="A30" s="32" t="s">
         <v>262</v>
       </c>
       <c r="B30" s="34" t="s">
         <v>265</v>
       </c>
-      <c r="C30" s="25" t="s">
+      <c r="C30" s="24" t="s">
+        <v>282</v>
+      </c>
+      <c r="D30" s="24" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" ht="33" customHeight="1">
+      <c r="A31" s="32"/>
+      <c r="B31" s="35"/>
+      <c r="C31" s="24" t="s">
+        <v>283</v>
+      </c>
+      <c r="D31" s="24" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" ht="24" customHeight="1">
+      <c r="A32" s="32"/>
+      <c r="B32" s="36"/>
+      <c r="C32" s="24" t="s">
+        <v>284</v>
+      </c>
+      <c r="D32" s="24" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" ht="36.6" customHeight="1">
+      <c r="A33" s="32" t="s">
+        <v>263</v>
+      </c>
+      <c r="B33" s="34" t="s">
         <v>288</v>
       </c>
-      <c r="D30" s="25" t="s">
+      <c r="C33" s="24" t="s">
+        <v>289</v>
+      </c>
+      <c r="D33" s="24" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" ht="26.4" customHeight="1">
+      <c r="A34" s="32"/>
+      <c r="B34" s="35"/>
+      <c r="C34" s="24" t="s">
+        <v>290</v>
+      </c>
+      <c r="D34" s="24" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" ht="24" customHeight="1">
+      <c r="A35" s="32"/>
+      <c r="B35" s="36"/>
+      <c r="C35" s="24" t="s">
         <v>291</v>
       </c>
-    </row>
-    <row r="31" spans="1:4" ht="33" customHeight="1">
-      <c r="A31" s="33"/>
-      <c r="B31" s="35"/>
-      <c r="C31" s="25" t="s">
-        <v>289</v>
-      </c>
-      <c r="D31" s="25" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" ht="24" customHeight="1">
-      <c r="A32" s="33"/>
-      <c r="B32" s="36"/>
-      <c r="C32" s="25" t="s">
-        <v>290</v>
-      </c>
-      <c r="D32" s="25" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" ht="36.6" customHeight="1">
-      <c r="A33" s="33" t="s">
-        <v>263</v>
-      </c>
-      <c r="B33" s="34" t="s">
+      <c r="D35" s="24" t="s">
         <v>294</v>
       </c>
-      <c r="C33" s="25" t="s">
+    </row>
+    <row r="36" spans="1:4" ht="36.6" customHeight="1">
+      <c r="A36" s="32" t="s">
+        <v>264</v>
+      </c>
+      <c r="B36" s="34" t="s">
         <v>295</v>
       </c>
-      <c r="D33" s="25" t="s">
+      <c r="C36" s="21" t="s">
+        <v>296</v>
+      </c>
+      <c r="D36" s="21" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" ht="34.200000000000003" customHeight="1">
+      <c r="A37" s="32"/>
+      <c r="B37" s="35"/>
+      <c r="C37" s="21" t="s">
+        <v>297</v>
+      </c>
+      <c r="D37" s="21" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" ht="30" customHeight="1">
+      <c r="A38" s="32"/>
+      <c r="B38" s="36"/>
+      <c r="C38" s="21" t="s">
         <v>298</v>
       </c>
-    </row>
-    <row r="34" spans="1:4" ht="26.4" customHeight="1">
-      <c r="A34" s="33"/>
-      <c r="B34" s="35"/>
-      <c r="C34" s="25" t="s">
-        <v>296</v>
-      </c>
-      <c r="D34" s="25" t="s">
-        <v>299</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" ht="24" customHeight="1">
-      <c r="A35" s="33"/>
-      <c r="B35" s="36"/>
-      <c r="C35" s="25" t="s">
-        <v>297</v>
-      </c>
-      <c r="D35" s="25" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" ht="36.6" customHeight="1">
-      <c r="A36" s="33" t="s">
-        <v>264</v>
-      </c>
-      <c r="B36" s="34" t="s">
+      <c r="D38" s="21" t="s">
         <v>301</v>
       </c>
-      <c r="C36" s="22" t="s">
-        <v>302</v>
-      </c>
-      <c r="D36" s="22" t="s">
-        <v>305</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" ht="34.200000000000003" customHeight="1">
-      <c r="A37" s="33"/>
-      <c r="B37" s="35"/>
-      <c r="C37" s="22" t="s">
-        <v>303</v>
-      </c>
-      <c r="D37" s="22" t="s">
-        <v>306</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" ht="30" customHeight="1">
-      <c r="A38" s="33"/>
-      <c r="B38" s="36"/>
-      <c r="C38" s="22" t="s">
-        <v>304</v>
-      </c>
-      <c r="D38" s="22" t="s">
-        <v>307</v>
-      </c>
     </row>
     <row r="39" spans="1:4" ht="61.2" customHeight="1">
-      <c r="A39" s="33" t="s">
-        <v>268</v>
-      </c>
-      <c r="B39" s="40" t="s">
+      <c r="A39" s="32" t="s">
+        <v>266</v>
+      </c>
+      <c r="B39" s="33" t="s">
+        <v>316</v>
+      </c>
+      <c r="C39" s="21" t="s">
+        <v>321</v>
+      </c>
+      <c r="D39" s="27" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" ht="23.4" customHeight="1">
+      <c r="A40" s="32"/>
+      <c r="B40" s="33"/>
+      <c r="C40" s="27" t="s">
+        <v>319</v>
+      </c>
+      <c r="D40" s="27" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" ht="25.2" customHeight="1">
+      <c r="A41" s="32"/>
+      <c r="B41" s="33"/>
+      <c r="C41" s="27" t="s">
         <v>322</v>
       </c>
-      <c r="C39" s="22" t="s">
+      <c r="D41" s="27" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" ht="43.2" customHeight="1">
+      <c r="A42" s="32" t="s">
+        <v>318</v>
+      </c>
+      <c r="B42" s="33" t="s">
+        <v>317</v>
+      </c>
+      <c r="C42" s="21" t="s">
+        <v>325</v>
+      </c>
+      <c r="D42" s="21" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" ht="28.8">
+      <c r="A43" s="32"/>
+      <c r="B43" s="33"/>
+      <c r="C43" s="21" t="s">
+        <v>326</v>
+      </c>
+      <c r="D43" s="21" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" ht="28.8">
+      <c r="A44" s="32"/>
+      <c r="B44" s="33"/>
+      <c r="C44" s="21" t="s">
         <v>327</v>
       </c>
-      <c r="D39" s="42" t="s">
-        <v>329</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" ht="23.4" customHeight="1">
-      <c r="A40" s="33"/>
-      <c r="B40" s="40"/>
-      <c r="C40" s="42" t="s">
-        <v>325</v>
-      </c>
-      <c r="D40" s="42" t="s">
-        <v>326</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" ht="25.2" customHeight="1">
-      <c r="A41" s="33"/>
-      <c r="B41" s="40"/>
-      <c r="C41" s="42" t="s">
-        <v>328</v>
-      </c>
-      <c r="D41" s="42" t="s">
+      <c r="D44" s="21" t="s">
         <v>330</v>
       </c>
     </row>
-    <row r="42" spans="1:4" ht="43.2" customHeight="1">
-      <c r="A42" s="33" t="s">
-        <v>324</v>
-      </c>
-      <c r="B42" s="40" t="s">
-        <v>323</v>
-      </c>
-      <c r="C42" s="22" t="s">
+    <row r="45" spans="1:4" ht="43.2" customHeight="1">
+      <c r="A45" s="32" t="s">
         <v>331</v>
       </c>
-      <c r="D42" s="22" t="s">
+      <c r="B45" s="33" t="s">
+        <v>271</v>
+      </c>
+      <c r="C45" s="24" t="s">
+        <v>355</v>
+      </c>
+      <c r="D45" s="24" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" ht="28.8" customHeight="1">
+      <c r="A46" s="32"/>
+      <c r="B46" s="33"/>
+      <c r="C46" s="40" t="s">
+        <v>356</v>
+      </c>
+      <c r="D46" s="24" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" ht="28.8">
+      <c r="A47" s="32"/>
+      <c r="B47" s="33"/>
+      <c r="C47" s="40"/>
+      <c r="D47" s="24" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" ht="30.6" customHeight="1">
+      <c r="A48" s="32" t="s">
+        <v>332</v>
+      </c>
+      <c r="B48" s="33" t="s">
+        <v>342</v>
+      </c>
+      <c r="C48" s="24" t="s">
+        <v>360</v>
+      </c>
+      <c r="D48" s="24" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" ht="33.6" customHeight="1">
+      <c r="A49" s="32"/>
+      <c r="B49" s="33"/>
+      <c r="C49" s="40" t="s">
+        <v>361</v>
+      </c>
+      <c r="D49" s="24" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" ht="43.2">
+      <c r="A50" s="32"/>
+      <c r="B50" s="33"/>
+      <c r="C50" s="40"/>
+      <c r="D50" s="24" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" ht="43.2">
+      <c r="A51" s="32" t="s">
+        <v>333</v>
+      </c>
+      <c r="B51" s="33" t="s">
+        <v>354</v>
+      </c>
+      <c r="C51" s="41" t="s">
+        <v>365</v>
+      </c>
+      <c r="D51" s="24" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" ht="28.8">
+      <c r="A52" s="32"/>
+      <c r="B52" s="33"/>
+      <c r="C52" s="42"/>
+      <c r="D52" s="24" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" ht="43.2">
+      <c r="A53" s="32"/>
+      <c r="B53" s="33"/>
+      <c r="C53" s="43"/>
+      <c r="D53" s="24" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4">
+      <c r="A54" s="32" t="s">
         <v>334</v>
       </c>
-    </row>
-    <row r="43" spans="1:4" ht="28.8">
-      <c r="A43" s="33"/>
-      <c r="B43" s="40"/>
-      <c r="C43" s="22" t="s">
-        <v>332</v>
-      </c>
-      <c r="D43" s="22" t="s">
+      <c r="B54" s="34" t="s">
+        <v>345</v>
+      </c>
+      <c r="C54" s="26"/>
+      <c r="D54" s="26"/>
+    </row>
+    <row r="55" spans="1:4">
+      <c r="A55" s="32"/>
+      <c r="B55" s="35"/>
+      <c r="C55" s="26"/>
+      <c r="D55" s="26"/>
+    </row>
+    <row r="56" spans="1:4">
+      <c r="A56" s="32"/>
+      <c r="B56" s="36"/>
+      <c r="C56" s="26"/>
+      <c r="D56" s="26"/>
+    </row>
+    <row r="57" spans="1:4">
+      <c r="A57" s="32" t="s">
         <v>335</v>
       </c>
-    </row>
-    <row r="44" spans="1:4" ht="28.8">
-      <c r="A44" s="33"/>
-      <c r="B44" s="40"/>
-      <c r="C44" s="22" t="s">
-        <v>333</v>
-      </c>
-      <c r="D44" s="22" t="s">
+      <c r="B57" s="34" t="s">
+        <v>343</v>
+      </c>
+      <c r="C57" s="26"/>
+      <c r="D57" s="26"/>
+    </row>
+    <row r="58" spans="1:4">
+      <c r="A58" s="32"/>
+      <c r="B58" s="35"/>
+      <c r="C58" s="26"/>
+      <c r="D58" s="26"/>
+    </row>
+    <row r="59" spans="1:4">
+      <c r="A59" s="32"/>
+      <c r="B59" s="36"/>
+      <c r="C59" s="26"/>
+      <c r="D59" s="26"/>
+    </row>
+    <row r="60" spans="1:4">
+      <c r="A60" s="32" t="s">
         <v>336</v>
       </c>
-    </row>
-    <row r="45" spans="1:4">
-      <c r="A45" s="33" t="s">
-        <v>337</v>
-      </c>
-      <c r="B45" s="40"/>
-      <c r="C45" s="41"/>
-      <c r="D45" s="41"/>
-    </row>
-    <row r="46" spans="1:4">
-      <c r="A46" s="33"/>
-      <c r="B46" s="40"/>
-      <c r="C46" s="41"/>
-      <c r="D46" s="41"/>
-    </row>
-    <row r="47" spans="1:4">
-      <c r="A47" s="33"/>
-      <c r="B47" s="40"/>
-      <c r="C47" s="41"/>
-      <c r="D47" s="41"/>
-    </row>
-    <row r="48" spans="1:4">
-      <c r="A48" s="33" t="s">
-        <v>338</v>
-      </c>
-      <c r="B48" s="40"/>
-      <c r="C48" s="41"/>
-      <c r="D48" s="41"/>
-    </row>
-    <row r="49" spans="1:4">
-      <c r="A49" s="33"/>
-      <c r="B49" s="40"/>
-      <c r="C49" s="41"/>
-      <c r="D49" s="41"/>
-    </row>
-    <row r="50" spans="1:4">
-      <c r="A50" s="33"/>
-      <c r="B50" s="40"/>
-      <c r="C50" s="41"/>
-      <c r="D50" s="41"/>
-    </row>
-    <row r="51" spans="1:4">
-      <c r="A51" s="33" t="s">
-        <v>339</v>
-      </c>
-      <c r="B51" s="40"/>
-      <c r="C51" s="41"/>
-      <c r="D51" s="41"/>
-    </row>
-    <row r="52" spans="1:4">
-      <c r="A52" s="33"/>
-      <c r="B52" s="40"/>
-      <c r="C52" s="41"/>
-      <c r="D52" s="41"/>
-    </row>
-    <row r="53" spans="1:4">
-      <c r="A53" s="33"/>
-      <c r="B53" s="40"/>
-      <c r="C53" s="41"/>
-      <c r="D53" s="41"/>
-    </row>
-    <row r="54" spans="1:4">
-      <c r="A54" s="33" t="s">
-        <v>340</v>
-      </c>
-      <c r="B54" s="40"/>
-      <c r="C54" s="41"/>
-      <c r="D54" s="41"/>
-    </row>
-    <row r="55" spans="1:4">
-      <c r="A55" s="33"/>
-      <c r="B55" s="40"/>
-      <c r="C55" s="41"/>
-      <c r="D55" s="41"/>
-    </row>
-    <row r="56" spans="1:4">
-      <c r="A56" s="33"/>
-      <c r="B56" s="40"/>
-      <c r="C56" s="41"/>
-      <c r="D56" s="41"/>
-    </row>
-    <row r="57" spans="1:4">
-      <c r="A57" s="33" t="s">
-        <v>341</v>
-      </c>
-      <c r="B57" s="40"/>
-      <c r="C57" s="41"/>
-      <c r="D57" s="41"/>
-    </row>
-    <row r="58" spans="1:4">
-      <c r="A58" s="33"/>
-      <c r="B58" s="40"/>
-      <c r="C58" s="41"/>
-      <c r="D58" s="41"/>
-    </row>
-    <row r="59" spans="1:4">
-      <c r="A59" s="33"/>
-      <c r="B59" s="40"/>
-      <c r="C59" s="41"/>
-      <c r="D59" s="41"/>
-    </row>
-    <row r="60" spans="1:4">
-      <c r="A60" s="33" t="s">
-        <v>342</v>
-      </c>
-      <c r="B60" s="40"/>
-      <c r="C60" s="41"/>
-      <c r="D60" s="41"/>
+      <c r="B60" s="34"/>
+      <c r="C60" s="26"/>
+      <c r="D60" s="26"/>
     </row>
     <row r="61" spans="1:4">
-      <c r="A61" s="33"/>
-      <c r="B61" s="40"/>
-      <c r="C61" s="41"/>
-      <c r="D61" s="41"/>
+      <c r="A61" s="32"/>
+      <c r="B61" s="35"/>
+      <c r="C61" s="26"/>
+      <c r="D61" s="26"/>
     </row>
     <row r="62" spans="1:4">
-      <c r="A62" s="33"/>
-      <c r="B62" s="40"/>
-      <c r="C62" s="41"/>
-      <c r="D62" s="41"/>
+      <c r="A62" s="32"/>
+      <c r="B62" s="36"/>
+      <c r="C62" s="26"/>
+      <c r="D62" s="26"/>
     </row>
   </sheetData>
-  <mergeCells count="32">
+  <mergeCells count="35">
+    <mergeCell ref="C46:C47"/>
+    <mergeCell ref="C49:C50"/>
+    <mergeCell ref="C51:C53"/>
+    <mergeCell ref="A27:A29"/>
+    <mergeCell ref="B21:B23"/>
+    <mergeCell ref="B24:B26"/>
+    <mergeCell ref="B27:B29"/>
+    <mergeCell ref="B15:B17"/>
+    <mergeCell ref="A15:A17"/>
+    <mergeCell ref="B18:B20"/>
+    <mergeCell ref="A18:A20"/>
+    <mergeCell ref="A21:A23"/>
+    <mergeCell ref="A24:A26"/>
+    <mergeCell ref="B42:B44"/>
+    <mergeCell ref="A42:A44"/>
+    <mergeCell ref="A39:A41"/>
+    <mergeCell ref="B39:B41"/>
+    <mergeCell ref="A30:A32"/>
+    <mergeCell ref="B30:B32"/>
+    <mergeCell ref="A33:A35"/>
+    <mergeCell ref="B33:B35"/>
+    <mergeCell ref="A36:A38"/>
+    <mergeCell ref="B36:B38"/>
     <mergeCell ref="A60:A62"/>
     <mergeCell ref="B45:B47"/>
     <mergeCell ref="B48:B50"/>
@@ -3503,26 +3713,6 @@
     <mergeCell ref="A51:A53"/>
     <mergeCell ref="A54:A56"/>
     <mergeCell ref="A57:A59"/>
-    <mergeCell ref="B42:B44"/>
-    <mergeCell ref="A42:A44"/>
-    <mergeCell ref="A39:A41"/>
-    <mergeCell ref="B39:B41"/>
-    <mergeCell ref="A30:A32"/>
-    <mergeCell ref="B30:B32"/>
-    <mergeCell ref="A33:A35"/>
-    <mergeCell ref="B33:B35"/>
-    <mergeCell ref="A36:A38"/>
-    <mergeCell ref="B36:B38"/>
-    <mergeCell ref="A27:A29"/>
-    <mergeCell ref="B21:B23"/>
-    <mergeCell ref="B24:B26"/>
-    <mergeCell ref="B27:B29"/>
-    <mergeCell ref="B15:B17"/>
-    <mergeCell ref="A15:A17"/>
-    <mergeCell ref="B18:B20"/>
-    <mergeCell ref="A18:A20"/>
-    <mergeCell ref="A21:A23"/>
-    <mergeCell ref="A24:A26"/>
   </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3531,10 +3721,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{113AD7C8-E432-4900-8C71-627982E552B0}">
-  <dimension ref="A1:D13"/>
+  <dimension ref="A1:D16"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11:B13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
@@ -3545,165 +3735,201 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="32.4" customHeight="1">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="12" t="s">
+      <c r="B1" s="11" t="s">
         <v>54</v>
       </c>
-      <c r="C1" s="12" t="s">
+      <c r="C1" s="11" t="s">
         <v>55</v>
       </c>
-      <c r="D1" s="12" t="s">
+      <c r="D1" s="11" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="57.6">
-      <c r="A2" s="13" t="s">
+    <row r="2" spans="1:4" ht="57.6" hidden="1">
+      <c r="A2" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="B2" s="24" t="s">
+      <c r="B2" s="23" t="s">
         <v>28</v>
       </c>
-      <c r="C2" s="22" t="s">
+      <c r="C2" s="21" t="s">
         <v>161</v>
       </c>
-      <c r="D2" s="22" t="s">
+      <c r="D2" s="21" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="86.4">
-      <c r="A3" s="13" t="s">
+    <row r="3" spans="1:4" ht="86.4" hidden="1">
+      <c r="A3" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="B3" s="23" t="s">
+      <c r="B3" s="22" t="s">
         <v>163</v>
       </c>
-      <c r="C3" s="22" t="s">
+      <c r="C3" s="21" t="s">
         <v>164</v>
       </c>
-      <c r="D3" s="22" t="s">
+      <c r="D3" s="21" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="72">
-      <c r="A4" s="13" t="s">
+    <row r="4" spans="1:4" ht="72" hidden="1">
+      <c r="A4" s="12" t="s">
         <v>49</v>
       </c>
-      <c r="B4" s="23" t="s">
+      <c r="B4" s="22" t="s">
         <v>166</v>
       </c>
-      <c r="C4" s="22" t="s">
+      <c r="C4" s="21" t="s">
         <v>168</v>
       </c>
-      <c r="D4" s="22" t="s">
+      <c r="D4" s="21" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="28.8">
-      <c r="A5" s="33" t="s">
+    <row r="5" spans="1:4" ht="28.8" hidden="1">
+      <c r="A5" s="32" t="s">
         <v>50</v>
       </c>
       <c r="B5" s="34" t="s">
         <v>255</v>
       </c>
-      <c r="C5" s="25" t="s">
+      <c r="C5" s="24" t="s">
         <v>256</v>
       </c>
-      <c r="D5" s="25" t="s">
+      <c r="D5" s="24" t="s">
         <v>259</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="28.8">
-      <c r="A6" s="33"/>
+    <row r="6" spans="1:4" ht="28.8" hidden="1">
+      <c r="A6" s="32"/>
       <c r="B6" s="35"/>
-      <c r="C6" s="25" t="s">
+      <c r="C6" s="24" t="s">
         <v>257</v>
       </c>
-      <c r="D6" s="25" t="s">
+      <c r="D6" s="24" t="s">
         <v>260</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="43.2">
-      <c r="A7" s="33"/>
+    <row r="7" spans="1:4" ht="43.2" hidden="1">
+      <c r="A7" s="32"/>
       <c r="B7" s="36"/>
-      <c r="C7" s="25" t="s">
+      <c r="C7" s="24" t="s">
         <v>258</v>
       </c>
-      <c r="D7" s="25" t="s">
+      <c r="D7" s="24" t="s">
         <v>261</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="28.8" customHeight="1">
-      <c r="A8" s="33" t="s">
-        <v>343</v>
+      <c r="A8" s="32" t="s">
+        <v>337</v>
       </c>
       <c r="B8" s="34" t="s">
+        <v>302</v>
+      </c>
+      <c r="C8" s="24" t="s">
+        <v>303</v>
+      </c>
+      <c r="D8" s="24" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="28.8">
+      <c r="A9" s="32"/>
+      <c r="B9" s="35"/>
+      <c r="C9" s="24" t="s">
+        <v>304</v>
+      </c>
+      <c r="D9" s="24" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="28.8">
+      <c r="A10" s="32"/>
+      <c r="B10" s="36"/>
+      <c r="C10" s="24" t="s">
+        <v>305</v>
+      </c>
+      <c r="D10" s="24" t="s">
         <v>308</v>
       </c>
-      <c r="C8" s="25" t="s">
+    </row>
+    <row r="11" spans="1:4" ht="14.4" customHeight="1">
+      <c r="A11" s="32" t="s">
+        <v>338</v>
+      </c>
+      <c r="B11" s="34" t="s">
         <v>309</v>
       </c>
-      <c r="D8" s="25" t="s">
+      <c r="C11" s="24" t="s">
+        <v>310</v>
+      </c>
+      <c r="D11" s="24" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="37.200000000000003" customHeight="1">
+      <c r="A12" s="32"/>
+      <c r="B12" s="35"/>
+      <c r="C12" s="24" t="s">
+        <v>311</v>
+      </c>
+      <c r="D12" s="24" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="26.4" customHeight="1">
+      <c r="A13" s="32"/>
+      <c r="B13" s="36"/>
+      <c r="C13" s="24" t="s">
         <v>312</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" ht="28.8">
-      <c r="A9" s="33"/>
-      <c r="B9" s="35"/>
-      <c r="C9" s="25" t="s">
-        <v>310</v>
-      </c>
-      <c r="D9" s="25" t="s">
-        <v>313</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" ht="28.8">
-      <c r="A10" s="33"/>
-      <c r="B10" s="36"/>
-      <c r="C10" s="25" t="s">
-        <v>311</v>
-      </c>
-      <c r="D10" s="25" t="s">
-        <v>314</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" ht="14.4" customHeight="1">
-      <c r="A11" s="33" t="s">
-        <v>344</v>
-      </c>
-      <c r="B11" s="34" t="s">
+      <c r="D13" s="24" t="s">
         <v>315</v>
       </c>
-      <c r="C11" s="25" t="s">
-        <v>316</v>
-      </c>
-      <c r="D11" s="25" t="s">
-        <v>319</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" ht="28.8">
-      <c r="A12" s="33"/>
-      <c r="B12" s="35"/>
-      <c r="C12" s="25" t="s">
-        <v>317</v>
-      </c>
-      <c r="D12" s="25" t="s">
-        <v>320</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4">
-      <c r="A13" s="33"/>
-      <c r="B13" s="36"/>
-      <c r="C13" s="25" t="s">
-        <v>318</v>
-      </c>
-      <c r="D13" s="25" t="s">
-        <v>321</v>
+    </row>
+    <row r="14" spans="1:4" ht="43.2">
+      <c r="A14" s="32" t="s">
+        <v>348</v>
+      </c>
+      <c r="B14" s="34" t="s">
+        <v>353</v>
+      </c>
+      <c r="C14" s="24" t="s">
+        <v>369</v>
+      </c>
+      <c r="D14" s="24" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="43.2">
+      <c r="A15" s="32"/>
+      <c r="B15" s="35"/>
+      <c r="C15" s="24" t="s">
+        <v>371</v>
+      </c>
+      <c r="D15" s="24" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="43.2">
+      <c r="A16" s="32"/>
+      <c r="B16" s="36"/>
+      <c r="C16" s="24" t="s">
+        <v>373</v>
+      </c>
+      <c r="D16" s="24" t="s">
+        <v>374</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="6">
+  <mergeCells count="8">
+    <mergeCell ref="A14:A16"/>
+    <mergeCell ref="B14:B16"/>
     <mergeCell ref="A11:A13"/>
     <mergeCell ref="B11:B13"/>
     <mergeCell ref="A5:A7"/>
@@ -3727,474 +3953,474 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
   <sheetData>
     <row r="2" spans="2:2">
-      <c r="B2" s="14" t="s">
+      <c r="B2" s="13" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="4" spans="2:2" ht="18">
-      <c r="B4" s="15" t="s">
+      <c r="B4" s="14" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="5" spans="2:2">
-      <c r="B5" s="16"/>
+      <c r="B5" s="15"/>
     </row>
     <row r="6" spans="2:2">
-      <c r="B6" s="16" t="s">
+      <c r="B6" s="15" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="7" spans="2:2">
-      <c r="B7" s="16" t="s">
+      <c r="B7" s="15" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="8" spans="2:2">
-      <c r="B8" s="16" t="s">
+      <c r="B8" s="15" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="9" spans="2:2">
-      <c r="B9" s="16" t="s">
+      <c r="B9" s="15" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="11" spans="2:2">
-      <c r="B11" s="14" t="s">
+      <c r="B11" s="13" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="12" spans="2:2">
-      <c r="B12" s="16"/>
+      <c r="B12" s="15"/>
     </row>
     <row r="13" spans="2:2">
-      <c r="B13" s="16" t="s">
+      <c r="B13" s="15" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="14" spans="2:2">
-      <c r="B14" s="16" t="s">
+      <c r="B14" s="15" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="18" spans="2:2" ht="18">
-      <c r="B18" s="15" t="s">
+      <c r="B18" s="14" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="19" spans="2:2">
-      <c r="B19" s="16"/>
+      <c r="B19" s="15"/>
     </row>
     <row r="20" spans="2:2">
-      <c r="B20" s="16" t="s">
+      <c r="B20" s="15" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="21" spans="2:2">
-      <c r="B21" s="16" t="s">
+      <c r="B21" s="15" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="22" spans="2:2">
-      <c r="B22" s="16" t="s">
+      <c r="B22" s="15" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="24" spans="2:2">
-      <c r="B24" s="14" t="s">
+      <c r="B24" s="13" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="25" spans="2:2">
-      <c r="B25" s="16"/>
+      <c r="B25" s="15"/>
     </row>
     <row r="26" spans="2:2">
-      <c r="B26" s="16" t="s">
+      <c r="B26" s="15" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="27" spans="2:2">
-      <c r="B27" s="16" t="s">
+      <c r="B27" s="15" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="31" spans="2:2" ht="18">
-      <c r="B31" s="15" t="s">
+      <c r="B31" s="14" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="32" spans="2:2">
-      <c r="B32" s="16"/>
+      <c r="B32" s="15"/>
     </row>
     <row r="33" spans="2:2">
-      <c r="B33" s="16" t="s">
+      <c r="B33" s="15" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="34" spans="2:2">
-      <c r="B34" s="16" t="s">
+      <c r="B34" s="15" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="35" spans="2:2">
-      <c r="B35" s="16" t="s">
+      <c r="B35" s="15" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="37" spans="2:2">
-      <c r="B37" s="14" t="s">
+      <c r="B37" s="13" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="38" spans="2:2">
-      <c r="B38" s="16"/>
+      <c r="B38" s="15"/>
     </row>
     <row r="39" spans="2:2">
-      <c r="B39" s="16" t="s">
+      <c r="B39" s="15" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="40" spans="2:2">
-      <c r="B40" s="16" t="s">
+      <c r="B40" s="15" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="44" spans="2:2" ht="18">
-      <c r="B44" s="15" t="s">
+      <c r="B44" s="14" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="45" spans="2:2">
-      <c r="B45" s="16"/>
+      <c r="B45" s="15"/>
     </row>
     <row r="46" spans="2:2">
-      <c r="B46" s="16" t="s">
+      <c r="B46" s="15" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="47" spans="2:2">
-      <c r="B47" s="16" t="s">
+      <c r="B47" s="15" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="48" spans="2:2">
-      <c r="B48" s="16" t="s">
+      <c r="B48" s="15" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="50" spans="2:2">
-      <c r="B50" s="14" t="s">
+      <c r="B50" s="13" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="51" spans="2:2">
-      <c r="B51" s="16"/>
+      <c r="B51" s="15"/>
     </row>
     <row r="52" spans="2:2">
-      <c r="B52" s="16" t="s">
+      <c r="B52" s="15" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="53" spans="2:2">
-      <c r="B53" s="16" t="s">
+      <c r="B53" s="15" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="57" spans="2:2" ht="18">
-      <c r="B57" s="15" t="s">
+      <c r="B57" s="14" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="58" spans="2:2">
-      <c r="B58" s="16"/>
+      <c r="B58" s="15"/>
     </row>
     <row r="59" spans="2:2">
-      <c r="B59" s="16" t="s">
+      <c r="B59" s="15" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="60" spans="2:2">
-      <c r="B60" s="16" t="s">
+      <c r="B60" s="15" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="61" spans="2:2">
-      <c r="B61" s="16" t="s">
+      <c r="B61" s="15" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="63" spans="2:2">
-      <c r="B63" s="14" t="s">
+      <c r="B63" s="13" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="64" spans="2:2">
-      <c r="B64" s="16"/>
+      <c r="B64" s="15"/>
     </row>
     <row r="65" spans="2:2">
-      <c r="B65" s="16" t="s">
+      <c r="B65" s="15" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="66" spans="2:2">
-      <c r="B66" s="16" t="s">
+      <c r="B66" s="15" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="70" spans="2:2" ht="18">
-      <c r="B70" s="15" t="s">
+      <c r="B70" s="14" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="71" spans="2:2">
-      <c r="B71" s="16"/>
+      <c r="B71" s="15"/>
     </row>
     <row r="72" spans="2:2">
-      <c r="B72" s="16" t="s">
+      <c r="B72" s="15" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="73" spans="2:2">
-      <c r="B73" s="16" t="s">
+      <c r="B73" s="15" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="74" spans="2:2">
-      <c r="B74" s="16" t="s">
+      <c r="B74" s="15" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="76" spans="2:2">
-      <c r="B76" s="14" t="s">
+      <c r="B76" s="13" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="77" spans="2:2">
-      <c r="B77" s="16"/>
+      <c r="B77" s="15"/>
     </row>
     <row r="78" spans="2:2">
-      <c r="B78" s="16" t="s">
+      <c r="B78" s="15" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="79" spans="2:2">
-      <c r="B79" s="16" t="s">
+      <c r="B79" s="15" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="83" spans="2:2" ht="18">
-      <c r="B83" s="15" t="s">
+      <c r="B83" s="14" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="84" spans="2:2">
-      <c r="B84" s="16"/>
+      <c r="B84" s="15"/>
     </row>
     <row r="85" spans="2:2">
-      <c r="B85" s="16" t="s">
+      <c r="B85" s="15" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="86" spans="2:2">
-      <c r="B86" s="16" t="s">
+      <c r="B86" s="15" t="s">
         <v>99</v>
       </c>
     </row>
     <row r="88" spans="2:2">
-      <c r="B88" s="14" t="s">
+      <c r="B88" s="13" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="89" spans="2:2">
-      <c r="B89" s="16"/>
+      <c r="B89" s="15"/>
     </row>
     <row r="90" spans="2:2">
-      <c r="B90" s="16" t="s">
+      <c r="B90" s="15" t="s">
         <v>100</v>
       </c>
     </row>
     <row r="91" spans="2:2">
-      <c r="B91" s="16" t="s">
+      <c r="B91" s="15" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="95" spans="2:2" ht="18">
-      <c r="B95" s="15" t="s">
+      <c r="B95" s="14" t="s">
         <v>102</v>
       </c>
     </row>
     <row r="96" spans="2:2">
-      <c r="B96" s="16"/>
+      <c r="B96" s="15"/>
     </row>
     <row r="97" spans="2:2">
-      <c r="B97" s="16" t="s">
+      <c r="B97" s="15" t="s">
         <v>103</v>
       </c>
     </row>
     <row r="98" spans="2:2">
-      <c r="B98" s="16" t="s">
+      <c r="B98" s="15" t="s">
         <v>104</v>
       </c>
     </row>
     <row r="100" spans="2:2">
-      <c r="B100" s="14" t="s">
+      <c r="B100" s="13" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="101" spans="2:2">
-      <c r="B101" s="16"/>
+      <c r="B101" s="15"/>
     </row>
     <row r="102" spans="2:2">
-      <c r="B102" s="16" t="s">
+      <c r="B102" s="15" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="103" spans="2:2">
-      <c r="B103" s="16" t="s">
+      <c r="B103" s="15" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="107" spans="2:2" ht="18">
-      <c r="B107" s="15" t="s">
+      <c r="B107" s="14" t="s">
         <v>107</v>
       </c>
     </row>
     <row r="108" spans="2:2">
-      <c r="B108" s="16"/>
+      <c r="B108" s="15"/>
     </row>
     <row r="109" spans="2:2">
-      <c r="B109" s="16" t="s">
+      <c r="B109" s="15" t="s">
         <v>108</v>
       </c>
     </row>
     <row r="110" spans="2:2">
-      <c r="B110" s="16" t="s">
+      <c r="B110" s="15" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="112" spans="2:2">
-      <c r="B112" s="14" t="s">
+      <c r="B112" s="13" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="113" spans="2:2">
-      <c r="B113" s="16"/>
+      <c r="B113" s="15"/>
     </row>
     <row r="114" spans="2:2">
-      <c r="B114" s="16" t="s">
+      <c r="B114" s="15" t="s">
         <v>110</v>
       </c>
     </row>
     <row r="115" spans="2:2">
-      <c r="B115" s="16" t="s">
+      <c r="B115" s="15" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="119" spans="2:2" ht="18">
-      <c r="B119" s="15" t="s">
+      <c r="B119" s="14" t="s">
         <v>112</v>
       </c>
     </row>
     <row r="120" spans="2:2">
-      <c r="B120" s="16"/>
+      <c r="B120" s="15"/>
     </row>
     <row r="121" spans="2:2">
-      <c r="B121" s="16" t="s">
+      <c r="B121" s="15" t="s">
         <v>113</v>
       </c>
     </row>
     <row r="122" spans="2:2">
-      <c r="B122" s="16" t="s">
+      <c r="B122" s="15" t="s">
         <v>114</v>
       </c>
     </row>
     <row r="124" spans="2:2">
-      <c r="B124" s="14" t="s">
+      <c r="B124" s="13" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="125" spans="2:2">
-      <c r="B125" s="16"/>
+      <c r="B125" s="15"/>
     </row>
     <row r="126" spans="2:2">
-      <c r="B126" s="16" t="s">
+      <c r="B126" s="15" t="s">
         <v>115</v>
       </c>
     </row>
     <row r="127" spans="2:2">
-      <c r="B127" s="16" t="s">
+      <c r="B127" s="15" t="s">
         <v>116</v>
       </c>
     </row>
     <row r="131" spans="2:2" ht="18">
-      <c r="B131" s="15" t="s">
+      <c r="B131" s="14" t="s">
         <v>117</v>
       </c>
     </row>
     <row r="132" spans="2:2">
-      <c r="B132" s="16"/>
+      <c r="B132" s="15"/>
     </row>
     <row r="133" spans="2:2">
-      <c r="B133" s="16" t="s">
+      <c r="B133" s="15" t="s">
         <v>118</v>
       </c>
     </row>
     <row r="134" spans="2:2">
-      <c r="B134" s="16" t="s">
+      <c r="B134" s="15" t="s">
         <v>119</v>
       </c>
     </row>
     <row r="136" spans="2:2">
-      <c r="B136" s="14" t="s">
+      <c r="B136" s="13" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="137" spans="2:2">
-      <c r="B137" s="16"/>
+      <c r="B137" s="15"/>
     </row>
     <row r="138" spans="2:2">
-      <c r="B138" s="16" t="s">
+      <c r="B138" s="15" t="s">
         <v>120</v>
       </c>
     </row>
     <row r="139" spans="2:2">
-      <c r="B139" s="16" t="s">
+      <c r="B139" s="15" t="s">
         <v>121</v>
       </c>
     </row>
     <row r="143" spans="2:2" ht="18">
-      <c r="B143" s="15" t="s">
+      <c r="B143" s="14" t="s">
         <v>122</v>
       </c>
     </row>
     <row r="144" spans="2:2">
-      <c r="B144" s="16"/>
+      <c r="B144" s="15"/>
     </row>
     <row r="145" spans="2:2">
-      <c r="B145" s="16" t="s">
+      <c r="B145" s="15" t="s">
         <v>123</v>
       </c>
     </row>
     <row r="146" spans="2:2">
-      <c r="B146" s="16" t="s">
+      <c r="B146" s="15" t="s">
         <v>124</v>
       </c>
     </row>
     <row r="148" spans="2:2">
-      <c r="B148" s="14" t="s">
+      <c r="B148" s="13" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="149" spans="2:2">
-      <c r="B149" s="16"/>
+      <c r="B149" s="15"/>
     </row>
     <row r="150" spans="2:2">
-      <c r="B150" s="16" t="s">
+      <c r="B150" s="15" t="s">
         <v>125</v>
       </c>
     </row>
     <row r="151" spans="2:2">
-      <c r="B151" s="16" t="s">
+      <c r="B151" s="15" t="s">
         <v>126</v>
       </c>
     </row>
@@ -4218,50 +4444,50 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:3" ht="39" customHeight="1">
-      <c r="B2" s="17" t="s">
+      <c r="B2" s="16" t="s">
         <v>127</v>
       </c>
-      <c r="C2" s="17" t="s">
+      <c r="C2" s="16" t="s">
         <v>128</v>
       </c>
     </row>
     <row r="3" spans="2:3">
-      <c r="B3" s="18" t="s">
+      <c r="B3" s="17" t="s">
         <v>129</v>
       </c>
-      <c r="C3" s="19" t="s">
+      <c r="C3" s="18" t="s">
         <v>130</v>
       </c>
     </row>
     <row r="4" spans="2:3">
-      <c r="B4" s="18" t="s">
+      <c r="B4" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="19" t="s">
+      <c r="C4" s="18" t="s">
         <v>139</v>
       </c>
     </row>
     <row r="5" spans="2:3">
-      <c r="B5" s="18" t="s">
+      <c r="B5" s="17" t="s">
         <v>132</v>
       </c>
-      <c r="C5" s="19" t="s">
+      <c r="C5" s="18" t="s">
         <v>131</v>
       </c>
     </row>
     <row r="6" spans="2:3">
-      <c r="B6" s="18" t="s">
+      <c r="B6" s="17" t="s">
         <v>54</v>
       </c>
-      <c r="C6" s="19" t="s">
+      <c r="C6" s="18" t="s">
         <v>133</v>
       </c>
     </row>
     <row r="7" spans="2:3">
-      <c r="B7" s="18" t="s">
+      <c r="B7" s="17" t="s">
         <v>134</v>
       </c>
-      <c r="C7" s="19" t="s">
+      <c r="C7" s="18" t="s">
         <v>135</v>
       </c>
     </row>
@@ -4269,19 +4495,19 @@
       <c r="B8" s="37" t="s">
         <v>140</v>
       </c>
-      <c r="C8" s="19" t="s">
+      <c r="C8" s="18" t="s">
         <v>136</v>
       </c>
     </row>
     <row r="9" spans="2:3">
       <c r="B9" s="38"/>
-      <c r="C9" s="19" t="s">
+      <c r="C9" s="18" t="s">
         <v>137</v>
       </c>
     </row>
     <row r="10" spans="2:3">
       <c r="B10" s="39"/>
-      <c r="C10" s="19" t="s">
+      <c r="C10" s="18" t="s">
         <v>138</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Sprint 10 - v2
</commit_message>
<xml_diff>
--- a/Documentos/ProductBacklogCorregido.xlsx
+++ b/Documentos/ProductBacklogCorregido.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://liveespochedu-my.sharepoint.com/personal/jonathan_aucancela_espoch_edu_ec/Documents/Documentos/Espoch/Octavo/Aplicaciones informáticas 2/SGT/Documentos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="14" documentId="13_ncr:1_{569A54D0-C256-42F5-A166-327ADD140FB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CE6CAEF2-F9AE-4146-B97E-147BDBD13E6B}"/>
+  <xr:revisionPtr revIDLastSave="93" documentId="13_ncr:1_{569A54D0-C256-42F5-A166-327ADD140FB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3FC34356-BCDE-477B-B551-D4467B3DB9FE}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{7A8F741B-9112-4896-B995-875A9BDE94F9}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{7A8F741B-9112-4896-B995-875A9BDE94F9}"/>
   </bookViews>
   <sheets>
     <sheet name="Final" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="481" uniqueCount="375">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="505" uniqueCount="398">
   <si>
     <t>Product Backlog - SecuraBank</t>
   </si>
@@ -1213,15 +1213,6 @@
     <t>Creación del modulo de configuración para los apartados de seguridad</t>
   </si>
   <si>
-    <t>Pruebas unitarias para validar la lógica de cada módulo</t>
-  </si>
-  <si>
-    <t>Pruebas de integración para asegurarse de que el front-end se comunique correctamente con la API.</t>
-  </si>
-  <si>
-    <t>NGIX para despligue de correos</t>
-  </si>
-  <si>
     <t>11 Correciones y mejoras</t>
   </si>
   <si>
@@ -1307,13 +1298,91 @@
   </si>
   <si>
     <t>Monitorear su rendimiento y realizar ajustes según sea necesario para mantener la eficiencia y funcionalidad.</t>
+  </si>
+  <si>
+    <t>22 de enero de 2025</t>
+  </si>
+  <si>
+    <t>27 de enero de 2025</t>
+  </si>
+  <si>
+    <t>26 de enero de 2025</t>
+  </si>
+  <si>
+    <t>Verificación de pruebas mediante Hydra y Resilence - Kali</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Incorporación de MFA en la aplicación de transacciones </t>
+  </si>
+  <si>
+    <t>Control de transacciones mediante la lógica de negocio.</t>
+  </si>
+  <si>
+    <t>HU9</t>
+  </si>
+  <si>
+    <t>Validación de Estado de Transacción</t>
+  </si>
+  <si>
+    <t>Confirmación de Transacción</t>
+  </si>
+  <si>
+    <t>Reglas de Validación</t>
+  </si>
+  <si>
+    <t>Las transacciones deben ser procesadas solo si cumplen con saldo suficiente, límites de transacciones</t>
+  </si>
+  <si>
+    <t>validar todos los parámetros de la transacción antes de ser ejecutada</t>
+  </si>
+  <si>
+    <t>El sistema debe generar una confirmación explícita de la transacción antes de su ejecución</t>
+  </si>
+  <si>
+    <t>Tiempo de Expiración de Códigos MFA</t>
+  </si>
+  <si>
+    <t>Mensajes de Error de MFA</t>
+  </si>
+  <si>
+    <t>El sistema debe proporcionar mensajes de error claros y fáciles de entender si el usuario falla al ingresar el código MFA</t>
+  </si>
+  <si>
+    <t>El sistema debe permitir a los usuarios recuperar el acceso a su cuenta en caso de pérdida de acceso al método MFA</t>
+  </si>
+  <si>
+    <t>Si el monto de la transacción supera el umbral de "alto valor", se debe solicitar una verificación adicional a través de MFA</t>
+  </si>
+  <si>
+    <t>HU10</t>
+  </si>
+  <si>
+    <t>Verificación de Pruebas mediante Hydra y Resilience - Kali</t>
+  </si>
+  <si>
+    <t>Hydra debe ser capaz de realizar ataques de fuerza bruta a servicios de autenticación (como SSH, FTP, HTTP) sin errores</t>
+  </si>
+  <si>
+    <t>Resilience debe identificar correctamente posibles vulnerabilidades en la gestión de sesiones, como la falta de expiración de sesiones, protección de cookies y validación de CSRF.</t>
+  </si>
+  <si>
+    <t>manejar los errores y excepciones de manera adecuada, proporcionando mensajes claros y detallados en caso de que la prueba falle o no se pueda completar.</t>
+  </si>
+  <si>
+    <t>Iniciar un ataque o una prueba en Hydra o Resilience con configuraciones incorrectas</t>
+  </si>
+  <si>
+    <t>Ejecutar Resilience en una aplicación web para verificar si existen problemas en la gestión de sesiones</t>
+  </si>
+  <si>
+    <t>Ejecutar un ataque de fuerza bruta en una aplicación local</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9">
+  <fonts count="10">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1377,6 +1446,14 @@
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial Unicode MS"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="13">
@@ -1554,7 +1631,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1645,18 +1722,6 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1672,6 +1737,18 @@
     <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1681,6 +1758,7 @@
     <xf numFmtId="0" fontId="0" fillId="10" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1701,6 +1779,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2020,10 +2102,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83A87B21-3BDC-40F9-B20F-2399C52423D9}">
-  <dimension ref="A1:G44"/>
+  <dimension ref="A1:K44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E27" sqref="E27"/>
+    <sheetView topLeftCell="A34" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D41" sqref="D41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
@@ -2068,7 +2150,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="43.2" customHeight="1">
+    <row r="3" spans="1:7" ht="43.2" hidden="1" customHeight="1">
       <c r="A3" s="28" t="s">
         <v>27</v>
       </c>
@@ -2091,7 +2173,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="39" customHeight="1">
+    <row r="4" spans="1:7" ht="39" hidden="1" customHeight="1">
       <c r="A4" s="29"/>
       <c r="B4" s="2" t="s">
         <v>4</v>
@@ -2112,7 +2194,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="45.6" customHeight="1">
+    <row r="5" spans="1:7" ht="45.6" hidden="1" customHeight="1">
       <c r="A5" s="29"/>
       <c r="B5" s="2" t="s">
         <v>21</v>
@@ -2133,7 +2215,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="36" customHeight="1">
+    <row r="6" spans="1:7" ht="36" hidden="1" customHeight="1">
       <c r="A6" s="29"/>
       <c r="B6" s="2" t="s">
         <v>22</v>
@@ -2154,7 +2236,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="39" customHeight="1">
+    <row r="7" spans="1:7" ht="39" hidden="1" customHeight="1">
       <c r="A7" s="30"/>
       <c r="B7" s="2" t="s">
         <v>153</v>
@@ -2175,7 +2257,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="37.799999999999997" customHeight="1">
+    <row r="8" spans="1:7" ht="37.799999999999997" hidden="1" customHeight="1">
       <c r="A8" s="28" t="s">
         <v>7</v>
       </c>
@@ -2198,7 +2280,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="43.2" customHeight="1">
+    <row r="9" spans="1:7" ht="43.2" hidden="1" customHeight="1">
       <c r="A9" s="29"/>
       <c r="B9" s="2" t="s">
         <v>30</v>
@@ -2219,7 +2301,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="39.6" customHeight="1">
+    <row r="10" spans="1:7" ht="39.6" hidden="1" customHeight="1">
       <c r="A10" s="29"/>
       <c r="B10" s="2" t="s">
         <v>32</v>
@@ -2240,7 +2322,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="40.200000000000003" customHeight="1">
+    <row r="11" spans="1:7" ht="40.200000000000003" hidden="1" customHeight="1">
       <c r="A11" s="29"/>
       <c r="B11" s="2" t="s">
         <v>34</v>
@@ -2261,7 +2343,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="50.4" customHeight="1">
+    <row r="12" spans="1:7" ht="50.4" hidden="1" customHeight="1">
       <c r="A12" s="30"/>
       <c r="B12" s="2" t="s">
         <v>52</v>
@@ -2282,7 +2364,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="48.6" customHeight="1">
+    <row r="13" spans="1:7" ht="48.6" hidden="1" customHeight="1">
       <c r="A13" s="28" t="s">
         <v>9</v>
       </c>
@@ -2305,7 +2387,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="54.6" customHeight="1">
+    <row r="14" spans="1:7" ht="54.6" hidden="1" customHeight="1">
       <c r="A14" s="29"/>
       <c r="B14" s="2" t="s">
         <v>155</v>
@@ -2326,7 +2408,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="45.6" customHeight="1">
+    <row r="15" spans="1:7" ht="45.6" hidden="1" customHeight="1">
       <c r="A15" s="30"/>
       <c r="B15" s="2" t="s">
         <v>156</v>
@@ -2347,7 +2429,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="51.6" customHeight="1">
+    <row r="16" spans="1:7" ht="51.6" hidden="1" customHeight="1">
       <c r="A16" s="28" t="s">
         <v>160</v>
       </c>
@@ -2370,7 +2452,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="58.8" customHeight="1">
+    <row r="17" spans="1:7" ht="58.8" hidden="1" customHeight="1">
       <c r="A17" s="29"/>
       <c r="B17" s="2" t="s">
         <v>159</v>
@@ -2391,7 +2473,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="53.4" customHeight="1">
+    <row r="18" spans="1:7" ht="53.4" hidden="1" customHeight="1">
       <c r="A18" s="30"/>
       <c r="B18" s="2" t="s">
         <v>157</v>
@@ -2412,7 +2494,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="43.2" customHeight="1">
+    <row r="19" spans="1:7" ht="43.2" hidden="1" customHeight="1">
       <c r="A19" s="31" t="s">
         <v>210</v>
       </c>
@@ -2435,7 +2517,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="43.2">
+    <row r="20" spans="1:7" ht="43.2" hidden="1">
       <c r="A20" s="31"/>
       <c r="B20" s="2" t="s">
         <v>205</v>
@@ -2456,7 +2538,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="31.2" customHeight="1">
+    <row r="21" spans="1:7" ht="31.2" hidden="1" customHeight="1">
       <c r="A21" s="31"/>
       <c r="B21" s="2" t="s">
         <v>206</v>
@@ -2477,7 +2559,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="22" spans="1:7" ht="34.200000000000003" customHeight="1">
+    <row r="22" spans="1:7" ht="34.200000000000003" hidden="1" customHeight="1">
       <c r="A22" s="31"/>
       <c r="B22" s="2" t="s">
         <v>211</v>
@@ -2498,7 +2580,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="23" spans="1:7" ht="43.2">
+    <row r="23" spans="1:7" ht="43.2" hidden="1">
       <c r="A23" s="28" t="s">
         <v>20</v>
       </c>
@@ -2521,7 +2603,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="24" spans="1:7" ht="28.8">
+    <row r="24" spans="1:7" ht="28.8" hidden="1">
       <c r="A24" s="29"/>
       <c r="B24" s="2" t="s">
         <v>213</v>
@@ -2542,7 +2624,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="25" spans="1:7" ht="43.2">
+    <row r="25" spans="1:7" ht="43.2" hidden="1">
       <c r="A25" s="30"/>
       <c r="B25" s="2" t="s">
         <v>214</v>
@@ -2563,7 +2645,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="26" spans="1:7" ht="45" customHeight="1">
+    <row r="26" spans="1:7" ht="45" hidden="1" customHeight="1">
       <c r="A26" s="28" t="s">
         <v>267</v>
       </c>
@@ -2586,7 +2668,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="27" spans="1:7" ht="41.4" customHeight="1">
+    <row r="27" spans="1:7" ht="41.4" hidden="1" customHeight="1">
       <c r="A27" s="29"/>
       <c r="B27" s="2" t="s">
         <v>263</v>
@@ -2607,7 +2689,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="28" spans="1:7" ht="38.4" customHeight="1">
+    <row r="28" spans="1:7" ht="38.4" hidden="1" customHeight="1">
       <c r="A28" s="30"/>
       <c r="B28" s="2" t="s">
         <v>264</v>
@@ -2628,7 +2710,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="29" spans="1:7" ht="44.4" customHeight="1">
+    <row r="29" spans="1:7" ht="44.4" hidden="1" customHeight="1">
       <c r="A29" s="28" t="s">
         <v>268</v>
       </c>
@@ -2651,7 +2733,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="30" spans="1:7" ht="58.2" customHeight="1">
+    <row r="30" spans="1:7" ht="58.2" hidden="1" customHeight="1">
       <c r="A30" s="29"/>
       <c r="B30" s="2" t="s">
         <v>318</v>
@@ -2672,7 +2754,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="31" spans="1:7" ht="57.6">
+    <row r="31" spans="1:7" ht="57.6" hidden="1">
       <c r="A31" s="30"/>
       <c r="B31" s="2" t="s">
         <v>338</v>
@@ -2698,13 +2780,13 @@
         <v>269</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
       <c r="C32" s="9" t="s">
         <v>24</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>353</v>
+        <v>350</v>
       </c>
       <c r="E32" s="2">
         <v>4</v>
@@ -2716,7 +2798,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="33" spans="1:7" ht="48" customHeight="1">
+    <row r="33" spans="1:11" ht="48" customHeight="1">
       <c r="A33" s="29"/>
       <c r="B33" s="2" t="s">
         <v>331</v>
@@ -2737,7 +2819,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="34" spans="1:7" ht="45" customHeight="1">
+    <row r="34" spans="1:11" ht="45" customHeight="1">
       <c r="A34" s="29"/>
       <c r="B34" s="2" t="s">
         <v>332</v>
@@ -2758,7 +2840,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="35" spans="1:7" ht="45" customHeight="1">
+    <row r="35" spans="1:11" ht="45" customHeight="1">
       <c r="A35" s="30"/>
       <c r="B35" s="2" t="s">
         <v>333</v>
@@ -2767,7 +2849,7 @@
         <v>24</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>354</v>
+        <v>351</v>
       </c>
       <c r="E35" s="2">
         <v>4</v>
@@ -2776,21 +2858,21 @@
         <v>1</v>
       </c>
       <c r="G35" s="2" t="s">
-        <v>349</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7" ht="36.6" customHeight="1">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" ht="36.6" customHeight="1">
       <c r="A36" s="28" t="s">
         <v>272</v>
       </c>
       <c r="B36" s="2" t="s">
         <v>334</v>
       </c>
-      <c r="C36" s="10" t="s">
-        <v>5</v>
+      <c r="C36" s="9" t="s">
+        <v>24</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>345</v>
+        <v>377</v>
       </c>
       <c r="E36" s="2">
         <v>4</v>
@@ -2798,48 +2880,59 @@
       <c r="F36" s="2">
         <v>2</v>
       </c>
-      <c r="G36" s="2"/>
-    </row>
-    <row r="37" spans="1:7" ht="42" customHeight="1">
+      <c r="G36" s="2" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" ht="42" customHeight="1">
       <c r="A37" s="29"/>
       <c r="B37" s="2" t="s">
         <v>335</v>
       </c>
-      <c r="C37" s="10" t="s">
-        <v>5</v>
+      <c r="C37" s="9" t="s">
+        <v>24</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>343</v>
-      </c>
-      <c r="E37" s="2"/>
-      <c r="F37" s="2"/>
-      <c r="G37" s="2"/>
-    </row>
-    <row r="38" spans="1:7" ht="57.6">
+        <v>376</v>
+      </c>
+      <c r="E37" s="2">
+        <v>4</v>
+      </c>
+      <c r="F37" s="2">
+        <v>2</v>
+      </c>
+      <c r="G37" s="2" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" ht="41.4" customHeight="1">
       <c r="A38" s="30"/>
       <c r="B38" s="2" t="s">
-        <v>336</v>
-      </c>
-      <c r="C38" s="10" t="s">
-        <v>5</v>
+        <v>378</v>
+      </c>
+      <c r="C38" s="9" t="s">
+        <v>24</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>344</v>
+        <v>375</v>
       </c>
       <c r="E38" s="2">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="F38" s="2">
-        <v>1</v>
-      </c>
-      <c r="G38" s="2"/>
-    </row>
-    <row r="39" spans="1:7" ht="43.2">
+        <v>2</v>
+      </c>
+      <c r="G38" s="2" t="s">
+        <v>373</v>
+      </c>
+      <c r="K38" s="44"/>
+    </row>
+    <row r="39" spans="1:11" ht="43.2">
       <c r="A39" s="28" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>350</v>
+        <v>347</v>
       </c>
       <c r="C39" s="10" t="s">
         <v>5</v>
@@ -2855,10 +2948,10 @@
       </c>
       <c r="G39" s="2"/>
     </row>
-    <row r="40" spans="1:7" ht="43.2">
+    <row r="40" spans="1:11" ht="43.2">
       <c r="A40" s="29"/>
       <c r="B40" s="2" t="s">
-        <v>351</v>
+        <v>348</v>
       </c>
       <c r="C40" s="10" t="s">
         <v>5</v>
@@ -2874,10 +2967,10 @@
       </c>
       <c r="G40" s="2"/>
     </row>
-    <row r="41" spans="1:7" ht="28.8">
+    <row r="41" spans="1:11" ht="28.8">
       <c r="A41" s="30"/>
       <c r="B41" s="2" t="s">
-        <v>352</v>
+        <v>349</v>
       </c>
       <c r="C41" s="10" t="s">
         <v>5</v>
@@ -2893,9 +2986,9 @@
       </c>
       <c r="G41" s="2"/>
     </row>
-    <row r="42" spans="1:7" ht="28.8">
+    <row r="42" spans="1:11" ht="28.8">
       <c r="A42" s="28" t="s">
-        <v>347</v>
+        <v>344</v>
       </c>
       <c r="B42" s="2"/>
       <c r="C42" s="10" t="s">
@@ -2912,7 +3005,7 @@
       </c>
       <c r="G42" s="2"/>
     </row>
-    <row r="43" spans="1:7" ht="43.2">
+    <row r="43" spans="1:11" ht="43.2">
       <c r="A43" s="29"/>
       <c r="B43" s="2"/>
       <c r="C43" s="10" t="s">
@@ -2929,7 +3022,7 @@
       </c>
       <c r="G43" s="2"/>
     </row>
-    <row r="44" spans="1:7" ht="28.8">
+    <row r="44" spans="1:11" ht="28.8">
       <c r="A44" s="30"/>
       <c r="B44" s="2"/>
       <c r="C44" s="10" t="s">
@@ -2948,6 +3041,11 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A39:A41"/>
+    <mergeCell ref="A42:A44"/>
+    <mergeCell ref="A32:A35"/>
+    <mergeCell ref="A29:A31"/>
+    <mergeCell ref="A36:A38"/>
     <mergeCell ref="A26:A28"/>
     <mergeCell ref="A23:A25"/>
     <mergeCell ref="A16:A18"/>
@@ -2955,14 +3053,10 @@
     <mergeCell ref="A8:A12"/>
     <mergeCell ref="A13:A15"/>
     <mergeCell ref="A19:A22"/>
-    <mergeCell ref="A39:A41"/>
-    <mergeCell ref="A42:A44"/>
-    <mergeCell ref="A32:A35"/>
-    <mergeCell ref="A29:A31"/>
-    <mergeCell ref="A36:A38"/>
   </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2970,8 +3064,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68EE2C79-A7B0-4BE1-9026-6C6F59ABCFC9}">
   <dimension ref="A1:D62"/>
   <sheetViews>
-    <sheetView topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="C49" sqref="C49:C50"/>
+    <sheetView topLeftCell="A50" workbookViewId="0">
+      <selection activeCell="H56" sqref="H56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
@@ -2996,7 +3090,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="72">
+    <row r="2" spans="1:4" ht="72" hidden="1">
       <c r="A2" s="20" t="s">
         <v>4</v>
       </c>
@@ -3010,7 +3104,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="43.2">
+    <row r="3" spans="1:4" ht="43.2" hidden="1">
       <c r="A3" s="20" t="s">
         <v>21</v>
       </c>
@@ -3024,7 +3118,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="57.6">
+    <row r="4" spans="1:4" ht="57.6" hidden="1">
       <c r="A4" s="20" t="s">
         <v>22</v>
       </c>
@@ -3038,7 +3132,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="57.6">
+    <row r="5" spans="1:4" ht="57.6" hidden="1">
       <c r="A5" s="20" t="s">
         <v>23</v>
       </c>
@@ -3052,7 +3146,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="57.6">
+    <row r="6" spans="1:4" ht="57.6" hidden="1">
       <c r="A6" s="20" t="s">
         <v>30</v>
       </c>
@@ -3066,7 +3160,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="43.2">
+    <row r="7" spans="1:4" ht="43.2" hidden="1">
       <c r="A7" s="20" t="s">
         <v>32</v>
       </c>
@@ -3080,7 +3174,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="43.2">
+    <row r="8" spans="1:4" ht="43.2" hidden="1">
       <c r="A8" s="20" t="s">
         <v>34</v>
       </c>
@@ -3094,7 +3188,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="43.2">
+    <row r="9" spans="1:4" ht="43.2" hidden="1">
       <c r="A9" s="20" t="s">
         <v>52</v>
       </c>
@@ -3108,7 +3202,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="57.6">
+    <row r="10" spans="1:4" ht="57.6" hidden="1">
       <c r="A10" s="20" t="s">
         <v>154</v>
       </c>
@@ -3122,7 +3216,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="57.6">
+    <row r="11" spans="1:4" ht="57.6" hidden="1">
       <c r="A11" s="20" t="s">
         <v>155</v>
       </c>
@@ -3136,7 +3230,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="57.6">
+    <row r="12" spans="1:4" ht="57.6" hidden="1">
       <c r="A12" s="20" t="s">
         <v>156</v>
       </c>
@@ -3150,7 +3244,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="43.2">
+    <row r="13" spans="1:4" ht="43.2" hidden="1">
       <c r="A13" s="20" t="s">
         <v>158</v>
       </c>
@@ -3164,7 +3258,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="43.2">
+    <row r="14" spans="1:4" ht="43.2" hidden="1">
       <c r="A14" s="20" t="s">
         <v>159</v>
       </c>
@@ -3178,11 +3272,11 @@
         <v>203</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="28.8">
-      <c r="A15" s="36" t="s">
+    <row r="15" spans="1:4" ht="28.8" hidden="1">
+      <c r="A15" s="32" t="s">
         <v>204</v>
       </c>
-      <c r="B15" s="37" t="s">
+      <c r="B15" s="33" t="s">
         <v>220</v>
       </c>
       <c r="C15" s="25" t="s">
@@ -3192,9 +3286,9 @@
         <v>224</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="28.8">
-      <c r="A16" s="36"/>
-      <c r="B16" s="38"/>
+    <row r="16" spans="1:4" ht="28.8" hidden="1">
+      <c r="A16" s="32"/>
+      <c r="B16" s="34"/>
       <c r="C16" s="25" t="s">
         <v>222</v>
       </c>
@@ -3202,9 +3296,9 @@
         <v>225</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="28.8">
-      <c r="A17" s="36"/>
-      <c r="B17" s="39"/>
+    <row r="17" spans="1:4" ht="28.8" hidden="1">
+      <c r="A17" s="32"/>
+      <c r="B17" s="35"/>
       <c r="C17" s="25" t="s">
         <v>223</v>
       </c>
@@ -3212,11 +3306,11 @@
         <v>226</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="43.2">
-      <c r="A18" s="36" t="s">
+    <row r="18" spans="1:4" ht="43.2" hidden="1">
+      <c r="A18" s="32" t="s">
         <v>205</v>
       </c>
-      <c r="B18" s="37" t="s">
+      <c r="B18" s="33" t="s">
         <v>227</v>
       </c>
       <c r="C18" s="25" t="s">
@@ -3226,9 +3320,9 @@
         <v>231</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="28.8">
-      <c r="A19" s="36"/>
-      <c r="B19" s="38"/>
+    <row r="19" spans="1:4" ht="28.8" hidden="1">
+      <c r="A19" s="32"/>
+      <c r="B19" s="34"/>
       <c r="C19" s="25" t="s">
         <v>229</v>
       </c>
@@ -3236,9 +3330,9 @@
         <v>232</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="28.8">
-      <c r="A20" s="36"/>
-      <c r="B20" s="39"/>
+    <row r="20" spans="1:4" ht="28.8" hidden="1">
+      <c r="A20" s="32"/>
+      <c r="B20" s="35"/>
       <c r="C20" s="25" t="s">
         <v>230</v>
       </c>
@@ -3246,11 +3340,11 @@
         <v>233</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="28.8">
-      <c r="A21" s="36" t="s">
+    <row r="21" spans="1:4" ht="28.8" hidden="1">
+      <c r="A21" s="32" t="s">
         <v>206</v>
       </c>
-      <c r="B21" s="37" t="s">
+      <c r="B21" s="33" t="s">
         <v>240</v>
       </c>
       <c r="C21" s="21" t="s">
@@ -3260,9 +3354,9 @@
         <v>237</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="28.8">
-      <c r="A22" s="36"/>
-      <c r="B22" s="38"/>
+    <row r="22" spans="1:4" ht="28.8" hidden="1">
+      <c r="A22" s="32"/>
+      <c r="B22" s="34"/>
       <c r="C22" s="21" t="s">
         <v>235</v>
       </c>
@@ -3270,9 +3364,9 @@
         <v>238</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="28.8">
-      <c r="A23" s="36"/>
-      <c r="B23" s="39"/>
+    <row r="23" spans="1:4" ht="28.8" hidden="1">
+      <c r="A23" s="32"/>
+      <c r="B23" s="35"/>
       <c r="C23" s="21" t="s">
         <v>236</v>
       </c>
@@ -3280,11 +3374,11 @@
         <v>239</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="28.8">
-      <c r="A24" s="36" t="s">
+    <row r="24" spans="1:4" ht="28.8" hidden="1">
+      <c r="A24" s="32" t="s">
         <v>211</v>
       </c>
-      <c r="B24" s="37" t="s">
+      <c r="B24" s="33" t="s">
         <v>241</v>
       </c>
       <c r="C24" s="24" t="s">
@@ -3294,9 +3388,9 @@
         <v>245</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="28.8">
-      <c r="A25" s="36"/>
-      <c r="B25" s="38"/>
+    <row r="25" spans="1:4" ht="28.8" hidden="1">
+      <c r="A25" s="32"/>
+      <c r="B25" s="34"/>
       <c r="C25" s="24" t="s">
         <v>243</v>
       </c>
@@ -3304,9 +3398,9 @@
         <v>246</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="28.8">
-      <c r="A26" s="36"/>
-      <c r="B26" s="39"/>
+    <row r="26" spans="1:4" ht="28.8" hidden="1">
+      <c r="A26" s="32"/>
+      <c r="B26" s="35"/>
       <c r="C26" s="24" t="s">
         <v>244</v>
       </c>
@@ -3314,11 +3408,11 @@
         <v>247</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="28.8">
-      <c r="A27" s="36" t="s">
+    <row r="27" spans="1:4" ht="28.8" hidden="1">
+      <c r="A27" s="32" t="s">
         <v>213</v>
       </c>
-      <c r="B27" s="37" t="s">
+      <c r="B27" s="33" t="s">
         <v>248</v>
       </c>
       <c r="C27" s="24" t="s">
@@ -3328,9 +3422,9 @@
         <v>252</v>
       </c>
     </row>
-    <row r="28" spans="1:4" ht="28.8">
-      <c r="A28" s="36"/>
-      <c r="B28" s="38"/>
+    <row r="28" spans="1:4" ht="28.8" hidden="1">
+      <c r="A28" s="32"/>
+      <c r="B28" s="34"/>
       <c r="C28" s="24" t="s">
         <v>250</v>
       </c>
@@ -3338,9 +3432,9 @@
         <v>253</v>
       </c>
     </row>
-    <row r="29" spans="1:4" ht="28.8">
-      <c r="A29" s="36"/>
-      <c r="B29" s="39"/>
+    <row r="29" spans="1:4" ht="28.8" hidden="1">
+      <c r="A29" s="32"/>
+      <c r="B29" s="35"/>
       <c r="C29" s="24" t="s">
         <v>251</v>
       </c>
@@ -3348,11 +3442,11 @@
         <v>254</v>
       </c>
     </row>
-    <row r="30" spans="1:4" ht="14.4" customHeight="1">
-      <c r="A30" s="36" t="s">
+    <row r="30" spans="1:4" ht="14.4" hidden="1" customHeight="1">
+      <c r="A30" s="32" t="s">
         <v>214</v>
       </c>
-      <c r="B30" s="37" t="s">
+      <c r="B30" s="33" t="s">
         <v>265</v>
       </c>
       <c r="C30" s="24" t="s">
@@ -3362,9 +3456,9 @@
         <v>285</v>
       </c>
     </row>
-    <row r="31" spans="1:4" ht="33" customHeight="1">
-      <c r="A31" s="36"/>
-      <c r="B31" s="38"/>
+    <row r="31" spans="1:4" ht="33" hidden="1" customHeight="1">
+      <c r="A31" s="32"/>
+      <c r="B31" s="34"/>
       <c r="C31" s="24" t="s">
         <v>283</v>
       </c>
@@ -3372,9 +3466,9 @@
         <v>286</v>
       </c>
     </row>
-    <row r="32" spans="1:4" ht="24" customHeight="1">
-      <c r="A32" s="36"/>
-      <c r="B32" s="39"/>
+    <row r="32" spans="1:4" ht="24" hidden="1" customHeight="1">
+      <c r="A32" s="32"/>
+      <c r="B32" s="35"/>
       <c r="C32" s="24" t="s">
         <v>284</v>
       </c>
@@ -3382,11 +3476,11 @@
         <v>287</v>
       </c>
     </row>
-    <row r="33" spans="1:4" ht="36.6" customHeight="1">
-      <c r="A33" s="36" t="s">
+    <row r="33" spans="1:4" ht="36.6" hidden="1" customHeight="1">
+      <c r="A33" s="32" t="s">
         <v>262</v>
       </c>
-      <c r="B33" s="37" t="s">
+      <c r="B33" s="33" t="s">
         <v>288</v>
       </c>
       <c r="C33" s="24" t="s">
@@ -3396,9 +3490,9 @@
         <v>292</v>
       </c>
     </row>
-    <row r="34" spans="1:4" ht="26.4" customHeight="1">
-      <c r="A34" s="36"/>
-      <c r="B34" s="38"/>
+    <row r="34" spans="1:4" ht="26.4" hidden="1" customHeight="1">
+      <c r="A34" s="32"/>
+      <c r="B34" s="34"/>
       <c r="C34" s="24" t="s">
         <v>290</v>
       </c>
@@ -3406,9 +3500,9 @@
         <v>293</v>
       </c>
     </row>
-    <row r="35" spans="1:4" ht="24" customHeight="1">
-      <c r="A35" s="36"/>
-      <c r="B35" s="39"/>
+    <row r="35" spans="1:4" ht="24" hidden="1" customHeight="1">
+      <c r="A35" s="32"/>
+      <c r="B35" s="35"/>
       <c r="C35" s="24" t="s">
         <v>291</v>
       </c>
@@ -3416,11 +3510,11 @@
         <v>294</v>
       </c>
     </row>
-    <row r="36" spans="1:4" ht="36.6" customHeight="1">
-      <c r="A36" s="36" t="s">
+    <row r="36" spans="1:4" ht="36.6" hidden="1" customHeight="1">
+      <c r="A36" s="32" t="s">
         <v>263</v>
       </c>
-      <c r="B36" s="37" t="s">
+      <c r="B36" s="33" t="s">
         <v>295</v>
       </c>
       <c r="C36" s="21" t="s">
@@ -3430,9 +3524,9 @@
         <v>299</v>
       </c>
     </row>
-    <row r="37" spans="1:4" ht="34.200000000000003" customHeight="1">
-      <c r="A37" s="36"/>
-      <c r="B37" s="38"/>
+    <row r="37" spans="1:4" ht="34.200000000000003" hidden="1" customHeight="1">
+      <c r="A37" s="32"/>
+      <c r="B37" s="34"/>
       <c r="C37" s="21" t="s">
         <v>297</v>
       </c>
@@ -3440,9 +3534,9 @@
         <v>300</v>
       </c>
     </row>
-    <row r="38" spans="1:4" ht="30" customHeight="1">
-      <c r="A38" s="36"/>
-      <c r="B38" s="39"/>
+    <row r="38" spans="1:4" ht="30" hidden="1" customHeight="1">
+      <c r="A38" s="32"/>
+      <c r="B38" s="35"/>
       <c r="C38" s="21" t="s">
         <v>298</v>
       </c>
@@ -3450,11 +3544,11 @@
         <v>301</v>
       </c>
     </row>
-    <row r="39" spans="1:4" ht="61.2" customHeight="1">
-      <c r="A39" s="36" t="s">
+    <row r="39" spans="1:4" ht="61.2" hidden="1" customHeight="1">
+      <c r="A39" s="32" t="s">
         <v>264</v>
       </c>
-      <c r="B39" s="40" t="s">
+      <c r="B39" s="36" t="s">
         <v>316</v>
       </c>
       <c r="C39" s="21" t="s">
@@ -3464,9 +3558,9 @@
         <v>323</v>
       </c>
     </row>
-    <row r="40" spans="1:4" ht="23.4" customHeight="1">
-      <c r="A40" s="36"/>
-      <c r="B40" s="40"/>
+    <row r="40" spans="1:4" ht="23.4" hidden="1" customHeight="1">
+      <c r="A40" s="32"/>
+      <c r="B40" s="36"/>
       <c r="C40" s="27" t="s">
         <v>319</v>
       </c>
@@ -3474,9 +3568,9 @@
         <v>320</v>
       </c>
     </row>
-    <row r="41" spans="1:4" ht="25.2" customHeight="1">
-      <c r="A41" s="36"/>
-      <c r="B41" s="40"/>
+    <row r="41" spans="1:4" ht="25.2" hidden="1" customHeight="1">
+      <c r="A41" s="32"/>
+      <c r="B41" s="36"/>
       <c r="C41" s="27" t="s">
         <v>322</v>
       </c>
@@ -3484,11 +3578,11 @@
         <v>324</v>
       </c>
     </row>
-    <row r="42" spans="1:4" ht="43.2" customHeight="1">
-      <c r="A42" s="36" t="s">
+    <row r="42" spans="1:4" ht="43.2" hidden="1" customHeight="1">
+      <c r="A42" s="32" t="s">
         <v>266</v>
       </c>
-      <c r="B42" s="40" t="s">
+      <c r="B42" s="36" t="s">
         <v>317</v>
       </c>
       <c r="C42" s="21" t="s">
@@ -3498,9 +3592,9 @@
         <v>328</v>
       </c>
     </row>
-    <row r="43" spans="1:4" ht="28.8">
-      <c r="A43" s="36"/>
-      <c r="B43" s="40"/>
+    <row r="43" spans="1:4" ht="28.8" hidden="1">
+      <c r="A43" s="32"/>
+      <c r="B43" s="36"/>
       <c r="C43" s="21" t="s">
         <v>326</v>
       </c>
@@ -3508,9 +3602,9 @@
         <v>329</v>
       </c>
     </row>
-    <row r="44" spans="1:4" ht="28.8">
-      <c r="A44" s="36"/>
-      <c r="B44" s="40"/>
+    <row r="44" spans="1:4" ht="28.8" hidden="1">
+      <c r="A44" s="32"/>
+      <c r="B44" s="36"/>
       <c r="C44" s="21" t="s">
         <v>327</v>
       </c>
@@ -3518,185 +3612,190 @@
         <v>330</v>
       </c>
     </row>
-    <row r="45" spans="1:4" ht="43.2" customHeight="1">
-      <c r="A45" s="36" t="s">
+    <row r="45" spans="1:4" ht="43.2" hidden="1" customHeight="1">
+      <c r="A45" s="32" t="s">
         <v>331</v>
       </c>
-      <c r="B45" s="40" t="s">
+      <c r="B45" s="36" t="s">
         <v>271</v>
       </c>
       <c r="C45" s="24" t="s">
+        <v>352</v>
+      </c>
+      <c r="D45" s="24" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" ht="28.8" hidden="1" customHeight="1">
+      <c r="A46" s="32"/>
+      <c r="B46" s="36"/>
+      <c r="C46" s="37" t="s">
+        <v>353</v>
+      </c>
+      <c r="D46" s="24" t="s">
         <v>355</v>
       </c>
-      <c r="D45" s="24" t="s">
+    </row>
+    <row r="47" spans="1:4" ht="28.8" hidden="1">
+      <c r="A47" s="32"/>
+      <c r="B47" s="36"/>
+      <c r="C47" s="37"/>
+      <c r="D47" s="24" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" ht="30.6" customHeight="1">
+      <c r="A48" s="32" t="s">
+        <v>332</v>
+      </c>
+      <c r="B48" s="36" t="s">
+        <v>342</v>
+      </c>
+      <c r="C48" s="24" t="s">
         <v>357</v>
       </c>
-    </row>
-    <row r="46" spans="1:4" ht="28.8" customHeight="1">
-      <c r="A46" s="36"/>
-      <c r="B46" s="40"/>
-      <c r="C46" s="32" t="s">
-        <v>356</v>
-      </c>
-      <c r="D46" s="24" t="s">
+      <c r="D48" s="24" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" ht="33.6" customHeight="1">
+      <c r="A49" s="32"/>
+      <c r="B49" s="36"/>
+      <c r="C49" s="37" t="s">
         <v>358</v>
       </c>
-    </row>
-    <row r="47" spans="1:4" ht="28.8">
-      <c r="A47" s="36"/>
-      <c r="B47" s="40"/>
-      <c r="C47" s="32"/>
-      <c r="D47" s="24" t="s">
-        <v>359</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4" ht="30.6" customHeight="1">
-      <c r="A48" s="36" t="s">
-        <v>332</v>
-      </c>
-      <c r="B48" s="40" t="s">
-        <v>342</v>
-      </c>
-      <c r="C48" s="24" t="s">
+      <c r="D49" s="24" t="s">
         <v>360</v>
       </c>
-      <c r="D48" s="24" t="s">
+    </row>
+    <row r="50" spans="1:4" ht="43.2">
+      <c r="A50" s="32"/>
+      <c r="B50" s="36"/>
+      <c r="C50" s="37"/>
+      <c r="D50" s="24" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" ht="43.2">
+      <c r="A51" s="32" t="s">
+        <v>333</v>
+      </c>
+      <c r="B51" s="33" t="s">
+        <v>351</v>
+      </c>
+      <c r="C51" s="38" t="s">
         <v>362</v>
       </c>
-    </row>
-    <row r="49" spans="1:4" ht="33.6" customHeight="1">
-      <c r="A49" s="36"/>
-      <c r="B49" s="40"/>
-      <c r="C49" s="32" t="s">
-        <v>361</v>
-      </c>
-      <c r="D49" s="24" t="s">
+      <c r="D51" s="24" t="s">
         <v>363</v>
       </c>
     </row>
-    <row r="50" spans="1:4" ht="43.2">
-      <c r="A50" s="36"/>
-      <c r="B50" s="40"/>
-      <c r="C50" s="32"/>
-      <c r="D50" s="24" t="s">
+    <row r="52" spans="1:4" ht="28.8">
+      <c r="A52" s="32"/>
+      <c r="B52" s="34"/>
+      <c r="C52" s="39"/>
+      <c r="D52" s="24" t="s">
         <v>364</v>
       </c>
     </row>
-    <row r="51" spans="1:4" ht="43.2">
-      <c r="A51" s="36" t="s">
-        <v>333</v>
-      </c>
-      <c r="B51" s="40" t="s">
-        <v>354</v>
-      </c>
-      <c r="C51" s="33" t="s">
+    <row r="53" spans="1:4" ht="43.2">
+      <c r="A53" s="32"/>
+      <c r="B53" s="35"/>
+      <c r="C53" s="40"/>
+      <c r="D53" s="24" t="s">
         <v>365</v>
       </c>
-      <c r="D51" s="24" t="s">
-        <v>366</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4" ht="28.8">
-      <c r="A52" s="36"/>
-      <c r="B52" s="40"/>
-      <c r="C52" s="34"/>
-      <c r="D52" s="24" t="s">
-        <v>367</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4" ht="43.2">
-      <c r="A53" s="36"/>
-      <c r="B53" s="40"/>
-      <c r="C53" s="35"/>
-      <c r="D53" s="24" t="s">
-        <v>368</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4">
-      <c r="A54" s="36" t="s">
+    </row>
+    <row r="54" spans="1:4" ht="28.8" customHeight="1">
+      <c r="A54" s="32" t="s">
         <v>334</v>
       </c>
-      <c r="B54" s="37" t="s">
-        <v>345</v>
-      </c>
-      <c r="C54" s="26"/>
-      <c r="D54" s="26"/>
-    </row>
-    <row r="55" spans="1:4">
-      <c r="A55" s="36"/>
-      <c r="B55" s="38"/>
-      <c r="C55" s="26"/>
-      <c r="D55" s="26"/>
-    </row>
-    <row r="56" spans="1:4">
-      <c r="A56" s="36"/>
-      <c r="B56" s="39"/>
-      <c r="C56" s="26"/>
-      <c r="D56" s="26"/>
-    </row>
-    <row r="57" spans="1:4">
-      <c r="A57" s="36" t="s">
+      <c r="B54" s="33" t="s">
+        <v>377</v>
+      </c>
+      <c r="C54" s="26" t="s">
+        <v>379</v>
+      </c>
+      <c r="D54" s="24" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" ht="28.8">
+      <c r="A55" s="32"/>
+      <c r="B55" s="34"/>
+      <c r="C55" s="26" t="s">
+        <v>381</v>
+      </c>
+      <c r="D55" s="24" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" ht="28.8">
+      <c r="A56" s="32"/>
+      <c r="B56" s="35"/>
+      <c r="C56" s="26" t="s">
+        <v>380</v>
+      </c>
+      <c r="D56" s="24" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" ht="43.2">
+      <c r="A57" s="32" t="s">
         <v>335</v>
       </c>
-      <c r="B57" s="37" t="s">
-        <v>343</v>
-      </c>
-      <c r="C57" s="26"/>
-      <c r="D57" s="26"/>
-    </row>
-    <row r="58" spans="1:4">
-      <c r="A58" s="36"/>
-      <c r="B58" s="38"/>
-      <c r="C58" s="26"/>
-      <c r="D58" s="26"/>
-    </row>
-    <row r="59" spans="1:4">
-      <c r="A59" s="36"/>
-      <c r="B59" s="39"/>
-      <c r="C59" s="26"/>
-      <c r="D59" s="26"/>
+      <c r="B57" s="33" t="s">
+        <v>376</v>
+      </c>
+      <c r="C57" s="24" t="s">
+        <v>384</v>
+      </c>
+      <c r="D57" s="24" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" ht="28.8">
+      <c r="A58" s="32"/>
+      <c r="B58" s="34"/>
+      <c r="C58" s="26" t="s">
+        <v>385</v>
+      </c>
+      <c r="D58" s="24" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" ht="43.2">
+      <c r="A59" s="32"/>
+      <c r="B59" s="35"/>
+      <c r="C59" s="26" t="s">
+        <v>386</v>
+      </c>
+      <c r="D59" s="24" t="s">
+        <v>387</v>
+      </c>
     </row>
     <row r="60" spans="1:4">
-      <c r="A60" s="36" t="s">
+      <c r="A60" s="32" t="s">
         <v>336</v>
       </c>
-      <c r="B60" s="37"/>
+      <c r="B60" s="33"/>
       <c r="C60" s="26"/>
       <c r="D60" s="26"/>
     </row>
     <row r="61" spans="1:4">
-      <c r="A61" s="36"/>
-      <c r="B61" s="38"/>
+      <c r="A61" s="32"/>
+      <c r="B61" s="34"/>
       <c r="C61" s="26"/>
       <c r="D61" s="26"/>
     </row>
     <row r="62" spans="1:4">
-      <c r="A62" s="36"/>
-      <c r="B62" s="39"/>
+      <c r="A62" s="32"/>
+      <c r="B62" s="35"/>
       <c r="C62" s="26"/>
       <c r="D62" s="26"/>
     </row>
   </sheetData>
   <mergeCells count="35">
-    <mergeCell ref="A36:A38"/>
-    <mergeCell ref="B36:B38"/>
-    <mergeCell ref="A60:A62"/>
-    <mergeCell ref="B45:B47"/>
-    <mergeCell ref="B48:B50"/>
-    <mergeCell ref="B51:B53"/>
-    <mergeCell ref="B54:B56"/>
-    <mergeCell ref="B57:B59"/>
-    <mergeCell ref="B60:B62"/>
-    <mergeCell ref="A45:A47"/>
-    <mergeCell ref="A48:A50"/>
-    <mergeCell ref="A51:A53"/>
-    <mergeCell ref="A54:A56"/>
-    <mergeCell ref="A57:A59"/>
-    <mergeCell ref="B15:B17"/>
-    <mergeCell ref="A15:A17"/>
-    <mergeCell ref="B18:B20"/>
-    <mergeCell ref="A18:A20"/>
-    <mergeCell ref="A21:A23"/>
     <mergeCell ref="C46:C47"/>
     <mergeCell ref="C49:C50"/>
     <mergeCell ref="C51:C53"/>
@@ -3713,6 +3812,25 @@
     <mergeCell ref="B30:B32"/>
     <mergeCell ref="A33:A35"/>
     <mergeCell ref="B33:B35"/>
+    <mergeCell ref="B15:B17"/>
+    <mergeCell ref="A15:A17"/>
+    <mergeCell ref="B18:B20"/>
+    <mergeCell ref="A18:A20"/>
+    <mergeCell ref="A21:A23"/>
+    <mergeCell ref="A36:A38"/>
+    <mergeCell ref="B36:B38"/>
+    <mergeCell ref="A60:A62"/>
+    <mergeCell ref="B45:B47"/>
+    <mergeCell ref="B48:B50"/>
+    <mergeCell ref="B51:B53"/>
+    <mergeCell ref="B54:B56"/>
+    <mergeCell ref="B57:B59"/>
+    <mergeCell ref="B60:B62"/>
+    <mergeCell ref="A45:A47"/>
+    <mergeCell ref="A48:A50"/>
+    <mergeCell ref="A51:A53"/>
+    <mergeCell ref="A54:A56"/>
+    <mergeCell ref="A57:A59"/>
   </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3721,10 +3839,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{113AD7C8-E432-4900-8C71-627982E552B0}">
-  <dimension ref="A1:D16"/>
+  <dimension ref="A1:D22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
@@ -3791,10 +3909,10 @@
       </c>
     </row>
     <row r="5" spans="1:4" ht="28.8" hidden="1">
-      <c r="A5" s="36" t="s">
+      <c r="A5" s="32" t="s">
         <v>50</v>
       </c>
-      <c r="B5" s="37" t="s">
+      <c r="B5" s="33" t="s">
         <v>255</v>
       </c>
       <c r="C5" s="24" t="s">
@@ -3805,8 +3923,8 @@
       </c>
     </row>
     <row r="6" spans="1:4" ht="28.8" hidden="1">
-      <c r="A6" s="36"/>
-      <c r="B6" s="38"/>
+      <c r="A6" s="32"/>
+      <c r="B6" s="34"/>
       <c r="C6" s="24" t="s">
         <v>257</v>
       </c>
@@ -3815,8 +3933,8 @@
       </c>
     </row>
     <row r="7" spans="1:4" ht="43.2" hidden="1">
-      <c r="A7" s="36"/>
-      <c r="B7" s="39"/>
+      <c r="A7" s="32"/>
+      <c r="B7" s="35"/>
       <c r="C7" s="24" t="s">
         <v>258</v>
       </c>
@@ -3825,10 +3943,10 @@
       </c>
     </row>
     <row r="8" spans="1:4" ht="28.8" customHeight="1">
-      <c r="A8" s="36" t="s">
+      <c r="A8" s="32" t="s">
         <v>337</v>
       </c>
-      <c r="B8" s="37" t="s">
+      <c r="B8" s="33" t="s">
         <v>302</v>
       </c>
       <c r="C8" s="24" t="s">
@@ -3839,8 +3957,8 @@
       </c>
     </row>
     <row r="9" spans="1:4" ht="28.8">
-      <c r="A9" s="36"/>
-      <c r="B9" s="38"/>
+      <c r="A9" s="32"/>
+      <c r="B9" s="34"/>
       <c r="C9" s="24" t="s">
         <v>304</v>
       </c>
@@ -3849,8 +3967,8 @@
       </c>
     </row>
     <row r="10" spans="1:4" ht="28.8">
-      <c r="A10" s="36"/>
-      <c r="B10" s="39"/>
+      <c r="A10" s="32"/>
+      <c r="B10" s="35"/>
       <c r="C10" s="24" t="s">
         <v>305</v>
       </c>
@@ -3859,10 +3977,10 @@
       </c>
     </row>
     <row r="11" spans="1:4" ht="14.4" customHeight="1">
-      <c r="A11" s="36" t="s">
+      <c r="A11" s="32" t="s">
         <v>338</v>
       </c>
-      <c r="B11" s="37" t="s">
+      <c r="B11" s="33" t="s">
         <v>309</v>
       </c>
       <c r="C11" s="24" t="s">
@@ -3873,8 +3991,8 @@
       </c>
     </row>
     <row r="12" spans="1:4" ht="37.200000000000003" customHeight="1">
-      <c r="A12" s="36"/>
-      <c r="B12" s="38"/>
+      <c r="A12" s="32"/>
+      <c r="B12" s="34"/>
       <c r="C12" s="24" t="s">
         <v>311</v>
       </c>
@@ -3883,8 +4001,8 @@
       </c>
     </row>
     <row r="13" spans="1:4" ht="26.4" customHeight="1">
-      <c r="A13" s="36"/>
-      <c r="B13" s="39"/>
+      <c r="A13" s="32"/>
+      <c r="B13" s="35"/>
       <c r="C13" s="24" t="s">
         <v>312</v>
       </c>
@@ -3893,41 +4011,99 @@
       </c>
     </row>
     <row r="14" spans="1:4" ht="43.2">
-      <c r="A14" s="36" t="s">
-        <v>348</v>
-      </c>
-      <c r="B14" s="37" t="s">
-        <v>353</v>
+      <c r="A14" s="32" t="s">
+        <v>345</v>
+      </c>
+      <c r="B14" s="33" t="s">
+        <v>350</v>
       </c>
       <c r="C14" s="24" t="s">
+        <v>366</v>
+      </c>
+      <c r="D14" s="24" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="43.2">
+      <c r="A15" s="32"/>
+      <c r="B15" s="34"/>
+      <c r="C15" s="24" t="s">
+        <v>368</v>
+      </c>
+      <c r="D15" s="24" t="s">
         <v>369</v>
       </c>
-      <c r="D14" s="24" t="s">
+    </row>
+    <row r="16" spans="1:4" ht="43.2">
+      <c r="A16" s="32"/>
+      <c r="B16" s="35"/>
+      <c r="C16" s="24" t="s">
         <v>370</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" ht="43.2">
-      <c r="A15" s="36"/>
-      <c r="B15" s="38"/>
-      <c r="C15" s="24" t="s">
+      <c r="D16" s="24" t="s">
         <v>371</v>
       </c>
-      <c r="D15" s="24" t="s">
-        <v>372</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" ht="43.2">
-      <c r="A16" s="36"/>
-      <c r="B16" s="39"/>
-      <c r="C16" s="24" t="s">
-        <v>373</v>
-      </c>
-      <c r="D16" s="24" t="s">
-        <v>374</v>
-      </c>
+    </row>
+    <row r="17" spans="1:4" ht="57.6">
+      <c r="A17" s="32" t="s">
+        <v>378</v>
+      </c>
+      <c r="B17" s="33" t="s">
+        <v>391</v>
+      </c>
+      <c r="C17" s="24" t="s">
+        <v>392</v>
+      </c>
+      <c r="D17" s="24" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="72">
+      <c r="A18" s="32"/>
+      <c r="B18" s="34"/>
+      <c r="C18" s="24" t="s">
+        <v>393</v>
+      </c>
+      <c r="D18" s="24" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="31.2" customHeight="1">
+      <c r="A19" s="32"/>
+      <c r="B19" s="35"/>
+      <c r="C19" s="24" t="s">
+        <v>394</v>
+      </c>
+      <c r="D19" s="24" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4">
+      <c r="A20" s="32" t="s">
+        <v>390</v>
+      </c>
+      <c r="B20" s="33"/>
+      <c r="C20" s="24"/>
+      <c r="D20" s="24"/>
+    </row>
+    <row r="21" spans="1:4">
+      <c r="A21" s="32"/>
+      <c r="B21" s="34"/>
+      <c r="C21" s="24"/>
+      <c r="D21" s="24"/>
+    </row>
+    <row r="22" spans="1:4">
+      <c r="A22" s="32"/>
+      <c r="B22" s="35"/>
+      <c r="C22" s="24"/>
+      <c r="D22" s="24"/>
     </row>
   </sheetData>
-  <mergeCells count="8">
+  <mergeCells count="12">
+    <mergeCell ref="A17:A19"/>
+    <mergeCell ref="B17:B19"/>
+    <mergeCell ref="A20:A22"/>
+    <mergeCell ref="B20:B22"/>
     <mergeCell ref="A14:A16"/>
     <mergeCell ref="B14:B16"/>
     <mergeCell ref="A11:A13"/>

</xml_diff>

<commit_message>
Sprint 12 - v1
</commit_message>
<xml_diff>
--- a/Documentos/ProductBacklogCorregido.xlsx
+++ b/Documentos/ProductBacklogCorregido.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://liveespochedu-my.sharepoint.com/personal/jonathan_aucancela_espoch_edu_ec/Documents/Documentos/Espoch/Octavo/Aplicaciones informáticas 2/SGT/Documentos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="93" documentId="13_ncr:1_{569A54D0-C256-42F5-A166-327ADD140FB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3FC34356-BCDE-477B-B551-D4467B3DB9FE}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="6_{03CBC970-F92A-40AE-9A66-0714A992D452}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{7A8F741B-9112-4896-B995-875A9BDE94F9}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{7A8F741B-9112-4896-B995-875A9BDE94F9}"/>
   </bookViews>
   <sheets>
     <sheet name="Final" sheetId="1" r:id="rId1"/>
@@ -82,15 +82,6 @@
   </si>
   <si>
     <t>Diseñar notificaciones automáticas para administradores en caso de incidentes.</t>
-  </si>
-  <si>
-    <t>Implementar protección contra ataques CSRF y deserialización insegura.</t>
-  </si>
-  <si>
-    <t>Realizar una auditoría completa para verificar el cumplimiento de OWASP.</t>
-  </si>
-  <si>
-    <t>Mejorar el cifrado de datos en tránsito usando TLS.</t>
   </si>
   <si>
     <t>Redactar documentación técnica del sistema y manuales de usuario.</t>
@@ -1376,6 +1367,15 @@
   </si>
   <si>
     <t>Ejecutar un ataque de fuerza bruta en una aplicación local</t>
+  </si>
+  <si>
+    <t>Incorporación del protocolo HTTPS para fortalecer los niveles de seguridad en el sistema</t>
+  </si>
+  <si>
+    <t>Pruebas NGIX - correos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Despligue del proyecto SGT en un servidor free. Apache y Gunicorn </t>
   </si>
 </sst>
 </file>
@@ -1710,6 +1710,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1721,6 +1722,18 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1737,18 +1750,6 @@
     <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1758,7 +1759,6 @@
     <xf numFmtId="0" fontId="0" fillId="10" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1779,10 +1779,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2104,8 +2100,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83A87B21-3BDC-40F9-B20F-2399C52423D9}">
   <dimension ref="A1:K44"/>
   <sheetViews>
-    <sheetView topLeftCell="A34" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D41" sqref="D41"/>
+    <sheetView tabSelected="1" topLeftCell="A35" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D39" sqref="D39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
@@ -2141,27 +2137,27 @@
         <v>10</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="F2" s="8" t="s">
         <v>6</v>
       </c>
       <c r="G2" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="43.2" hidden="1" customHeight="1">
+      <c r="A3" s="29" t="s">
+        <v>24</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>25</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" ht="43.2" hidden="1" customHeight="1">
-      <c r="A3" s="28" t="s">
-        <v>27</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>152</v>
-      </c>
-      <c r="C3" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>28</v>
       </c>
       <c r="E3" s="2">
         <v>4</v>
@@ -2170,19 +2166,19 @@
         <v>1</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="39" hidden="1" customHeight="1">
-      <c r="A4" s="29"/>
+      <c r="A4" s="30"/>
       <c r="B4" s="2" t="s">
         <v>4</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="E4" s="2">
         <v>4</v>
@@ -2191,19 +2187,19 @@
         <v>1</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="45.6" hidden="1" customHeight="1">
-      <c r="A5" s="29"/>
+      <c r="A5" s="30"/>
       <c r="B5" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="C5" s="9" t="s">
-        <v>24</v>
-      </c>
       <c r="D5" s="1" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="E5" s="2">
         <v>4</v>
@@ -2212,19 +2208,19 @@
         <v>1</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="36" hidden="1" customHeight="1">
-      <c r="A6" s="29"/>
+      <c r="A6" s="30"/>
       <c r="B6" s="2" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="E6" s="2">
         <v>4</v>
@@ -2233,19 +2229,19 @@
         <v>1</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="39" hidden="1" customHeight="1">
-      <c r="A7" s="30"/>
+      <c r="A7" s="31"/>
       <c r="B7" s="2" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="E7" s="2">
         <v>4</v>
@@ -2254,21 +2250,21 @@
         <v>1</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="37.799999999999997" hidden="1" customHeight="1">
-      <c r="A8" s="28" t="s">
+      <c r="A8" s="29" t="s">
         <v>7</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="E8" s="2">
         <v>4</v>
@@ -2277,16 +2273,16 @@
         <v>1</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="43.2" hidden="1" customHeight="1">
-      <c r="A9" s="29"/>
+      <c r="A9" s="30"/>
       <c r="B9" s="2" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>8</v>
@@ -2298,19 +2294,19 @@
         <v>2</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="39.6" hidden="1" customHeight="1">
-      <c r="A10" s="29"/>
+      <c r="A10" s="30"/>
       <c r="B10" s="2" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="E10" s="2">
         <v>4</v>
@@ -2319,19 +2315,19 @@
         <v>1</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="40.200000000000003" hidden="1" customHeight="1">
-      <c r="A11" s="29"/>
+      <c r="A11" s="30"/>
       <c r="B11" s="2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C11" s="9" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="E11" s="2">
         <v>4</v>
@@ -2340,19 +2336,19 @@
         <v>2</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="50.4" hidden="1" customHeight="1">
-      <c r="A12" s="30"/>
+      <c r="A12" s="31"/>
       <c r="B12" s="2" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="E12" s="2">
         <v>4</v>
@@ -2361,21 +2357,21 @@
         <v>2</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="48.6" hidden="1" customHeight="1">
-      <c r="A13" s="28" t="s">
+      <c r="A13" s="29" t="s">
         <v>9</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="E13" s="2">
         <v>4</v>
@@ -2384,19 +2380,19 @@
         <v>1</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="54.6" hidden="1" customHeight="1">
-      <c r="A14" s="29"/>
+      <c r="A14" s="30"/>
       <c r="B14" s="2" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="C14" s="9" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="E14" s="2">
         <v>4</v>
@@ -2405,19 +2401,19 @@
         <v>2</v>
       </c>
       <c r="G14" s="2" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="45.6" hidden="1" customHeight="1">
+      <c r="A15" s="31"/>
+      <c r="B15" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="C15" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="D15" s="1" t="s">
         <v>143</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" ht="45.6" hidden="1" customHeight="1">
-      <c r="A15" s="30"/>
-      <c r="B15" s="2" t="s">
-        <v>156</v>
-      </c>
-      <c r="C15" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>146</v>
       </c>
       <c r="E15" s="2">
         <v>4</v>
@@ -2426,21 +2422,21 @@
         <v>1</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="51.6" hidden="1" customHeight="1">
-      <c r="A16" s="28" t="s">
-        <v>160</v>
+      <c r="A16" s="29" t="s">
+        <v>157</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="C16" s="9" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="E16" s="2">
         <v>4</v>
@@ -2449,19 +2445,19 @@
         <v>1</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="58.8" hidden="1" customHeight="1">
-      <c r="A17" s="29"/>
+      <c r="A17" s="30"/>
       <c r="B17" s="2" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="C17" s="9" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="E17" s="2">
         <v>4</v>
@@ -2470,19 +2466,19 @@
         <v>1</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
     </row>
     <row r="18" spans="1:7" ht="53.4" hidden="1" customHeight="1">
-      <c r="A18" s="30"/>
+      <c r="A18" s="31"/>
       <c r="B18" s="2" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="C18" s="9" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="E18" s="2">
         <v>4</v>
@@ -2491,21 +2487,21 @@
         <v>1</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
     </row>
     <row r="19" spans="1:7" ht="43.2" hidden="1" customHeight="1">
-      <c r="A19" s="31" t="s">
-        <v>210</v>
+      <c r="A19" s="32" t="s">
+        <v>207</v>
       </c>
       <c r="B19" s="2" t="s">
+        <v>201</v>
+      </c>
+      <c r="C19" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="D19" s="1" t="s">
         <v>204</v>
-      </c>
-      <c r="C19" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>207</v>
       </c>
       <c r="E19" s="2">
         <v>2</v>
@@ -2514,19 +2510,19 @@
         <v>2</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="43.2" hidden="1">
-      <c r="A20" s="31"/>
+      <c r="A20" s="32"/>
       <c r="B20" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="C20" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="D20" s="1" t="s">
         <v>205</v>
-      </c>
-      <c r="C20" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="D20" s="1" t="s">
-        <v>208</v>
       </c>
       <c r="E20" s="2">
         <v>4</v>
@@ -2535,19 +2531,19 @@
         <v>2</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="31.2" hidden="1" customHeight="1">
-      <c r="A21" s="31"/>
+      <c r="A21" s="32"/>
       <c r="B21" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="C21" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="D21" s="1" t="s">
         <v>206</v>
-      </c>
-      <c r="C21" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="D21" s="1" t="s">
-        <v>209</v>
       </c>
       <c r="E21" s="2">
         <v>4</v>
@@ -2556,19 +2552,19 @@
         <v>2</v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
     </row>
     <row r="22" spans="1:7" ht="34.200000000000003" hidden="1" customHeight="1">
-      <c r="A22" s="31"/>
+      <c r="A22" s="32"/>
       <c r="B22" s="2" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="C22" s="9" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="E22" s="2">
         <v>1</v>
@@ -2577,18 +2573,18 @@
         <v>1</v>
       </c>
       <c r="G22" s="2" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
     </row>
     <row r="23" spans="1:7" ht="43.2" hidden="1">
-      <c r="A23" s="28" t="s">
-        <v>20</v>
+      <c r="A23" s="29" t="s">
+        <v>17</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C23" s="9" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="D23" s="1" t="s">
         <v>11</v>
@@ -2600,16 +2596,16 @@
         <v>2</v>
       </c>
       <c r="G23" s="2" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
     </row>
     <row r="24" spans="1:7" ht="28.8" hidden="1">
-      <c r="A24" s="29"/>
+      <c r="A24" s="30"/>
       <c r="B24" s="2" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="C24" s="9" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="D24" s="1" t="s">
         <v>12</v>
@@ -2621,16 +2617,16 @@
         <v>1</v>
       </c>
       <c r="G24" s="2" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
     </row>
     <row r="25" spans="1:7" ht="43.2" hidden="1">
-      <c r="A25" s="30"/>
+      <c r="A25" s="31"/>
       <c r="B25" s="2" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="C25" s="9" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="D25" s="1" t="s">
         <v>13</v>
@@ -2642,21 +2638,21 @@
         <v>1</v>
       </c>
       <c r="G25" s="2" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
     </row>
     <row r="26" spans="1:7" ht="45" hidden="1" customHeight="1">
-      <c r="A26" s="28" t="s">
-        <v>267</v>
+      <c r="A26" s="29" t="s">
+        <v>264</v>
       </c>
       <c r="B26" s="2" t="s">
+        <v>259</v>
+      </c>
+      <c r="C26" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="D26" s="1" t="s">
         <v>262</v>
-      </c>
-      <c r="C26" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="D26" s="1" t="s">
-        <v>265</v>
       </c>
       <c r="E26" s="2">
         <v>4</v>
@@ -2665,19 +2661,19 @@
         <v>2</v>
       </c>
       <c r="G26" s="2" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
     </row>
     <row r="27" spans="1:7" ht="41.4" hidden="1" customHeight="1">
-      <c r="A27" s="29"/>
+      <c r="A27" s="30"/>
       <c r="B27" s="2" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="C27" s="9" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="E27" s="2">
         <v>4</v>
@@ -2686,19 +2682,19 @@
         <v>2</v>
       </c>
       <c r="G27" s="2" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
     </row>
     <row r="28" spans="1:7" ht="38.4" hidden="1" customHeight="1">
-      <c r="A28" s="30"/>
+      <c r="A28" s="31"/>
       <c r="B28" s="2" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="C28" s="9" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
       <c r="E28" s="2">
         <v>4</v>
@@ -2707,21 +2703,21 @@
         <v>1</v>
       </c>
       <c r="G28" s="2" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
     </row>
     <row r="29" spans="1:7" ht="44.4" hidden="1" customHeight="1">
-      <c r="A29" s="28" t="s">
-        <v>268</v>
+      <c r="A29" s="29" t="s">
+        <v>265</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="C29" s="9" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
       <c r="E29" s="2">
         <v>4</v>
@@ -2730,19 +2726,19 @@
         <v>1</v>
       </c>
       <c r="G29" s="2" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
     </row>
     <row r="30" spans="1:7" ht="58.2" hidden="1" customHeight="1">
-      <c r="A30" s="29"/>
+      <c r="A30" s="30"/>
       <c r="B30" s="2" t="s">
-        <v>318</v>
+        <v>315</v>
       </c>
       <c r="C30" s="9" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
       <c r="E30" s="2">
         <v>4</v>
@@ -2751,19 +2747,19 @@
         <v>1</v>
       </c>
       <c r="G30" s="2" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
     </row>
     <row r="31" spans="1:7" ht="57.6" hidden="1">
-      <c r="A31" s="30"/>
+      <c r="A31" s="31"/>
       <c r="B31" s="2" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="C31" s="9" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="E31" s="2">
         <v>4</v>
@@ -2772,21 +2768,21 @@
         <v>2</v>
       </c>
       <c r="G31" s="2" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
     </row>
     <row r="32" spans="1:7" ht="43.2">
-      <c r="A32" s="28" t="s">
-        <v>269</v>
+      <c r="A32" s="29" t="s">
+        <v>266</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>345</v>
+        <v>342</v>
       </c>
       <c r="C32" s="9" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>350</v>
+        <v>347</v>
       </c>
       <c r="E32" s="2">
         <v>4</v>
@@ -2795,19 +2791,19 @@
         <v>2</v>
       </c>
       <c r="G32" s="2" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
     </row>
     <row r="33" spans="1:11" ht="48" customHeight="1">
-      <c r="A33" s="29"/>
+      <c r="A33" s="30"/>
       <c r="B33" s="2" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
       <c r="C33" s="9" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="E33" s="2">
         <v>4</v>
@@ -2816,19 +2812,19 @@
         <v>1</v>
       </c>
       <c r="G33" s="2" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
     </row>
     <row r="34" spans="1:11" ht="45" customHeight="1">
-      <c r="A34" s="29"/>
+      <c r="A34" s="30"/>
       <c r="B34" s="2" t="s">
-        <v>332</v>
+        <v>329</v>
       </c>
       <c r="C34" s="9" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>342</v>
+        <v>339</v>
       </c>
       <c r="E34" s="2">
         <v>4</v>
@@ -2837,19 +2833,19 @@
         <v>2</v>
       </c>
       <c r="G34" s="2" t="s">
-        <v>341</v>
+        <v>338</v>
       </c>
     </row>
     <row r="35" spans="1:11" ht="45" customHeight="1">
-      <c r="A35" s="30"/>
+      <c r="A35" s="31"/>
       <c r="B35" s="2" t="s">
-        <v>333</v>
+        <v>330</v>
       </c>
       <c r="C35" s="9" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>351</v>
+        <v>348</v>
       </c>
       <c r="E35" s="2">
         <v>4</v>
@@ -2858,21 +2854,21 @@
         <v>1</v>
       </c>
       <c r="G35" s="2" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
     </row>
     <row r="36" spans="1:11" ht="36.6" customHeight="1">
-      <c r="A36" s="28" t="s">
-        <v>272</v>
+      <c r="A36" s="29" t="s">
+        <v>269</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
       <c r="C36" s="9" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>377</v>
+        <v>374</v>
       </c>
       <c r="E36" s="2">
         <v>4</v>
@@ -2881,19 +2877,19 @@
         <v>2</v>
       </c>
       <c r="G36" s="2" t="s">
-        <v>372</v>
+        <v>369</v>
       </c>
     </row>
     <row r="37" spans="1:11" ht="42" customHeight="1">
-      <c r="A37" s="29"/>
+      <c r="A37" s="30"/>
       <c r="B37" s="2" t="s">
-        <v>335</v>
+        <v>332</v>
       </c>
       <c r="C37" s="9" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>376</v>
+        <v>373</v>
       </c>
       <c r="E37" s="2">
         <v>4</v>
@@ -2902,19 +2898,19 @@
         <v>2</v>
       </c>
       <c r="G37" s="2" t="s">
-        <v>374</v>
+        <v>371</v>
       </c>
     </row>
     <row r="38" spans="1:11" ht="41.4" customHeight="1">
-      <c r="A38" s="30"/>
+      <c r="A38" s="31"/>
       <c r="B38" s="2" t="s">
-        <v>378</v>
+        <v>375</v>
       </c>
       <c r="C38" s="9" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>375</v>
+        <v>372</v>
       </c>
       <c r="E38" s="2">
         <v>8</v>
@@ -2923,129 +2919,112 @@
         <v>2</v>
       </c>
       <c r="G38" s="2" t="s">
-        <v>373</v>
-      </c>
-      <c r="K38" s="44"/>
-    </row>
-    <row r="39" spans="1:11" ht="43.2">
-      <c r="A39" s="28" t="s">
-        <v>343</v>
+        <v>370</v>
+      </c>
+      <c r="K38" s="28"/>
+    </row>
+    <row r="39" spans="1:11" ht="28.8">
+      <c r="A39" s="29" t="s">
+        <v>340</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>347</v>
+        <v>344</v>
       </c>
       <c r="C39" s="10" t="s">
         <v>5</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>14</v>
+        <v>397</v>
       </c>
       <c r="E39" s="2">
-        <v>4</v>
-      </c>
-      <c r="F39" s="2">
-        <v>2</v>
-      </c>
+        <v>8</v>
+      </c>
+      <c r="F39" s="2"/>
       <c r="G39" s="2"/>
     </row>
     <row r="40" spans="1:11" ht="43.2">
-      <c r="A40" s="29"/>
+      <c r="A40" s="30"/>
       <c r="B40" s="2" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
       <c r="C40" s="10" t="s">
         <v>5</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>15</v>
+        <v>395</v>
       </c>
       <c r="E40" s="2">
-        <v>4</v>
-      </c>
-      <c r="F40" s="2">
-        <v>1</v>
-      </c>
+        <v>8</v>
+      </c>
+      <c r="F40" s="2"/>
       <c r="G40" s="2"/>
     </row>
-    <row r="41" spans="1:11" ht="28.8">
-      <c r="A41" s="30"/>
+    <row r="41" spans="1:11">
+      <c r="A41" s="31"/>
       <c r="B41" s="2" t="s">
-        <v>349</v>
+        <v>346</v>
       </c>
       <c r="C41" s="10" t="s">
         <v>5</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>16</v>
+        <v>396</v>
       </c>
       <c r="E41" s="2">
-        <v>4</v>
-      </c>
-      <c r="F41" s="2">
-        <v>2</v>
-      </c>
+        <v>8</v>
+      </c>
+      <c r="F41" s="2"/>
       <c r="G41" s="2"/>
     </row>
     <row r="42" spans="1:11" ht="28.8">
-      <c r="A42" s="28" t="s">
-        <v>344</v>
+      <c r="A42" s="29" t="s">
+        <v>341</v>
       </c>
       <c r="B42" s="2"/>
       <c r="C42" s="10" t="s">
         <v>5</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="E42" s="2">
-        <v>4</v>
-      </c>
-      <c r="F42" s="2">
-        <v>1</v>
-      </c>
+        <v>8</v>
+      </c>
+      <c r="F42" s="2"/>
       <c r="G42" s="2"/>
     </row>
     <row r="43" spans="1:11" ht="43.2">
-      <c r="A43" s="29"/>
+      <c r="A43" s="30"/>
       <c r="B43" s="2"/>
       <c r="C43" s="10" t="s">
         <v>5</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="E43" s="2">
-        <v>4</v>
-      </c>
-      <c r="F43" s="2">
-        <v>1</v>
-      </c>
+        <v>8</v>
+      </c>
+      <c r="F43" s="2"/>
       <c r="G43" s="2"/>
     </row>
     <row r="44" spans="1:11" ht="28.8">
-      <c r="A44" s="30"/>
+      <c r="A44" s="31"/>
       <c r="B44" s="2"/>
       <c r="C44" s="10" t="s">
         <v>5</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="E44" s="2">
-        <v>4</v>
-      </c>
-      <c r="F44" s="2">
-        <v>1</v>
-      </c>
+        <v>8</v>
+      </c>
+      <c r="F44" s="2"/>
       <c r="G44" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="A39:A41"/>
-    <mergeCell ref="A42:A44"/>
-    <mergeCell ref="A32:A35"/>
-    <mergeCell ref="A29:A31"/>
-    <mergeCell ref="A36:A38"/>
     <mergeCell ref="A26:A28"/>
     <mergeCell ref="A23:A25"/>
     <mergeCell ref="A16:A18"/>
@@ -3053,6 +3032,11 @@
     <mergeCell ref="A8:A12"/>
     <mergeCell ref="A13:A15"/>
     <mergeCell ref="A19:A22"/>
+    <mergeCell ref="A39:A41"/>
+    <mergeCell ref="A42:A44"/>
+    <mergeCell ref="A32:A35"/>
+    <mergeCell ref="A29:A31"/>
+    <mergeCell ref="A36:A38"/>
   </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3081,13 +3065,13 @@
         <v>1</v>
       </c>
       <c r="B1" s="19" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C1" s="19" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="D1" s="19" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="72" hidden="1">
@@ -3095,707 +3079,726 @@
         <v>4</v>
       </c>
       <c r="B2" s="22" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C2" s="25" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="D2" s="25" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="43.2" hidden="1">
       <c r="A3" s="20" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B3" s="22" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="C3" s="25" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="D3" s="25" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="57.6" hidden="1">
       <c r="A4" s="20" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B4" s="22" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C4" s="25" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="D4" s="25" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="57.6" hidden="1">
       <c r="A5" s="20" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B5" s="22" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="C5" s="25" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="D5" s="25" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="57.6" hidden="1">
       <c r="A6" s="20" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B6" s="22" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="C6" s="25" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="D6" s="25" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="43.2" hidden="1">
       <c r="A7" s="20" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B7" s="22" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="C7" s="25" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="D7" s="25" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="43.2" hidden="1">
       <c r="A8" s="20" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B8" s="22" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="C8" s="25" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="D8" s="25" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="43.2" hidden="1">
       <c r="A9" s="20" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="B9" s="22" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="C9" s="25" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="D9" s="25" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="57.6" hidden="1">
       <c r="A10" s="20" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="B10" s="22" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="C10" s="25" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="D10" s="25" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="57.6" hidden="1">
       <c r="A11" s="20" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="B11" s="22" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="C11" s="25" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="D11" s="25" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="57.6" hidden="1">
       <c r="A12" s="20" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="B12" s="22" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="C12" s="25" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="D12" s="25" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="43.2" hidden="1">
       <c r="A13" s="20" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="B13" s="22" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="C13" s="25" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="D13" s="25" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="43.2" hidden="1">
       <c r="A14" s="20" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="B14" s="22" t="s">
+        <v>198</v>
+      </c>
+      <c r="C14" s="25" t="s">
+        <v>199</v>
+      </c>
+      <c r="D14" s="25" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="28.8" hidden="1">
+      <c r="A15" s="37" t="s">
         <v>201</v>
       </c>
-      <c r="C14" s="25" t="s">
+      <c r="B15" s="38" t="s">
+        <v>217</v>
+      </c>
+      <c r="C15" s="25" t="s">
+        <v>218</v>
+      </c>
+      <c r="D15" s="25" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="28.8" hidden="1">
+      <c r="A16" s="37"/>
+      <c r="B16" s="39"/>
+      <c r="C16" s="25" t="s">
+        <v>219</v>
+      </c>
+      <c r="D16" s="25" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="28.8" hidden="1">
+      <c r="A17" s="37"/>
+      <c r="B17" s="40"/>
+      <c r="C17" s="25" t="s">
+        <v>220</v>
+      </c>
+      <c r="D17" s="25" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="43.2" hidden="1">
+      <c r="A18" s="37" t="s">
         <v>202</v>
       </c>
-      <c r="D14" s="25" t="s">
+      <c r="B18" s="38" t="s">
+        <v>224</v>
+      </c>
+      <c r="C18" s="25" t="s">
+        <v>225</v>
+      </c>
+      <c r="D18" s="25" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="28.8" hidden="1">
+      <c r="A19" s="37"/>
+      <c r="B19" s="39"/>
+      <c r="C19" s="25" t="s">
+        <v>226</v>
+      </c>
+      <c r="D19" s="25" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="28.8" hidden="1">
+      <c r="A20" s="37"/>
+      <c r="B20" s="40"/>
+      <c r="C20" s="25" t="s">
+        <v>227</v>
+      </c>
+      <c r="D20" s="25" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="28.8" hidden="1">
+      <c r="A21" s="37" t="s">
         <v>203</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" ht="28.8" hidden="1">
-      <c r="A15" s="32" t="s">
-        <v>204</v>
-      </c>
-      <c r="B15" s="33" t="s">
-        <v>220</v>
-      </c>
-      <c r="C15" s="25" t="s">
-        <v>221</v>
-      </c>
-      <c r="D15" s="25" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" ht="28.8" hidden="1">
-      <c r="A16" s="32"/>
-      <c r="B16" s="34"/>
-      <c r="C16" s="25" t="s">
-        <v>222</v>
-      </c>
-      <c r="D16" s="25" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" ht="28.8" hidden="1">
-      <c r="A17" s="32"/>
-      <c r="B17" s="35"/>
-      <c r="C17" s="25" t="s">
-        <v>223</v>
-      </c>
-      <c r="D17" s="25" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" ht="43.2" hidden="1">
-      <c r="A18" s="32" t="s">
-        <v>205</v>
-      </c>
-      <c r="B18" s="33" t="s">
-        <v>227</v>
-      </c>
-      <c r="C18" s="25" t="s">
-        <v>228</v>
-      </c>
-      <c r="D18" s="25" t="s">
+      <c r="B21" s="38" t="s">
+        <v>237</v>
+      </c>
+      <c r="C21" s="21" t="s">
         <v>231</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" ht="28.8" hidden="1">
-      <c r="A19" s="32"/>
-      <c r="B19" s="34"/>
-      <c r="C19" s="25" t="s">
-        <v>229</v>
-      </c>
-      <c r="D19" s="25" t="s">
+      <c r="D21" s="21" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="28.8" hidden="1">
+      <c r="A22" s="37"/>
+      <c r="B22" s="39"/>
+      <c r="C22" s="21" t="s">
         <v>232</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" ht="28.8" hidden="1">
-      <c r="A20" s="32"/>
-      <c r="B20" s="35"/>
-      <c r="C20" s="25" t="s">
-        <v>230</v>
-      </c>
-      <c r="D20" s="25" t="s">
+      <c r="D22" s="21" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="28.8" hidden="1">
+      <c r="A23" s="37"/>
+      <c r="B23" s="40"/>
+      <c r="C23" s="21" t="s">
         <v>233</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" ht="28.8" hidden="1">
-      <c r="A21" s="32" t="s">
-        <v>206</v>
-      </c>
-      <c r="B21" s="33" t="s">
+      <c r="D23" s="21" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="28.8" hidden="1">
+      <c r="A24" s="37" t="s">
+        <v>208</v>
+      </c>
+      <c r="B24" s="38" t="s">
+        <v>238</v>
+      </c>
+      <c r="C24" s="24" t="s">
+        <v>239</v>
+      </c>
+      <c r="D24" s="24" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="28.8" hidden="1">
+      <c r="A25" s="37"/>
+      <c r="B25" s="39"/>
+      <c r="C25" s="24" t="s">
         <v>240</v>
       </c>
-      <c r="C21" s="21" t="s">
-        <v>234</v>
-      </c>
-      <c r="D21" s="21" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" ht="28.8" hidden="1">
-      <c r="A22" s="32"/>
-      <c r="B22" s="34"/>
-      <c r="C22" s="21" t="s">
-        <v>235</v>
-      </c>
-      <c r="D22" s="21" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" ht="28.8" hidden="1">
-      <c r="A23" s="32"/>
-      <c r="B23" s="35"/>
-      <c r="C23" s="21" t="s">
-        <v>236</v>
-      </c>
-      <c r="D23" s="21" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" ht="28.8" hidden="1">
-      <c r="A24" s="32" t="s">
+      <c r="D25" s="24" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="28.8" hidden="1">
+      <c r="A26" s="37"/>
+      <c r="B26" s="40"/>
+      <c r="C26" s="24" t="s">
+        <v>241</v>
+      </c>
+      <c r="D26" s="24" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" ht="28.8" hidden="1">
+      <c r="A27" s="37" t="s">
+        <v>210</v>
+      </c>
+      <c r="B27" s="38" t="s">
+        <v>245</v>
+      </c>
+      <c r="C27" s="24" t="s">
+        <v>246</v>
+      </c>
+      <c r="D27" s="24" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" ht="28.8" hidden="1">
+      <c r="A28" s="37"/>
+      <c r="B28" s="39"/>
+      <c r="C28" s="24" t="s">
+        <v>247</v>
+      </c>
+      <c r="D28" s="24" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" ht="28.8" hidden="1">
+      <c r="A29" s="37"/>
+      <c r="B29" s="40"/>
+      <c r="C29" s="24" t="s">
+        <v>248</v>
+      </c>
+      <c r="D29" s="24" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" ht="14.4" hidden="1" customHeight="1">
+      <c r="A30" s="37" t="s">
         <v>211</v>
       </c>
-      <c r="B24" s="33" t="s">
-        <v>241</v>
-      </c>
-      <c r="C24" s="24" t="s">
-        <v>242</v>
-      </c>
-      <c r="D24" s="24" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" ht="28.8" hidden="1">
-      <c r="A25" s="32"/>
-      <c r="B25" s="34"/>
-      <c r="C25" s="24" t="s">
-        <v>243</v>
-      </c>
-      <c r="D25" s="24" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" ht="28.8" hidden="1">
-      <c r="A26" s="32"/>
-      <c r="B26" s="35"/>
-      <c r="C26" s="24" t="s">
-        <v>244</v>
-      </c>
-      <c r="D26" s="24" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" ht="28.8" hidden="1">
-      <c r="A27" s="32" t="s">
-        <v>213</v>
-      </c>
-      <c r="B27" s="33" t="s">
-        <v>248</v>
-      </c>
-      <c r="C27" s="24" t="s">
-        <v>249</v>
-      </c>
-      <c r="D27" s="24" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" ht="28.8" hidden="1">
-      <c r="A28" s="32"/>
-      <c r="B28" s="34"/>
-      <c r="C28" s="24" t="s">
-        <v>250</v>
-      </c>
-      <c r="D28" s="24" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" ht="28.8" hidden="1">
-      <c r="A29" s="32"/>
-      <c r="B29" s="35"/>
-      <c r="C29" s="24" t="s">
-        <v>251</v>
-      </c>
-      <c r="D29" s="24" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" ht="14.4" hidden="1" customHeight="1">
-      <c r="A30" s="32" t="s">
-        <v>214</v>
-      </c>
-      <c r="B30" s="33" t="s">
-        <v>265</v>
+      <c r="B30" s="38" t="s">
+        <v>262</v>
       </c>
       <c r="C30" s="24" t="s">
+        <v>279</v>
+      </c>
+      <c r="D30" s="24" t="s">
         <v>282</v>
       </c>
-      <c r="D30" s="24" t="s">
+    </row>
+    <row r="31" spans="1:4" ht="33" hidden="1" customHeight="1">
+      <c r="A31" s="37"/>
+      <c r="B31" s="39"/>
+      <c r="C31" s="24" t="s">
+        <v>280</v>
+      </c>
+      <c r="D31" s="24" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" ht="24" hidden="1" customHeight="1">
+      <c r="A32" s="37"/>
+      <c r="B32" s="40"/>
+      <c r="C32" s="24" t="s">
+        <v>281</v>
+      </c>
+      <c r="D32" s="24" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" ht="36.6" hidden="1" customHeight="1">
+      <c r="A33" s="37" t="s">
+        <v>259</v>
+      </c>
+      <c r="B33" s="38" t="s">
         <v>285</v>
       </c>
-    </row>
-    <row r="31" spans="1:4" ht="33" hidden="1" customHeight="1">
-      <c r="A31" s="32"/>
-      <c r="B31" s="34"/>
-      <c r="C31" s="24" t="s">
-        <v>283</v>
-      </c>
-      <c r="D31" s="24" t="s">
+      <c r="C33" s="24" t="s">
         <v>286</v>
       </c>
-    </row>
-    <row r="32" spans="1:4" ht="24" hidden="1" customHeight="1">
-      <c r="A32" s="32"/>
-      <c r="B32" s="35"/>
-      <c r="C32" s="24" t="s">
-        <v>284</v>
-      </c>
-      <c r="D32" s="24" t="s">
+      <c r="D33" s="24" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" ht="26.4" hidden="1" customHeight="1">
+      <c r="A34" s="37"/>
+      <c r="B34" s="39"/>
+      <c r="C34" s="24" t="s">
         <v>287</v>
       </c>
-    </row>
-    <row r="33" spans="1:4" ht="36.6" hidden="1" customHeight="1">
-      <c r="A33" s="32" t="s">
-        <v>262</v>
-      </c>
-      <c r="B33" s="33" t="s">
+      <c r="D34" s="24" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" ht="24" hidden="1" customHeight="1">
+      <c r="A35" s="37"/>
+      <c r="B35" s="40"/>
+      <c r="C35" s="24" t="s">
         <v>288</v>
       </c>
-      <c r="C33" s="24" t="s">
-        <v>289</v>
-      </c>
-      <c r="D33" s="24" t="s">
+      <c r="D35" s="24" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" ht="36.6" hidden="1" customHeight="1">
+      <c r="A36" s="37" t="s">
+        <v>260</v>
+      </c>
+      <c r="B36" s="38" t="s">
         <v>292</v>
       </c>
-    </row>
-    <row r="34" spans="1:4" ht="26.4" hidden="1" customHeight="1">
-      <c r="A34" s="32"/>
-      <c r="B34" s="34"/>
-      <c r="C34" s="24" t="s">
-        <v>290</v>
-      </c>
-      <c r="D34" s="24" t="s">
+      <c r="C36" s="21" t="s">
         <v>293</v>
       </c>
-    </row>
-    <row r="35" spans="1:4" ht="24" hidden="1" customHeight="1">
-      <c r="A35" s="32"/>
-      <c r="B35" s="35"/>
-      <c r="C35" s="24" t="s">
-        <v>291</v>
-      </c>
-      <c r="D35" s="24" t="s">
+      <c r="D36" s="21" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" ht="34.200000000000003" hidden="1" customHeight="1">
+      <c r="A37" s="37"/>
+      <c r="B37" s="39"/>
+      <c r="C37" s="21" t="s">
         <v>294</v>
       </c>
-    </row>
-    <row r="36" spans="1:4" ht="36.6" hidden="1" customHeight="1">
-      <c r="A36" s="32" t="s">
+      <c r="D37" s="21" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" ht="30" hidden="1" customHeight="1">
+      <c r="A38" s="37"/>
+      <c r="B38" s="40"/>
+      <c r="C38" s="21" t="s">
+        <v>295</v>
+      </c>
+      <c r="D38" s="21" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" ht="61.2" hidden="1" customHeight="1">
+      <c r="A39" s="37" t="s">
+        <v>261</v>
+      </c>
+      <c r="B39" s="41" t="s">
+        <v>313</v>
+      </c>
+      <c r="C39" s="21" t="s">
+        <v>318</v>
+      </c>
+      <c r="D39" s="27" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" ht="23.4" hidden="1" customHeight="1">
+      <c r="A40" s="37"/>
+      <c r="B40" s="41"/>
+      <c r="C40" s="27" t="s">
+        <v>316</v>
+      </c>
+      <c r="D40" s="27" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" ht="25.2" hidden="1" customHeight="1">
+      <c r="A41" s="37"/>
+      <c r="B41" s="41"/>
+      <c r="C41" s="27" t="s">
+        <v>319</v>
+      </c>
+      <c r="D41" s="27" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" ht="43.2" hidden="1" customHeight="1">
+      <c r="A42" s="37" t="s">
         <v>263</v>
       </c>
-      <c r="B36" s="33" t="s">
-        <v>295</v>
-      </c>
-      <c r="C36" s="21" t="s">
-        <v>296</v>
-      </c>
-      <c r="D36" s="21" t="s">
-        <v>299</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" ht="34.200000000000003" hidden="1" customHeight="1">
-      <c r="A37" s="32"/>
-      <c r="B37" s="34"/>
-      <c r="C37" s="21" t="s">
-        <v>297</v>
-      </c>
-      <c r="D37" s="21" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" ht="30" hidden="1" customHeight="1">
-      <c r="A38" s="32"/>
-      <c r="B38" s="35"/>
-      <c r="C38" s="21" t="s">
-        <v>298</v>
-      </c>
-      <c r="D38" s="21" t="s">
-        <v>301</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" ht="61.2" hidden="1" customHeight="1">
-      <c r="A39" s="32" t="s">
-        <v>264</v>
-      </c>
-      <c r="B39" s="36" t="s">
-        <v>316</v>
-      </c>
-      <c r="C39" s="21" t="s">
-        <v>321</v>
-      </c>
-      <c r="D39" s="27" t="s">
+      <c r="B42" s="41" t="s">
+        <v>314</v>
+      </c>
+      <c r="C42" s="21" t="s">
+        <v>322</v>
+      </c>
+      <c r="D42" s="21" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" ht="28.8" hidden="1">
+      <c r="A43" s="37"/>
+      <c r="B43" s="41"/>
+      <c r="C43" s="21" t="s">
         <v>323</v>
       </c>
-    </row>
-    <row r="40" spans="1:4" ht="23.4" hidden="1" customHeight="1">
-      <c r="A40" s="32"/>
-      <c r="B40" s="36"/>
-      <c r="C40" s="27" t="s">
-        <v>319</v>
-      </c>
-      <c r="D40" s="27" t="s">
-        <v>320</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" ht="25.2" hidden="1" customHeight="1">
-      <c r="A41" s="32"/>
-      <c r="B41" s="36"/>
-      <c r="C41" s="27" t="s">
-        <v>322</v>
-      </c>
-      <c r="D41" s="27" t="s">
+      <c r="D43" s="21" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" ht="28.8" hidden="1">
+      <c r="A44" s="37"/>
+      <c r="B44" s="41"/>
+      <c r="C44" s="21" t="s">
         <v>324</v>
       </c>
-    </row>
-    <row r="42" spans="1:4" ht="43.2" hidden="1" customHeight="1">
-      <c r="A42" s="32" t="s">
-        <v>266</v>
-      </c>
-      <c r="B42" s="36" t="s">
-        <v>317</v>
-      </c>
-      <c r="C42" s="21" t="s">
-        <v>325</v>
-      </c>
-      <c r="D42" s="21" t="s">
+      <c r="D44" s="21" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" ht="43.2" hidden="1" customHeight="1">
+      <c r="A45" s="37" t="s">
         <v>328</v>
       </c>
-    </row>
-    <row r="43" spans="1:4" ht="28.8" hidden="1">
-      <c r="A43" s="32"/>
-      <c r="B43" s="36"/>
-      <c r="C43" s="21" t="s">
-        <v>326</v>
-      </c>
-      <c r="D43" s="21" t="s">
+      <c r="B45" s="41" t="s">
+        <v>268</v>
+      </c>
+      <c r="C45" s="24" t="s">
+        <v>349</v>
+      </c>
+      <c r="D45" s="24" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" ht="28.8" hidden="1" customHeight="1">
+      <c r="A46" s="37"/>
+      <c r="B46" s="41"/>
+      <c r="C46" s="33" t="s">
+        <v>350</v>
+      </c>
+      <c r="D46" s="24" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" ht="28.8" hidden="1">
+      <c r="A47" s="37"/>
+      <c r="B47" s="41"/>
+      <c r="C47" s="33"/>
+      <c r="D47" s="24" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" ht="30.6" customHeight="1">
+      <c r="A48" s="37" t="s">
         <v>329</v>
       </c>
-    </row>
-    <row r="44" spans="1:4" ht="28.8" hidden="1">
-      <c r="A44" s="32"/>
-      <c r="B44" s="36"/>
-      <c r="C44" s="21" t="s">
-        <v>327</v>
-      </c>
-      <c r="D44" s="21" t="s">
+      <c r="B48" s="41" t="s">
+        <v>339</v>
+      </c>
+      <c r="C48" s="24" t="s">
+        <v>354</v>
+      </c>
+      <c r="D48" s="24" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" ht="33.6" customHeight="1">
+      <c r="A49" s="37"/>
+      <c r="B49" s="41"/>
+      <c r="C49" s="33" t="s">
+        <v>355</v>
+      </c>
+      <c r="D49" s="24" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" ht="43.2">
+      <c r="A50" s="37"/>
+      <c r="B50" s="41"/>
+      <c r="C50" s="33"/>
+      <c r="D50" s="24" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" ht="43.2">
+      <c r="A51" s="37" t="s">
         <v>330</v>
       </c>
-    </row>
-    <row r="45" spans="1:4" ht="43.2" hidden="1" customHeight="1">
-      <c r="A45" s="32" t="s">
+      <c r="B51" s="38" t="s">
+        <v>348</v>
+      </c>
+      <c r="C51" s="34" t="s">
+        <v>359</v>
+      </c>
+      <c r="D51" s="24" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" ht="28.8">
+      <c r="A52" s="37"/>
+      <c r="B52" s="39"/>
+      <c r="C52" s="35"/>
+      <c r="D52" s="24" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" ht="43.2">
+      <c r="A53" s="37"/>
+      <c r="B53" s="40"/>
+      <c r="C53" s="36"/>
+      <c r="D53" s="24" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" ht="28.8" customHeight="1">
+      <c r="A54" s="37" t="s">
         <v>331</v>
       </c>
-      <c r="B45" s="36" t="s">
-        <v>271</v>
-      </c>
-      <c r="C45" s="24" t="s">
-        <v>352</v>
-      </c>
-      <c r="D45" s="24" t="s">
-        <v>354</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" ht="28.8" hidden="1" customHeight="1">
-      <c r="A46" s="32"/>
-      <c r="B46" s="36"/>
-      <c r="C46" s="37" t="s">
-        <v>353</v>
-      </c>
-      <c r="D46" s="24" t="s">
-        <v>355</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" ht="28.8" hidden="1">
-      <c r="A47" s="32"/>
-      <c r="B47" s="36"/>
-      <c r="C47" s="37"/>
-      <c r="D47" s="24" t="s">
-        <v>356</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4" ht="30.6" customHeight="1">
-      <c r="A48" s="32" t="s">
+      <c r="B54" s="38" t="s">
+        <v>374</v>
+      </c>
+      <c r="C54" s="26" t="s">
+        <v>376</v>
+      </c>
+      <c r="D54" s="24" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" ht="28.8">
+      <c r="A55" s="37"/>
+      <c r="B55" s="39"/>
+      <c r="C55" s="26" t="s">
+        <v>378</v>
+      </c>
+      <c r="D55" s="24" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" ht="28.8">
+      <c r="A56" s="37"/>
+      <c r="B56" s="40"/>
+      <c r="C56" s="26" t="s">
+        <v>377</v>
+      </c>
+      <c r="D56" s="24" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" ht="43.2">
+      <c r="A57" s="37" t="s">
         <v>332</v>
       </c>
-      <c r="B48" s="36" t="s">
-        <v>342</v>
-      </c>
-      <c r="C48" s="24" t="s">
-        <v>357</v>
-      </c>
-      <c r="D48" s="24" t="s">
-        <v>359</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" ht="33.6" customHeight="1">
-      <c r="A49" s="32"/>
-      <c r="B49" s="36"/>
-      <c r="C49" s="37" t="s">
-        <v>358</v>
-      </c>
-      <c r="D49" s="24" t="s">
-        <v>360</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4" ht="43.2">
-      <c r="A50" s="32"/>
-      <c r="B50" s="36"/>
-      <c r="C50" s="37"/>
-      <c r="D50" s="24" t="s">
-        <v>361</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4" ht="43.2">
-      <c r="A51" s="32" t="s">
+      <c r="B57" s="38" t="s">
+        <v>373</v>
+      </c>
+      <c r="C57" s="24" t="s">
+        <v>381</v>
+      </c>
+      <c r="D57" s="24" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" ht="28.8">
+      <c r="A58" s="37"/>
+      <c r="B58" s="39"/>
+      <c r="C58" s="26" t="s">
+        <v>382</v>
+      </c>
+      <c r="D58" s="24" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" ht="43.2">
+      <c r="A59" s="37"/>
+      <c r="B59" s="40"/>
+      <c r="C59" s="26" t="s">
+        <v>383</v>
+      </c>
+      <c r="D59" s="24" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4">
+      <c r="A60" s="37" t="s">
         <v>333</v>
       </c>
-      <c r="B51" s="33" t="s">
-        <v>351</v>
-      </c>
-      <c r="C51" s="38" t="s">
-        <v>362</v>
-      </c>
-      <c r="D51" s="24" t="s">
-        <v>363</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4" ht="28.8">
-      <c r="A52" s="32"/>
-      <c r="B52" s="34"/>
-      <c r="C52" s="39"/>
-      <c r="D52" s="24" t="s">
-        <v>364</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4" ht="43.2">
-      <c r="A53" s="32"/>
-      <c r="B53" s="35"/>
-      <c r="C53" s="40"/>
-      <c r="D53" s="24" t="s">
-        <v>365</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4" ht="28.8" customHeight="1">
-      <c r="A54" s="32" t="s">
-        <v>334</v>
-      </c>
-      <c r="B54" s="33" t="s">
-        <v>377</v>
-      </c>
-      <c r="C54" s="26" t="s">
-        <v>379</v>
-      </c>
-      <c r="D54" s="24" t="s">
-        <v>382</v>
-      </c>
-    </row>
-    <row r="55" spans="1:4" ht="28.8">
-      <c r="A55" s="32"/>
-      <c r="B55" s="34"/>
-      <c r="C55" s="26" t="s">
-        <v>381</v>
-      </c>
-      <c r="D55" s="24" t="s">
-        <v>383</v>
-      </c>
-    </row>
-    <row r="56" spans="1:4" ht="28.8">
-      <c r="A56" s="32"/>
-      <c r="B56" s="35"/>
-      <c r="C56" s="26" t="s">
-        <v>380</v>
-      </c>
-      <c r="D56" s="24" t="s">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="57" spans="1:4" ht="43.2">
-      <c r="A57" s="32" t="s">
-        <v>335</v>
-      </c>
-      <c r="B57" s="33" t="s">
-        <v>376</v>
-      </c>
-      <c r="C57" s="24" t="s">
-        <v>384</v>
-      </c>
-      <c r="D57" s="24" t="s">
-        <v>389</v>
-      </c>
-    </row>
-    <row r="58" spans="1:4" ht="28.8">
-      <c r="A58" s="32"/>
-      <c r="B58" s="34"/>
-      <c r="C58" s="26" t="s">
-        <v>385</v>
-      </c>
-      <c r="D58" s="24" t="s">
-        <v>388</v>
-      </c>
-    </row>
-    <row r="59" spans="1:4" ht="43.2">
-      <c r="A59" s="32"/>
-      <c r="B59" s="35"/>
-      <c r="C59" s="26" t="s">
-        <v>386</v>
-      </c>
-      <c r="D59" s="24" t="s">
-        <v>387</v>
-      </c>
-    </row>
-    <row r="60" spans="1:4">
-      <c r="A60" s="32" t="s">
-        <v>336</v>
-      </c>
-      <c r="B60" s="33"/>
+      <c r="B60" s="38"/>
       <c r="C60" s="26"/>
       <c r="D60" s="26"/>
     </row>
     <row r="61" spans="1:4">
-      <c r="A61" s="32"/>
-      <c r="B61" s="34"/>
+      <c r="A61" s="37"/>
+      <c r="B61" s="39"/>
       <c r="C61" s="26"/>
       <c r="D61" s="26"/>
     </row>
     <row r="62" spans="1:4">
-      <c r="A62" s="32"/>
-      <c r="B62" s="35"/>
+      <c r="A62" s="37"/>
+      <c r="B62" s="40"/>
       <c r="C62" s="26"/>
       <c r="D62" s="26"/>
     </row>
   </sheetData>
   <mergeCells count="35">
+    <mergeCell ref="A36:A38"/>
+    <mergeCell ref="B36:B38"/>
+    <mergeCell ref="A60:A62"/>
+    <mergeCell ref="B45:B47"/>
+    <mergeCell ref="B48:B50"/>
+    <mergeCell ref="B51:B53"/>
+    <mergeCell ref="B54:B56"/>
+    <mergeCell ref="B57:B59"/>
+    <mergeCell ref="B60:B62"/>
+    <mergeCell ref="A45:A47"/>
+    <mergeCell ref="A48:A50"/>
+    <mergeCell ref="A51:A53"/>
+    <mergeCell ref="A54:A56"/>
+    <mergeCell ref="A57:A59"/>
+    <mergeCell ref="B15:B17"/>
+    <mergeCell ref="A15:A17"/>
+    <mergeCell ref="B18:B20"/>
+    <mergeCell ref="A18:A20"/>
+    <mergeCell ref="A21:A23"/>
     <mergeCell ref="C46:C47"/>
     <mergeCell ref="C49:C50"/>
     <mergeCell ref="C51:C53"/>
@@ -3812,25 +3815,6 @@
     <mergeCell ref="B30:B32"/>
     <mergeCell ref="A33:A35"/>
     <mergeCell ref="B33:B35"/>
-    <mergeCell ref="B15:B17"/>
-    <mergeCell ref="A15:A17"/>
-    <mergeCell ref="B18:B20"/>
-    <mergeCell ref="A18:A20"/>
-    <mergeCell ref="A21:A23"/>
-    <mergeCell ref="A36:A38"/>
-    <mergeCell ref="B36:B38"/>
-    <mergeCell ref="A60:A62"/>
-    <mergeCell ref="B45:B47"/>
-    <mergeCell ref="B48:B50"/>
-    <mergeCell ref="B51:B53"/>
-    <mergeCell ref="B54:B56"/>
-    <mergeCell ref="B57:B59"/>
-    <mergeCell ref="B60:B62"/>
-    <mergeCell ref="A45:A47"/>
-    <mergeCell ref="A48:A50"/>
-    <mergeCell ref="A51:A53"/>
-    <mergeCell ref="A54:A56"/>
-    <mergeCell ref="A57:A59"/>
   </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3841,7 +3825,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{113AD7C8-E432-4900-8C71-627982E552B0}">
   <dimension ref="A1:D22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+    <sheetView topLeftCell="A16" workbookViewId="0">
       <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
@@ -3857,261 +3841,261 @@
         <v>1</v>
       </c>
       <c r="B1" s="11" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C1" s="11" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="D1" s="11" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="57.6" hidden="1">
       <c r="A2" s="12" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B2" s="23" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C2" s="21" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="D2" s="21" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="86.4" hidden="1">
       <c r="A3" s="12" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B3" s="22" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="C3" s="21" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="D3" s="21" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="72" hidden="1">
       <c r="A4" s="12" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="B4" s="22" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="C4" s="21" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="D4" s="21" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="28.8" hidden="1">
-      <c r="A5" s="32" t="s">
-        <v>50</v>
-      </c>
-      <c r="B5" s="33" t="s">
+      <c r="A5" s="37" t="s">
+        <v>47</v>
+      </c>
+      <c r="B5" s="38" t="s">
+        <v>252</v>
+      </c>
+      <c r="C5" s="24" t="s">
+        <v>253</v>
+      </c>
+      <c r="D5" s="24" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="28.8" hidden="1">
+      <c r="A6" s="37"/>
+      <c r="B6" s="39"/>
+      <c r="C6" s="24" t="s">
+        <v>254</v>
+      </c>
+      <c r="D6" s="24" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="43.2" hidden="1">
+      <c r="A7" s="37"/>
+      <c r="B7" s="40"/>
+      <c r="C7" s="24" t="s">
         <v>255</v>
       </c>
-      <c r="C5" s="24" t="s">
-        <v>256</v>
-      </c>
-      <c r="D5" s="24" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="28.8" hidden="1">
-      <c r="A6" s="32"/>
-      <c r="B6" s="34"/>
-      <c r="C6" s="24" t="s">
-        <v>257</v>
-      </c>
-      <c r="D6" s="24" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="43.2" hidden="1">
-      <c r="A7" s="32"/>
-      <c r="B7" s="35"/>
-      <c r="C7" s="24" t="s">
+      <c r="D7" s="24" t="s">
         <v>258</v>
       </c>
-      <c r="D7" s="24" t="s">
-        <v>261</v>
-      </c>
     </row>
     <row r="8" spans="1:4" ht="28.8" customHeight="1">
-      <c r="A8" s="32" t="s">
-        <v>337</v>
-      </c>
-      <c r="B8" s="33" t="s">
+      <c r="A8" s="37" t="s">
+        <v>334</v>
+      </c>
+      <c r="B8" s="38" t="s">
+        <v>299</v>
+      </c>
+      <c r="C8" s="24" t="s">
+        <v>300</v>
+      </c>
+      <c r="D8" s="24" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="28.8">
+      <c r="A9" s="37"/>
+      <c r="B9" s="39"/>
+      <c r="C9" s="24" t="s">
+        <v>301</v>
+      </c>
+      <c r="D9" s="24" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="28.8">
+      <c r="A10" s="37"/>
+      <c r="B10" s="40"/>
+      <c r="C10" s="24" t="s">
         <v>302</v>
       </c>
-      <c r="C8" s="24" t="s">
-        <v>303</v>
-      </c>
-      <c r="D8" s="24" t="s">
+      <c r="D10" s="24" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="14.4" customHeight="1">
+      <c r="A11" s="37" t="s">
+        <v>335</v>
+      </c>
+      <c r="B11" s="38" t="s">
         <v>306</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" ht="28.8">
-      <c r="A9" s="32"/>
-      <c r="B9" s="34"/>
-      <c r="C9" s="24" t="s">
-        <v>304</v>
-      </c>
-      <c r="D9" s="24" t="s">
+      <c r="C11" s="24" t="s">
         <v>307</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" ht="28.8">
-      <c r="A10" s="32"/>
-      <c r="B10" s="35"/>
-      <c r="C10" s="24" t="s">
-        <v>305</v>
-      </c>
-      <c r="D10" s="24" t="s">
+      <c r="D11" s="24" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="37.200000000000003" customHeight="1">
+      <c r="A12" s="37"/>
+      <c r="B12" s="39"/>
+      <c r="C12" s="24" t="s">
         <v>308</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" ht="14.4" customHeight="1">
-      <c r="A11" s="32" t="s">
-        <v>338</v>
-      </c>
-      <c r="B11" s="33" t="s">
+      <c r="D12" s="24" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="26.4" customHeight="1">
+      <c r="A13" s="37"/>
+      <c r="B13" s="40"/>
+      <c r="C13" s="24" t="s">
         <v>309</v>
       </c>
-      <c r="C11" s="24" t="s">
-        <v>310</v>
-      </c>
-      <c r="D11" s="24" t="s">
-        <v>313</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" ht="37.200000000000003" customHeight="1">
-      <c r="A12" s="32"/>
-      <c r="B12" s="34"/>
-      <c r="C12" s="24" t="s">
-        <v>311</v>
-      </c>
-      <c r="D12" s="24" t="s">
-        <v>314</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" ht="26.4" customHeight="1">
-      <c r="A13" s="32"/>
-      <c r="B13" s="35"/>
-      <c r="C13" s="24" t="s">
+      <c r="D13" s="24" t="s">
         <v>312</v>
       </c>
-      <c r="D13" s="24" t="s">
-        <v>315</v>
-      </c>
     </row>
     <row r="14" spans="1:4" ht="43.2">
-      <c r="A14" s="32" t="s">
-        <v>345</v>
-      </c>
-      <c r="B14" s="33" t="s">
-        <v>350</v>
+      <c r="A14" s="37" t="s">
+        <v>342</v>
+      </c>
+      <c r="B14" s="38" t="s">
+        <v>347</v>
       </c>
       <c r="C14" s="24" t="s">
+        <v>363</v>
+      </c>
+      <c r="D14" s="24" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="43.2">
+      <c r="A15" s="37"/>
+      <c r="B15" s="39"/>
+      <c r="C15" s="24" t="s">
+        <v>365</v>
+      </c>
+      <c r="D15" s="24" t="s">
         <v>366</v>
       </c>
-      <c r="D14" s="24" t="s">
+    </row>
+    <row r="16" spans="1:4" ht="43.2">
+      <c r="A16" s="37"/>
+      <c r="B16" s="40"/>
+      <c r="C16" s="24" t="s">
         <v>367</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" ht="43.2">
-      <c r="A15" s="32"/>
-      <c r="B15" s="34"/>
-      <c r="C15" s="24" t="s">
+      <c r="D16" s="24" t="s">
         <v>368</v>
       </c>
-      <c r="D15" s="24" t="s">
-        <v>369</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" ht="43.2">
-      <c r="A16" s="32"/>
-      <c r="B16" s="35"/>
-      <c r="C16" s="24" t="s">
-        <v>370</v>
-      </c>
-      <c r="D16" s="24" t="s">
-        <v>371</v>
-      </c>
     </row>
     <row r="17" spans="1:4" ht="57.6">
-      <c r="A17" s="32" t="s">
-        <v>378</v>
-      </c>
-      <c r="B17" s="33" t="s">
+      <c r="A17" s="37" t="s">
+        <v>375</v>
+      </c>
+      <c r="B17" s="38" t="s">
+        <v>388</v>
+      </c>
+      <c r="C17" s="24" t="s">
+        <v>389</v>
+      </c>
+      <c r="D17" s="24" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="72">
+      <c r="A18" s="37"/>
+      <c r="B18" s="39"/>
+      <c r="C18" s="24" t="s">
+        <v>390</v>
+      </c>
+      <c r="D18" s="24" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="31.2" customHeight="1">
+      <c r="A19" s="37"/>
+      <c r="B19" s="40"/>
+      <c r="C19" s="24" t="s">
         <v>391</v>
       </c>
-      <c r="C17" s="24" t="s">
+      <c r="D19" s="24" t="s">
         <v>392</v>
       </c>
-      <c r="D17" s="24" t="s">
-        <v>397</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" ht="72">
-      <c r="A18" s="32"/>
-      <c r="B18" s="34"/>
-      <c r="C18" s="24" t="s">
-        <v>393</v>
-      </c>
-      <c r="D18" s="24" t="s">
-        <v>396</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" ht="31.2" customHeight="1">
-      <c r="A19" s="32"/>
-      <c r="B19" s="35"/>
-      <c r="C19" s="24" t="s">
-        <v>394</v>
-      </c>
-      <c r="D19" s="24" t="s">
-        <v>395</v>
-      </c>
     </row>
     <row r="20" spans="1:4">
-      <c r="A20" s="32" t="s">
-        <v>390</v>
-      </c>
-      <c r="B20" s="33"/>
+      <c r="A20" s="37" t="s">
+        <v>387</v>
+      </c>
+      <c r="B20" s="38"/>
       <c r="C20" s="24"/>
       <c r="D20" s="24"/>
     </row>
     <row r="21" spans="1:4">
-      <c r="A21" s="32"/>
-      <c r="B21" s="34"/>
+      <c r="A21" s="37"/>
+      <c r="B21" s="39"/>
       <c r="C21" s="24"/>
       <c r="D21" s="24"/>
     </row>
     <row r="22" spans="1:4">
-      <c r="A22" s="32"/>
-      <c r="B22" s="35"/>
+      <c r="A22" s="37"/>
+      <c r="B22" s="40"/>
       <c r="C22" s="24"/>
       <c r="D22" s="24"/>
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A11:A13"/>
+    <mergeCell ref="B11:B13"/>
+    <mergeCell ref="A5:A7"/>
+    <mergeCell ref="B5:B7"/>
+    <mergeCell ref="A8:A10"/>
+    <mergeCell ref="B8:B10"/>
     <mergeCell ref="A17:A19"/>
     <mergeCell ref="B17:B19"/>
     <mergeCell ref="A20:A22"/>
     <mergeCell ref="B20:B22"/>
     <mergeCell ref="A14:A16"/>
     <mergeCell ref="B14:B16"/>
-    <mergeCell ref="A11:A13"/>
-    <mergeCell ref="B11:B13"/>
-    <mergeCell ref="A5:A7"/>
-    <mergeCell ref="B5:B7"/>
-    <mergeCell ref="A8:A10"/>
-    <mergeCell ref="B8:B10"/>
   </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4130,12 +4114,12 @@
   <sheetData>
     <row r="2" spans="2:2">
       <c r="B2" s="13" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
     </row>
     <row r="4" spans="2:2" ht="18">
       <c r="B4" s="14" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
     </row>
     <row r="5" spans="2:2">
@@ -4143,27 +4127,27 @@
     </row>
     <row r="6" spans="2:2">
       <c r="B6" s="15" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
     </row>
     <row r="7" spans="2:2">
       <c r="B7" s="15" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
     </row>
     <row r="8" spans="2:2">
       <c r="B8" s="15" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
     </row>
     <row r="9" spans="2:2">
       <c r="B9" s="15" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
     </row>
     <row r="11" spans="2:2">
       <c r="B11" s="13" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
     </row>
     <row r="12" spans="2:2">
@@ -4171,17 +4155,17 @@
     </row>
     <row r="13" spans="2:2">
       <c r="B13" s="15" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
     </row>
     <row r="14" spans="2:2">
       <c r="B14" s="15" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
     </row>
     <row r="18" spans="2:2" ht="18">
       <c r="B18" s="14" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
     </row>
     <row r="19" spans="2:2">
@@ -4189,22 +4173,22 @@
     </row>
     <row r="20" spans="2:2">
       <c r="B20" s="15" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="21" spans="2:2">
       <c r="B21" s="15" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
     </row>
     <row r="22" spans="2:2">
       <c r="B22" s="15" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
     </row>
     <row r="24" spans="2:2">
       <c r="B24" s="13" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
     </row>
     <row r="25" spans="2:2">
@@ -4212,17 +4196,17 @@
     </row>
     <row r="26" spans="2:2">
       <c r="B26" s="15" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
     </row>
     <row r="27" spans="2:2">
       <c r="B27" s="15" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
     </row>
     <row r="31" spans="2:2" ht="18">
       <c r="B31" s="14" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
     </row>
     <row r="32" spans="2:2">
@@ -4230,22 +4214,22 @@
     </row>
     <row r="33" spans="2:2">
       <c r="B33" s="15" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="34" spans="2:2">
       <c r="B34" s="15" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
     </row>
     <row r="35" spans="2:2">
       <c r="B35" s="15" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
     </row>
     <row r="37" spans="2:2">
       <c r="B37" s="13" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
     </row>
     <row r="38" spans="2:2">
@@ -4253,17 +4237,17 @@
     </row>
     <row r="39" spans="2:2">
       <c r="B39" s="15" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
     </row>
     <row r="40" spans="2:2">
       <c r="B40" s="15" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
     </row>
     <row r="44" spans="2:2" ht="18">
       <c r="B44" s="14" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
     </row>
     <row r="45" spans="2:2">
@@ -4271,22 +4255,22 @@
     </row>
     <row r="46" spans="2:2">
       <c r="B46" s="15" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
     </row>
     <row r="47" spans="2:2">
       <c r="B47" s="15" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
     </row>
     <row r="48" spans="2:2">
       <c r="B48" s="15" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
     </row>
     <row r="50" spans="2:2">
       <c r="B50" s="13" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
     </row>
     <row r="51" spans="2:2">
@@ -4294,17 +4278,17 @@
     </row>
     <row r="52" spans="2:2">
       <c r="B52" s="15" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
     </row>
     <row r="53" spans="2:2">
       <c r="B53" s="15" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
     </row>
     <row r="57" spans="2:2" ht="18">
       <c r="B57" s="14" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
     </row>
     <row r="58" spans="2:2">
@@ -4312,22 +4296,22 @@
     </row>
     <row r="59" spans="2:2">
       <c r="B59" s="15" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
     </row>
     <row r="60" spans="2:2">
       <c r="B60" s="15" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="61" spans="2:2">
       <c r="B61" s="15" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
     </row>
     <row r="63" spans="2:2">
       <c r="B63" s="13" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
     </row>
     <row r="64" spans="2:2">
@@ -4335,17 +4319,17 @@
     </row>
     <row r="65" spans="2:2">
       <c r="B65" s="15" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
     </row>
     <row r="66" spans="2:2">
       <c r="B66" s="15" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
     </row>
     <row r="70" spans="2:2" ht="18">
       <c r="B70" s="14" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
     </row>
     <row r="71" spans="2:2">
@@ -4353,22 +4337,22 @@
     </row>
     <row r="72" spans="2:2">
       <c r="B72" s="15" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
     </row>
     <row r="73" spans="2:2">
       <c r="B73" s="15" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
     </row>
     <row r="74" spans="2:2">
       <c r="B74" s="15" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
     </row>
     <row r="76" spans="2:2">
       <c r="B76" s="13" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
     </row>
     <row r="77" spans="2:2">
@@ -4376,17 +4360,17 @@
     </row>
     <row r="78" spans="2:2">
       <c r="B78" s="15" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
     </row>
     <row r="79" spans="2:2">
       <c r="B79" s="15" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
     </row>
     <row r="83" spans="2:2" ht="18">
       <c r="B83" s="14" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
     </row>
     <row r="84" spans="2:2">
@@ -4394,17 +4378,17 @@
     </row>
     <row r="85" spans="2:2">
       <c r="B85" s="15" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
     </row>
     <row r="86" spans="2:2">
       <c r="B86" s="15" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
     </row>
     <row r="88" spans="2:2">
       <c r="B88" s="13" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
     </row>
     <row r="89" spans="2:2">
@@ -4412,17 +4396,17 @@
     </row>
     <row r="90" spans="2:2">
       <c r="B90" s="15" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
     </row>
     <row r="91" spans="2:2">
       <c r="B91" s="15" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
     </row>
     <row r="95" spans="2:2" ht="18">
       <c r="B95" s="14" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
     </row>
     <row r="96" spans="2:2">
@@ -4430,17 +4414,17 @@
     </row>
     <row r="97" spans="2:2">
       <c r="B97" s="15" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="98" spans="2:2">
       <c r="B98" s="15" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
     </row>
     <row r="100" spans="2:2">
       <c r="B100" s="13" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
     </row>
     <row r="101" spans="2:2">
@@ -4448,17 +4432,17 @@
     </row>
     <row r="102" spans="2:2">
       <c r="B102" s="15" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
     </row>
     <row r="103" spans="2:2">
       <c r="B103" s="15" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="107" spans="2:2" ht="18">
       <c r="B107" s="14" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
     </row>
     <row r="108" spans="2:2">
@@ -4466,17 +4450,17 @@
     </row>
     <row r="109" spans="2:2">
       <c r="B109" s="15" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
     </row>
     <row r="110" spans="2:2">
       <c r="B110" s="15" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
     </row>
     <row r="112" spans="2:2">
       <c r="B112" s="13" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
     </row>
     <row r="113" spans="2:2">
@@ -4484,17 +4468,17 @@
     </row>
     <row r="114" spans="2:2">
       <c r="B114" s="15" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
     </row>
     <row r="115" spans="2:2">
       <c r="B115" s="15" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
     </row>
     <row r="119" spans="2:2" ht="18">
       <c r="B119" s="14" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
     </row>
     <row r="120" spans="2:2">
@@ -4502,17 +4486,17 @@
     </row>
     <row r="121" spans="2:2">
       <c r="B121" s="15" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
     </row>
     <row r="122" spans="2:2">
       <c r="B122" s="15" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
     </row>
     <row r="124" spans="2:2">
       <c r="B124" s="13" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
     </row>
     <row r="125" spans="2:2">
@@ -4520,17 +4504,17 @@
     </row>
     <row r="126" spans="2:2">
       <c r="B126" s="15" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
     </row>
     <row r="127" spans="2:2">
       <c r="B127" s="15" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
     </row>
     <row r="131" spans="2:2" ht="18">
       <c r="B131" s="14" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
     </row>
     <row r="132" spans="2:2">
@@ -4538,17 +4522,17 @@
     </row>
     <row r="133" spans="2:2">
       <c r="B133" s="15" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
     </row>
     <row r="134" spans="2:2">
       <c r="B134" s="15" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
     </row>
     <row r="136" spans="2:2">
       <c r="B136" s="13" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
     </row>
     <row r="137" spans="2:2">
@@ -4556,17 +4540,17 @@
     </row>
     <row r="138" spans="2:2">
       <c r="B138" s="15" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
     </row>
     <row r="139" spans="2:2">
       <c r="B139" s="15" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
     </row>
     <row r="143" spans="2:2" ht="18">
       <c r="B143" s="14" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
     </row>
     <row r="144" spans="2:2">
@@ -4574,17 +4558,17 @@
     </row>
     <row r="145" spans="2:2">
       <c r="B145" s="15" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
     </row>
     <row r="146" spans="2:2">
       <c r="B146" s="15" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
     </row>
     <row r="148" spans="2:2">
       <c r="B148" s="13" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
     </row>
     <row r="149" spans="2:2">
@@ -4592,12 +4576,12 @@
     </row>
     <row r="150" spans="2:2">
       <c r="B150" s="15" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
     </row>
     <row r="151" spans="2:2">
       <c r="B151" s="15" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
     </row>
   </sheetData>
@@ -4621,18 +4605,18 @@
   <sheetData>
     <row r="2" spans="2:3" ht="39" customHeight="1">
       <c r="B2" s="16" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="C2" s="16" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
     </row>
     <row r="3" spans="2:3">
       <c r="B3" s="17" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="C3" s="18" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
     </row>
     <row r="4" spans="2:3">
@@ -4640,51 +4624,51 @@
         <v>1</v>
       </c>
       <c r="C4" s="18" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
     </row>
     <row r="5" spans="2:3">
       <c r="B5" s="17" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="C5" s="18" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
     </row>
     <row r="6" spans="2:3">
       <c r="B6" s="17" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C6" s="18" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
     </row>
     <row r="7" spans="2:3">
       <c r="B7" s="17" t="s">
+        <v>131</v>
+      </c>
+      <c r="C7" s="18" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="8" spans="2:3">
+      <c r="B8" s="42" t="s">
+        <v>137</v>
+      </c>
+      <c r="C8" s="18" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="9" spans="2:3">
+      <c r="B9" s="43"/>
+      <c r="C9" s="18" t="s">
         <v>134</v>
       </c>
-      <c r="C7" s="18" t="s">
+    </row>
+    <row r="10" spans="2:3">
+      <c r="B10" s="44"/>
+      <c r="C10" s="18" t="s">
         <v>135</v>
-      </c>
-    </row>
-    <row r="8" spans="2:3">
-      <c r="B8" s="41" t="s">
-        <v>140</v>
-      </c>
-      <c r="C8" s="18" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="9" spans="2:3">
-      <c r="B9" s="42"/>
-      <c r="C9" s="18" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="10" spans="2:3">
-      <c r="B10" s="43"/>
-      <c r="C10" s="18" t="s">
-        <v>138</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Sprint 12 - archivos nuevos
</commit_message>
<xml_diff>
--- a/Documentos/ProductBacklogCorregido.xlsx
+++ b/Documentos/ProductBacklogCorregido.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://liveespochedu-my.sharepoint.com/personal/jonathan_aucancela_espoch_edu_ec/Documents/Documentos/Espoch/Octavo/Aplicaciones informáticas 2/SGT/Documentos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="6_{03CBC970-F92A-40AE-9A66-0714A992D452}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="14" documentId="6_{03CBC970-F92A-40AE-9A66-0714A992D452}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7E325069-C6F7-41CD-ACCA-72D3B3F81A98}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{7A8F741B-9112-4896-B995-875A9BDE94F9}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="505" uniqueCount="398">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="514" uniqueCount="407">
   <si>
     <t>Product Backlog - SecuraBank</t>
   </si>
@@ -1376,6 +1376,33 @@
   </si>
   <si>
     <t xml:space="preserve">Despligue del proyecto SGT en un servidor free. Apache y Gunicorn </t>
+  </si>
+  <si>
+    <t>HT34</t>
+  </si>
+  <si>
+    <t>HT35</t>
+  </si>
+  <si>
+    <t>HT36</t>
+  </si>
+  <si>
+    <t>29 de enero de 2025</t>
+  </si>
+  <si>
+    <t>31 de enero de 2025</t>
+  </si>
+  <si>
+    <t>2 de febrero de 2025</t>
+  </si>
+  <si>
+    <t>3 de febrero de 2025</t>
+  </si>
+  <si>
+    <t>4 de febrero de 2025</t>
+  </si>
+  <si>
+    <t>1 de febrero de 2025</t>
   </si>
 </sst>
 </file>
@@ -1723,18 +1750,6 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1749,6 +1764,18 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2100,8 +2127,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83A87B21-3BDC-40F9-B20F-2399C52423D9}">
   <dimension ref="A1:K44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A35" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D39" sqref="D39"/>
+    <sheetView tabSelected="1" topLeftCell="A33" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K38" sqref="K38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
@@ -2916,7 +2943,7 @@
         <v>8</v>
       </c>
       <c r="F38" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G38" s="2" t="s">
         <v>370</v>
@@ -2939,8 +2966,12 @@
       <c r="E39" s="2">
         <v>8</v>
       </c>
-      <c r="F39" s="2"/>
-      <c r="G39" s="2"/>
+      <c r="F39" s="2">
+        <v>2</v>
+      </c>
+      <c r="G39" s="2" t="s">
+        <v>401</v>
+      </c>
     </row>
     <row r="40" spans="1:11" ht="43.2">
       <c r="A40" s="30"/>
@@ -2956,16 +2987,20 @@
       <c r="E40" s="2">
         <v>8</v>
       </c>
-      <c r="F40" s="2"/>
-      <c r="G40" s="2"/>
-    </row>
-    <row r="41" spans="1:11">
+      <c r="F40" s="2">
+        <v>2</v>
+      </c>
+      <c r="G40" s="2" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" ht="22.8" customHeight="1">
       <c r="A41" s="31"/>
       <c r="B41" s="2" t="s">
         <v>346</v>
       </c>
-      <c r="C41" s="10" t="s">
-        <v>5</v>
+      <c r="C41" s="9" t="s">
+        <v>21</v>
       </c>
       <c r="D41" s="1" t="s">
         <v>396</v>
@@ -2973,14 +3008,20 @@
       <c r="E41" s="2">
         <v>8</v>
       </c>
-      <c r="F41" s="2"/>
-      <c r="G41" s="2"/>
+      <c r="F41" s="2">
+        <v>2</v>
+      </c>
+      <c r="G41" s="2" t="s">
+        <v>406</v>
+      </c>
     </row>
     <row r="42" spans="1:11" ht="28.8">
       <c r="A42" s="29" t="s">
         <v>341</v>
       </c>
-      <c r="B42" s="2"/>
+      <c r="B42" s="2" t="s">
+        <v>398</v>
+      </c>
       <c r="C42" s="10" t="s">
         <v>5</v>
       </c>
@@ -2990,12 +3031,18 @@
       <c r="E42" s="2">
         <v>8</v>
       </c>
-      <c r="F42" s="2"/>
-      <c r="G42" s="2"/>
+      <c r="F42" s="2">
+        <v>1</v>
+      </c>
+      <c r="G42" s="2" t="s">
+        <v>403</v>
+      </c>
     </row>
     <row r="43" spans="1:11" ht="43.2">
       <c r="A43" s="30"/>
-      <c r="B43" s="2"/>
+      <c r="B43" s="2" t="s">
+        <v>399</v>
+      </c>
       <c r="C43" s="10" t="s">
         <v>5</v>
       </c>
@@ -3005,12 +3052,18 @@
       <c r="E43" s="2">
         <v>8</v>
       </c>
-      <c r="F43" s="2"/>
-      <c r="G43" s="2"/>
+      <c r="F43" s="2">
+        <v>1</v>
+      </c>
+      <c r="G43" s="2" t="s">
+        <v>404</v>
+      </c>
     </row>
     <row r="44" spans="1:11" ht="28.8">
       <c r="A44" s="31"/>
-      <c r="B44" s="2"/>
+      <c r="B44" s="2" t="s">
+        <v>400</v>
+      </c>
       <c r="C44" s="10" t="s">
         <v>5</v>
       </c>
@@ -3020,11 +3073,20 @@
       <c r="E44" s="2">
         <v>8</v>
       </c>
-      <c r="F44" s="2"/>
-      <c r="G44" s="2"/>
+      <c r="F44" s="2">
+        <v>2</v>
+      </c>
+      <c r="G44" s="2" t="s">
+        <v>405</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A39:A41"/>
+    <mergeCell ref="A42:A44"/>
+    <mergeCell ref="A32:A35"/>
+    <mergeCell ref="A29:A31"/>
+    <mergeCell ref="A36:A38"/>
     <mergeCell ref="A26:A28"/>
     <mergeCell ref="A23:A25"/>
     <mergeCell ref="A16:A18"/>
@@ -3032,11 +3094,6 @@
     <mergeCell ref="A8:A12"/>
     <mergeCell ref="A13:A15"/>
     <mergeCell ref="A19:A22"/>
-    <mergeCell ref="A39:A41"/>
-    <mergeCell ref="A42:A44"/>
-    <mergeCell ref="A32:A35"/>
-    <mergeCell ref="A29:A31"/>
-    <mergeCell ref="A36:A38"/>
   </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3048,7 +3105,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68EE2C79-A7B0-4BE1-9026-6C6F59ABCFC9}">
   <dimension ref="A1:D62"/>
   <sheetViews>
-    <sheetView topLeftCell="A50" workbookViewId="0">
+    <sheetView topLeftCell="A57" workbookViewId="0">
       <selection activeCell="H56" sqref="H56"/>
     </sheetView>
   </sheetViews>
@@ -3257,10 +3314,10 @@
       </c>
     </row>
     <row r="15" spans="1:4" ht="28.8" hidden="1">
-      <c r="A15" s="37" t="s">
+      <c r="A15" s="33" t="s">
         <v>201</v>
       </c>
-      <c r="B15" s="38" t="s">
+      <c r="B15" s="34" t="s">
         <v>217</v>
       </c>
       <c r="C15" s="25" t="s">
@@ -3271,8 +3328,8 @@
       </c>
     </row>
     <row r="16" spans="1:4" ht="28.8" hidden="1">
-      <c r="A16" s="37"/>
-      <c r="B16" s="39"/>
+      <c r="A16" s="33"/>
+      <c r="B16" s="35"/>
       <c r="C16" s="25" t="s">
         <v>219</v>
       </c>
@@ -3281,8 +3338,8 @@
       </c>
     </row>
     <row r="17" spans="1:4" ht="28.8" hidden="1">
-      <c r="A17" s="37"/>
-      <c r="B17" s="40"/>
+      <c r="A17" s="33"/>
+      <c r="B17" s="36"/>
       <c r="C17" s="25" t="s">
         <v>220</v>
       </c>
@@ -3291,10 +3348,10 @@
       </c>
     </row>
     <row r="18" spans="1:4" ht="43.2" hidden="1">
-      <c r="A18" s="37" t="s">
+      <c r="A18" s="33" t="s">
         <v>202</v>
       </c>
-      <c r="B18" s="38" t="s">
+      <c r="B18" s="34" t="s">
         <v>224</v>
       </c>
       <c r="C18" s="25" t="s">
@@ -3305,8 +3362,8 @@
       </c>
     </row>
     <row r="19" spans="1:4" ht="28.8" hidden="1">
-      <c r="A19" s="37"/>
-      <c r="B19" s="39"/>
+      <c r="A19" s="33"/>
+      <c r="B19" s="35"/>
       <c r="C19" s="25" t="s">
         <v>226</v>
       </c>
@@ -3315,8 +3372,8 @@
       </c>
     </row>
     <row r="20" spans="1:4" ht="28.8" hidden="1">
-      <c r="A20" s="37"/>
-      <c r="B20" s="40"/>
+      <c r="A20" s="33"/>
+      <c r="B20" s="36"/>
       <c r="C20" s="25" t="s">
         <v>227</v>
       </c>
@@ -3325,10 +3382,10 @@
       </c>
     </row>
     <row r="21" spans="1:4" ht="28.8" hidden="1">
-      <c r="A21" s="37" t="s">
+      <c r="A21" s="33" t="s">
         <v>203</v>
       </c>
-      <c r="B21" s="38" t="s">
+      <c r="B21" s="34" t="s">
         <v>237</v>
       </c>
       <c r="C21" s="21" t="s">
@@ -3339,8 +3396,8 @@
       </c>
     </row>
     <row r="22" spans="1:4" ht="28.8" hidden="1">
-      <c r="A22" s="37"/>
-      <c r="B22" s="39"/>
+      <c r="A22" s="33"/>
+      <c r="B22" s="35"/>
       <c r="C22" s="21" t="s">
         <v>232</v>
       </c>
@@ -3349,8 +3406,8 @@
       </c>
     </row>
     <row r="23" spans="1:4" ht="28.8" hidden="1">
-      <c r="A23" s="37"/>
-      <c r="B23" s="40"/>
+      <c r="A23" s="33"/>
+      <c r="B23" s="36"/>
       <c r="C23" s="21" t="s">
         <v>233</v>
       </c>
@@ -3359,10 +3416,10 @@
       </c>
     </row>
     <row r="24" spans="1:4" ht="28.8" hidden="1">
-      <c r="A24" s="37" t="s">
+      <c r="A24" s="33" t="s">
         <v>208</v>
       </c>
-      <c r="B24" s="38" t="s">
+      <c r="B24" s="34" t="s">
         <v>238</v>
       </c>
       <c r="C24" s="24" t="s">
@@ -3373,8 +3430,8 @@
       </c>
     </row>
     <row r="25" spans="1:4" ht="28.8" hidden="1">
-      <c r="A25" s="37"/>
-      <c r="B25" s="39"/>
+      <c r="A25" s="33"/>
+      <c r="B25" s="35"/>
       <c r="C25" s="24" t="s">
         <v>240</v>
       </c>
@@ -3383,8 +3440,8 @@
       </c>
     </row>
     <row r="26" spans="1:4" ht="28.8" hidden="1">
-      <c r="A26" s="37"/>
-      <c r="B26" s="40"/>
+      <c r="A26" s="33"/>
+      <c r="B26" s="36"/>
       <c r="C26" s="24" t="s">
         <v>241</v>
       </c>
@@ -3393,10 +3450,10 @@
       </c>
     </row>
     <row r="27" spans="1:4" ht="28.8" hidden="1">
-      <c r="A27" s="37" t="s">
+      <c r="A27" s="33" t="s">
         <v>210</v>
       </c>
-      <c r="B27" s="38" t="s">
+      <c r="B27" s="34" t="s">
         <v>245</v>
       </c>
       <c r="C27" s="24" t="s">
@@ -3407,8 +3464,8 @@
       </c>
     </row>
     <row r="28" spans="1:4" ht="28.8" hidden="1">
-      <c r="A28" s="37"/>
-      <c r="B28" s="39"/>
+      <c r="A28" s="33"/>
+      <c r="B28" s="35"/>
       <c r="C28" s="24" t="s">
         <v>247</v>
       </c>
@@ -3417,8 +3474,8 @@
       </c>
     </row>
     <row r="29" spans="1:4" ht="28.8" hidden="1">
-      <c r="A29" s="37"/>
-      <c r="B29" s="40"/>
+      <c r="A29" s="33"/>
+      <c r="B29" s="36"/>
       <c r="C29" s="24" t="s">
         <v>248</v>
       </c>
@@ -3427,10 +3484,10 @@
       </c>
     </row>
     <row r="30" spans="1:4" ht="14.4" hidden="1" customHeight="1">
-      <c r="A30" s="37" t="s">
+      <c r="A30" s="33" t="s">
         <v>211</v>
       </c>
-      <c r="B30" s="38" t="s">
+      <c r="B30" s="34" t="s">
         <v>262</v>
       </c>
       <c r="C30" s="24" t="s">
@@ -3441,8 +3498,8 @@
       </c>
     </row>
     <row r="31" spans="1:4" ht="33" hidden="1" customHeight="1">
-      <c r="A31" s="37"/>
-      <c r="B31" s="39"/>
+      <c r="A31" s="33"/>
+      <c r="B31" s="35"/>
       <c r="C31" s="24" t="s">
         <v>280</v>
       </c>
@@ -3451,8 +3508,8 @@
       </c>
     </row>
     <row r="32" spans="1:4" ht="24" hidden="1" customHeight="1">
-      <c r="A32" s="37"/>
-      <c r="B32" s="40"/>
+      <c r="A32" s="33"/>
+      <c r="B32" s="36"/>
       <c r="C32" s="24" t="s">
         <v>281</v>
       </c>
@@ -3461,10 +3518,10 @@
       </c>
     </row>
     <row r="33" spans="1:4" ht="36.6" hidden="1" customHeight="1">
-      <c r="A33" s="37" t="s">
+      <c r="A33" s="33" t="s">
         <v>259</v>
       </c>
-      <c r="B33" s="38" t="s">
+      <c r="B33" s="34" t="s">
         <v>285</v>
       </c>
       <c r="C33" s="24" t="s">
@@ -3475,8 +3532,8 @@
       </c>
     </row>
     <row r="34" spans="1:4" ht="26.4" hidden="1" customHeight="1">
-      <c r="A34" s="37"/>
-      <c r="B34" s="39"/>
+      <c r="A34" s="33"/>
+      <c r="B34" s="35"/>
       <c r="C34" s="24" t="s">
         <v>287</v>
       </c>
@@ -3485,8 +3542,8 @@
       </c>
     </row>
     <row r="35" spans="1:4" ht="24" hidden="1" customHeight="1">
-      <c r="A35" s="37"/>
-      <c r="B35" s="40"/>
+      <c r="A35" s="33"/>
+      <c r="B35" s="36"/>
       <c r="C35" s="24" t="s">
         <v>288</v>
       </c>
@@ -3495,10 +3552,10 @@
       </c>
     </row>
     <row r="36" spans="1:4" ht="36.6" hidden="1" customHeight="1">
-      <c r="A36" s="37" t="s">
+      <c r="A36" s="33" t="s">
         <v>260</v>
       </c>
-      <c r="B36" s="38" t="s">
+      <c r="B36" s="34" t="s">
         <v>292</v>
       </c>
       <c r="C36" s="21" t="s">
@@ -3509,8 +3566,8 @@
       </c>
     </row>
     <row r="37" spans="1:4" ht="34.200000000000003" hidden="1" customHeight="1">
-      <c r="A37" s="37"/>
-      <c r="B37" s="39"/>
+      <c r="A37" s="33"/>
+      <c r="B37" s="35"/>
       <c r="C37" s="21" t="s">
         <v>294</v>
       </c>
@@ -3519,8 +3576,8 @@
       </c>
     </row>
     <row r="38" spans="1:4" ht="30" hidden="1" customHeight="1">
-      <c r="A38" s="37"/>
-      <c r="B38" s="40"/>
+      <c r="A38" s="33"/>
+      <c r="B38" s="36"/>
       <c r="C38" s="21" t="s">
         <v>295</v>
       </c>
@@ -3529,10 +3586,10 @@
       </c>
     </row>
     <row r="39" spans="1:4" ht="61.2" hidden="1" customHeight="1">
-      <c r="A39" s="37" t="s">
+      <c r="A39" s="33" t="s">
         <v>261</v>
       </c>
-      <c r="B39" s="41" t="s">
+      <c r="B39" s="37" t="s">
         <v>313</v>
       </c>
       <c r="C39" s="21" t="s">
@@ -3543,8 +3600,8 @@
       </c>
     </row>
     <row r="40" spans="1:4" ht="23.4" hidden="1" customHeight="1">
-      <c r="A40" s="37"/>
-      <c r="B40" s="41"/>
+      <c r="A40" s="33"/>
+      <c r="B40" s="37"/>
       <c r="C40" s="27" t="s">
         <v>316</v>
       </c>
@@ -3553,8 +3610,8 @@
       </c>
     </row>
     <row r="41" spans="1:4" ht="25.2" hidden="1" customHeight="1">
-      <c r="A41" s="37"/>
-      <c r="B41" s="41"/>
+      <c r="A41" s="33"/>
+      <c r="B41" s="37"/>
       <c r="C41" s="27" t="s">
         <v>319</v>
       </c>
@@ -3563,10 +3620,10 @@
       </c>
     </row>
     <row r="42" spans="1:4" ht="43.2" hidden="1" customHeight="1">
-      <c r="A42" s="37" t="s">
+      <c r="A42" s="33" t="s">
         <v>263</v>
       </c>
-      <c r="B42" s="41" t="s">
+      <c r="B42" s="37" t="s">
         <v>314</v>
       </c>
       <c r="C42" s="21" t="s">
@@ -3577,8 +3634,8 @@
       </c>
     </row>
     <row r="43" spans="1:4" ht="28.8" hidden="1">
-      <c r="A43" s="37"/>
-      <c r="B43" s="41"/>
+      <c r="A43" s="33"/>
+      <c r="B43" s="37"/>
       <c r="C43" s="21" t="s">
         <v>323</v>
       </c>
@@ -3587,8 +3644,8 @@
       </c>
     </row>
     <row r="44" spans="1:4" ht="28.8" hidden="1">
-      <c r="A44" s="37"/>
-      <c r="B44" s="41"/>
+      <c r="A44" s="33"/>
+      <c r="B44" s="37"/>
       <c r="C44" s="21" t="s">
         <v>324</v>
       </c>
@@ -3597,10 +3654,10 @@
       </c>
     </row>
     <row r="45" spans="1:4" ht="43.2" hidden="1" customHeight="1">
-      <c r="A45" s="37" t="s">
+      <c r="A45" s="33" t="s">
         <v>328</v>
       </c>
-      <c r="B45" s="41" t="s">
+      <c r="B45" s="37" t="s">
         <v>268</v>
       </c>
       <c r="C45" s="24" t="s">
@@ -3611,9 +3668,9 @@
       </c>
     </row>
     <row r="46" spans="1:4" ht="28.8" hidden="1" customHeight="1">
-      <c r="A46" s="37"/>
-      <c r="B46" s="41"/>
-      <c r="C46" s="33" t="s">
+      <c r="A46" s="33"/>
+      <c r="B46" s="37"/>
+      <c r="C46" s="38" t="s">
         <v>350</v>
       </c>
       <c r="D46" s="24" t="s">
@@ -3621,18 +3678,18 @@
       </c>
     </row>
     <row r="47" spans="1:4" ht="28.8" hidden="1">
-      <c r="A47" s="37"/>
-      <c r="B47" s="41"/>
-      <c r="C47" s="33"/>
+      <c r="A47" s="33"/>
+      <c r="B47" s="37"/>
+      <c r="C47" s="38"/>
       <c r="D47" s="24" t="s">
         <v>353</v>
       </c>
     </row>
     <row r="48" spans="1:4" ht="30.6" customHeight="1">
-      <c r="A48" s="37" t="s">
+      <c r="A48" s="33" t="s">
         <v>329</v>
       </c>
-      <c r="B48" s="41" t="s">
+      <c r="B48" s="37" t="s">
         <v>339</v>
       </c>
       <c r="C48" s="24" t="s">
@@ -3643,9 +3700,9 @@
       </c>
     </row>
     <row r="49" spans="1:4" ht="33.6" customHeight="1">
-      <c r="A49" s="37"/>
-      <c r="B49" s="41"/>
-      <c r="C49" s="33" t="s">
+      <c r="A49" s="33"/>
+      <c r="B49" s="37"/>
+      <c r="C49" s="38" t="s">
         <v>355</v>
       </c>
       <c r="D49" s="24" t="s">
@@ -3653,21 +3710,21 @@
       </c>
     </row>
     <row r="50" spans="1:4" ht="43.2">
-      <c r="A50" s="37"/>
-      <c r="B50" s="41"/>
-      <c r="C50" s="33"/>
+      <c r="A50" s="33"/>
+      <c r="B50" s="37"/>
+      <c r="C50" s="38"/>
       <c r="D50" s="24" t="s">
         <v>358</v>
       </c>
     </row>
     <row r="51" spans="1:4" ht="43.2">
-      <c r="A51" s="37" t="s">
+      <c r="A51" s="33" t="s">
         <v>330</v>
       </c>
-      <c r="B51" s="38" t="s">
+      <c r="B51" s="34" t="s">
         <v>348</v>
       </c>
-      <c r="C51" s="34" t="s">
+      <c r="C51" s="39" t="s">
         <v>359</v>
       </c>
       <c r="D51" s="24" t="s">
@@ -3675,26 +3732,26 @@
       </c>
     </row>
     <row r="52" spans="1:4" ht="28.8">
-      <c r="A52" s="37"/>
-      <c r="B52" s="39"/>
-      <c r="C52" s="35"/>
+      <c r="A52" s="33"/>
+      <c r="B52" s="35"/>
+      <c r="C52" s="40"/>
       <c r="D52" s="24" t="s">
         <v>361</v>
       </c>
     </row>
     <row r="53" spans="1:4" ht="43.2">
-      <c r="A53" s="37"/>
-      <c r="B53" s="40"/>
-      <c r="C53" s="36"/>
+      <c r="A53" s="33"/>
+      <c r="B53" s="36"/>
+      <c r="C53" s="41"/>
       <c r="D53" s="24" t="s">
         <v>362</v>
       </c>
     </row>
     <row r="54" spans="1:4" ht="28.8" customHeight="1">
-      <c r="A54" s="37" t="s">
+      <c r="A54" s="33" t="s">
         <v>331</v>
       </c>
-      <c r="B54" s="38" t="s">
+      <c r="B54" s="34" t="s">
         <v>374</v>
       </c>
       <c r="C54" s="26" t="s">
@@ -3705,8 +3762,8 @@
       </c>
     </row>
     <row r="55" spans="1:4" ht="28.8">
-      <c r="A55" s="37"/>
-      <c r="B55" s="39"/>
+      <c r="A55" s="33"/>
+      <c r="B55" s="35"/>
       <c r="C55" s="26" t="s">
         <v>378</v>
       </c>
@@ -3715,8 +3772,8 @@
       </c>
     </row>
     <row r="56" spans="1:4" ht="28.8">
-      <c r="A56" s="37"/>
-      <c r="B56" s="40"/>
+      <c r="A56" s="33"/>
+      <c r="B56" s="36"/>
       <c r="C56" s="26" t="s">
         <v>377</v>
       </c>
@@ -3725,10 +3782,10 @@
       </c>
     </row>
     <row r="57" spans="1:4" ht="43.2">
-      <c r="A57" s="37" t="s">
+      <c r="A57" s="33" t="s">
         <v>332</v>
       </c>
-      <c r="B57" s="38" t="s">
+      <c r="B57" s="34" t="s">
         <v>373</v>
       </c>
       <c r="C57" s="24" t="s">
@@ -3739,8 +3796,8 @@
       </c>
     </row>
     <row r="58" spans="1:4" ht="28.8">
-      <c r="A58" s="37"/>
-      <c r="B58" s="39"/>
+      <c r="A58" s="33"/>
+      <c r="B58" s="35"/>
       <c r="C58" s="26" t="s">
         <v>382</v>
       </c>
@@ -3749,8 +3806,8 @@
       </c>
     </row>
     <row r="59" spans="1:4" ht="43.2">
-      <c r="A59" s="37"/>
-      <c r="B59" s="40"/>
+      <c r="A59" s="33"/>
+      <c r="B59" s="36"/>
       <c r="C59" s="26" t="s">
         <v>383</v>
       </c>
@@ -3759,46 +3816,27 @@
       </c>
     </row>
     <row r="60" spans="1:4">
-      <c r="A60" s="37" t="s">
+      <c r="A60" s="33" t="s">
         <v>333</v>
       </c>
-      <c r="B60" s="38"/>
+      <c r="B60" s="34"/>
       <c r="C60" s="26"/>
       <c r="D60" s="26"/>
     </row>
     <row r="61" spans="1:4">
-      <c r="A61" s="37"/>
-      <c r="B61" s="39"/>
+      <c r="A61" s="33"/>
+      <c r="B61" s="35"/>
       <c r="C61" s="26"/>
       <c r="D61" s="26"/>
     </row>
     <row r="62" spans="1:4">
-      <c r="A62" s="37"/>
-      <c r="B62" s="40"/>
+      <c r="A62" s="33"/>
+      <c r="B62" s="36"/>
       <c r="C62" s="26"/>
       <c r="D62" s="26"/>
     </row>
   </sheetData>
   <mergeCells count="35">
-    <mergeCell ref="A36:A38"/>
-    <mergeCell ref="B36:B38"/>
-    <mergeCell ref="A60:A62"/>
-    <mergeCell ref="B45:B47"/>
-    <mergeCell ref="B48:B50"/>
-    <mergeCell ref="B51:B53"/>
-    <mergeCell ref="B54:B56"/>
-    <mergeCell ref="B57:B59"/>
-    <mergeCell ref="B60:B62"/>
-    <mergeCell ref="A45:A47"/>
-    <mergeCell ref="A48:A50"/>
-    <mergeCell ref="A51:A53"/>
-    <mergeCell ref="A54:A56"/>
-    <mergeCell ref="A57:A59"/>
-    <mergeCell ref="B15:B17"/>
-    <mergeCell ref="A15:A17"/>
-    <mergeCell ref="B18:B20"/>
-    <mergeCell ref="A18:A20"/>
-    <mergeCell ref="A21:A23"/>
     <mergeCell ref="C46:C47"/>
     <mergeCell ref="C49:C50"/>
     <mergeCell ref="C51:C53"/>
@@ -3815,6 +3853,25 @@
     <mergeCell ref="B30:B32"/>
     <mergeCell ref="A33:A35"/>
     <mergeCell ref="B33:B35"/>
+    <mergeCell ref="B15:B17"/>
+    <mergeCell ref="A15:A17"/>
+    <mergeCell ref="B18:B20"/>
+    <mergeCell ref="A18:A20"/>
+    <mergeCell ref="A21:A23"/>
+    <mergeCell ref="A36:A38"/>
+    <mergeCell ref="B36:B38"/>
+    <mergeCell ref="A60:A62"/>
+    <mergeCell ref="B45:B47"/>
+    <mergeCell ref="B48:B50"/>
+    <mergeCell ref="B51:B53"/>
+    <mergeCell ref="B54:B56"/>
+    <mergeCell ref="B57:B59"/>
+    <mergeCell ref="B60:B62"/>
+    <mergeCell ref="A45:A47"/>
+    <mergeCell ref="A48:A50"/>
+    <mergeCell ref="A51:A53"/>
+    <mergeCell ref="A54:A56"/>
+    <mergeCell ref="A57:A59"/>
   </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3893,10 +3950,10 @@
       </c>
     </row>
     <row r="5" spans="1:4" ht="28.8" hidden="1">
-      <c r="A5" s="37" t="s">
+      <c r="A5" s="33" t="s">
         <v>47</v>
       </c>
-      <c r="B5" s="38" t="s">
+      <c r="B5" s="34" t="s">
         <v>252</v>
       </c>
       <c r="C5" s="24" t="s">
@@ -3907,8 +3964,8 @@
       </c>
     </row>
     <row r="6" spans="1:4" ht="28.8" hidden="1">
-      <c r="A6" s="37"/>
-      <c r="B6" s="39"/>
+      <c r="A6" s="33"/>
+      <c r="B6" s="35"/>
       <c r="C6" s="24" t="s">
         <v>254</v>
       </c>
@@ -3917,8 +3974,8 @@
       </c>
     </row>
     <row r="7" spans="1:4" ht="43.2" hidden="1">
-      <c r="A7" s="37"/>
-      <c r="B7" s="40"/>
+      <c r="A7" s="33"/>
+      <c r="B7" s="36"/>
       <c r="C7" s="24" t="s">
         <v>255</v>
       </c>
@@ -3927,10 +3984,10 @@
       </c>
     </row>
     <row r="8" spans="1:4" ht="28.8" customHeight="1">
-      <c r="A8" s="37" t="s">
+      <c r="A8" s="33" t="s">
         <v>334</v>
       </c>
-      <c r="B8" s="38" t="s">
+      <c r="B8" s="34" t="s">
         <v>299</v>
       </c>
       <c r="C8" s="24" t="s">
@@ -3941,8 +3998,8 @@
       </c>
     </row>
     <row r="9" spans="1:4" ht="28.8">
-      <c r="A9" s="37"/>
-      <c r="B9" s="39"/>
+      <c r="A9" s="33"/>
+      <c r="B9" s="35"/>
       <c r="C9" s="24" t="s">
         <v>301</v>
       </c>
@@ -3951,8 +4008,8 @@
       </c>
     </row>
     <row r="10" spans="1:4" ht="28.8">
-      <c r="A10" s="37"/>
-      <c r="B10" s="40"/>
+      <c r="A10" s="33"/>
+      <c r="B10" s="36"/>
       <c r="C10" s="24" t="s">
         <v>302</v>
       </c>
@@ -3961,10 +4018,10 @@
       </c>
     </row>
     <row r="11" spans="1:4" ht="14.4" customHeight="1">
-      <c r="A11" s="37" t="s">
+      <c r="A11" s="33" t="s">
         <v>335</v>
       </c>
-      <c r="B11" s="38" t="s">
+      <c r="B11" s="34" t="s">
         <v>306</v>
       </c>
       <c r="C11" s="24" t="s">
@@ -3975,8 +4032,8 @@
       </c>
     </row>
     <row r="12" spans="1:4" ht="37.200000000000003" customHeight="1">
-      <c r="A12" s="37"/>
-      <c r="B12" s="39"/>
+      <c r="A12" s="33"/>
+      <c r="B12" s="35"/>
       <c r="C12" s="24" t="s">
         <v>308</v>
       </c>
@@ -3985,8 +4042,8 @@
       </c>
     </row>
     <row r="13" spans="1:4" ht="26.4" customHeight="1">
-      <c r="A13" s="37"/>
-      <c r="B13" s="40"/>
+      <c r="A13" s="33"/>
+      <c r="B13" s="36"/>
       <c r="C13" s="24" t="s">
         <v>309</v>
       </c>
@@ -3995,10 +4052,10 @@
       </c>
     </row>
     <row r="14" spans="1:4" ht="43.2">
-      <c r="A14" s="37" t="s">
+      <c r="A14" s="33" t="s">
         <v>342</v>
       </c>
-      <c r="B14" s="38" t="s">
+      <c r="B14" s="34" t="s">
         <v>347</v>
       </c>
       <c r="C14" s="24" t="s">
@@ -4009,8 +4066,8 @@
       </c>
     </row>
     <row r="15" spans="1:4" ht="43.2">
-      <c r="A15" s="37"/>
-      <c r="B15" s="39"/>
+      <c r="A15" s="33"/>
+      <c r="B15" s="35"/>
       <c r="C15" s="24" t="s">
         <v>365</v>
       </c>
@@ -4019,8 +4076,8 @@
       </c>
     </row>
     <row r="16" spans="1:4" ht="43.2">
-      <c r="A16" s="37"/>
-      <c r="B16" s="40"/>
+      <c r="A16" s="33"/>
+      <c r="B16" s="36"/>
       <c r="C16" s="24" t="s">
         <v>367</v>
       </c>
@@ -4029,10 +4086,10 @@
       </c>
     </row>
     <row r="17" spans="1:4" ht="57.6">
-      <c r="A17" s="37" t="s">
+      <c r="A17" s="33" t="s">
         <v>375</v>
       </c>
-      <c r="B17" s="38" t="s">
+      <c r="B17" s="34" t="s">
         <v>388</v>
       </c>
       <c r="C17" s="24" t="s">
@@ -4043,8 +4100,8 @@
       </c>
     </row>
     <row r="18" spans="1:4" ht="72">
-      <c r="A18" s="37"/>
-      <c r="B18" s="39"/>
+      <c r="A18" s="33"/>
+      <c r="B18" s="35"/>
       <c r="C18" s="24" t="s">
         <v>390</v>
       </c>
@@ -4053,8 +4110,8 @@
       </c>
     </row>
     <row r="19" spans="1:4" ht="31.2" customHeight="1">
-      <c r="A19" s="37"/>
-      <c r="B19" s="40"/>
+      <c r="A19" s="33"/>
+      <c r="B19" s="36"/>
       <c r="C19" s="24" t="s">
         <v>391</v>
       </c>
@@ -4063,39 +4120,39 @@
       </c>
     </row>
     <row r="20" spans="1:4">
-      <c r="A20" s="37" t="s">
+      <c r="A20" s="33" t="s">
         <v>387</v>
       </c>
-      <c r="B20" s="38"/>
+      <c r="B20" s="34"/>
       <c r="C20" s="24"/>
       <c r="D20" s="24"/>
     </row>
     <row r="21" spans="1:4">
-      <c r="A21" s="37"/>
-      <c r="B21" s="39"/>
+      <c r="A21" s="33"/>
+      <c r="B21" s="35"/>
       <c r="C21" s="24"/>
       <c r="D21" s="24"/>
     </row>
     <row r="22" spans="1:4">
-      <c r="A22" s="37"/>
-      <c r="B22" s="40"/>
+      <c r="A22" s="33"/>
+      <c r="B22" s="36"/>
       <c r="C22" s="24"/>
       <c r="D22" s="24"/>
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A17:A19"/>
+    <mergeCell ref="B17:B19"/>
+    <mergeCell ref="A20:A22"/>
+    <mergeCell ref="B20:B22"/>
+    <mergeCell ref="A14:A16"/>
+    <mergeCell ref="B14:B16"/>
     <mergeCell ref="A11:A13"/>
     <mergeCell ref="B11:B13"/>
     <mergeCell ref="A5:A7"/>
     <mergeCell ref="B5:B7"/>
     <mergeCell ref="A8:A10"/>
     <mergeCell ref="B8:B10"/>
-    <mergeCell ref="A17:A19"/>
-    <mergeCell ref="B17:B19"/>
-    <mergeCell ref="A20:A22"/>
-    <mergeCell ref="B20:B22"/>
-    <mergeCell ref="A14:A16"/>
-    <mergeCell ref="B14:B16"/>
   </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>